<commit_message>
Cambios en la vista
</commit_message>
<xml_diff>
--- a/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
+++ b/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\PROYECTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1234\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919AAABB-E5C9-4E23-8F90-20831E169821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B87A376-54E1-4417-8E84-60D1F7F75693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diseño" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AS$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Diseño!$A$1:$AS$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1780,24 +1780,435 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1871,417 +2282,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2633,27 +2633,27 @@
   <dimension ref="A1:AS101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G84" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="31" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1"/>
+    <col min="7" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="31" width="11.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2757,17 +2757,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="326" t="s">
+    <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="188">
+      <c r="B2" s="326">
         <v>228183</v>
       </c>
-      <c r="C2" s="190">
+      <c r="C2" s="328">
         <v>2</v>
       </c>
-      <c r="D2" s="329" t="s">
+      <c r="D2" s="203" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
@@ -2776,7 +2776,7 @@
       <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="332">
+      <c r="G2" s="206">
         <v>528</v>
       </c>
       <c r="H2" s="12"/>
@@ -2788,7 +2788,7 @@
       <c r="N2" s="12">
         <v>72</v>
       </c>
-      <c r="O2" s="276">
+      <c r="O2" s="273">
         <f>SUM(P2:P5)</f>
         <v>528</v>
       </c>
@@ -2868,18 +2868,18 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="327"/>
-      <c r="B3" s="189"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="330"/>
+    <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="201"/>
+      <c r="B3" s="327"/>
+      <c r="C3" s="329"/>
+      <c r="D3" s="204"/>
       <c r="E3" s="13">
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="333"/>
+      <c r="G3" s="207"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -2889,7 +2889,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="277"/>
+      <c r="O3" s="274"/>
       <c r="P3" s="9">
         <f>SUM(H3:N3)</f>
         <v>64</v>
@@ -2924,18 +2924,18 @@
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="327"/>
-      <c r="B4" s="189"/>
-      <c r="C4" s="191"/>
-      <c r="D4" s="330"/>
+    <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="201"/>
+      <c r="B4" s="327"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="204"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="333"/>
+      <c r="G4" s="207"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2945,7 +2945,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="277"/>
+      <c r="O4" s="274"/>
       <c r="P4" s="9">
         <f>SUM(H4:N4)</f>
         <v>80</v>
@@ -2980,18 +2980,18 @@
       <c r="AR4" s="2"/>
       <c r="AS4" s="2"/>
     </row>
-    <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="327"/>
-      <c r="B5" s="189"/>
-      <c r="C5" s="191"/>
-      <c r="D5" s="331"/>
+    <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="201"/>
+      <c r="B5" s="327"/>
+      <c r="C5" s="329"/>
+      <c r="D5" s="205"/>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="334"/>
+      <c r="G5" s="208"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -3005,7 +3005,7 @@
       <c r="N5" s="18">
         <v>168</v>
       </c>
-      <c r="O5" s="278"/>
+      <c r="O5" s="275"/>
       <c r="P5" s="9">
         <f>SUM(H5:N5)</f>
         <v>312</v>
@@ -3040,14 +3040,14 @@
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
     </row>
-    <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="327"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="196"/>
+    <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="201"/>
+      <c r="B6" s="327"/>
+      <c r="C6" s="329"/>
+      <c r="D6" s="331"/>
+      <c r="E6" s="332"/>
+      <c r="F6" s="332"/>
+      <c r="G6" s="333"/>
       <c r="H6" s="56">
         <f>SUM(H2:H5)</f>
         <v>0</v>
@@ -3108,11 +3108,11 @@
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
     </row>
-    <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="327"/>
-      <c r="B7" s="189"/>
-      <c r="C7" s="191"/>
-      <c r="D7" s="335" t="s">
+    <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="201"/>
+      <c r="B7" s="327"/>
+      <c r="C7" s="329"/>
+      <c r="D7" s="215" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="19">
@@ -3121,7 +3121,7 @@
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="338">
+      <c r="G7" s="218">
         <v>384</v>
       </c>
       <c r="H7" s="25"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="279">
+      <c r="O7" s="276">
         <f>SUM(P7:P10)</f>
         <v>384</v>
       </c>
@@ -3213,18 +3213,18 @@
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
     </row>
-    <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="327"/>
-      <c r="B8" s="189"/>
-      <c r="C8" s="191"/>
-      <c r="D8" s="336"/>
+    <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="201"/>
+      <c r="B8" s="327"/>
+      <c r="C8" s="329"/>
+      <c r="D8" s="216"/>
       <c r="E8" s="21">
         <v>3</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="339"/>
+      <c r="G8" s="219"/>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
@@ -3234,7 +3234,7 @@
         <v>144</v>
       </c>
       <c r="N8" s="26"/>
-      <c r="O8" s="280"/>
+      <c r="O8" s="277"/>
       <c r="P8" s="9">
         <f t="shared" ref="P8:P10" si="1">SUM(H8:N8)</f>
         <v>144</v>
@@ -3269,18 +3269,18 @@
       <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
     </row>
-    <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="327"/>
-      <c r="B9" s="189"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="336"/>
+    <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="201"/>
+      <c r="B9" s="327"/>
+      <c r="C9" s="329"/>
+      <c r="D9" s="216"/>
       <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="339"/>
+      <c r="G9" s="219"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="280"/>
+      <c r="O9" s="277"/>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3325,18 +3325,18 @@
       <c r="AR9" s="3"/>
       <c r="AS9" s="3"/>
     </row>
-    <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="327"/>
-      <c r="B10" s="189"/>
-      <c r="C10" s="191"/>
-      <c r="D10" s="337"/>
+    <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="201"/>
+      <c r="B10" s="327"/>
+      <c r="C10" s="329"/>
+      <c r="D10" s="217"/>
       <c r="E10" s="23">
         <v>4</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="340"/>
+      <c r="G10" s="220"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -3346,7 +3346,7 @@
       <c r="N10" s="27">
         <v>96</v>
       </c>
-      <c r="O10" s="281"/>
+      <c r="O10" s="278"/>
       <c r="P10" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3381,14 +3381,14 @@
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
     </row>
-    <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="327"/>
-      <c r="B11" s="189"/>
-      <c r="C11" s="191"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="198"/>
-      <c r="F11" s="198"/>
-      <c r="G11" s="199"/>
+    <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="201"/>
+      <c r="B11" s="327"/>
+      <c r="C11" s="329"/>
+      <c r="D11" s="334"/>
+      <c r="E11" s="335"/>
+      <c r="F11" s="335"/>
+      <c r="G11" s="336"/>
       <c r="H11" s="61">
         <f>SUM(H7:H10)</f>
         <v>0</v>
@@ -3449,18 +3449,18 @@
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
     </row>
-    <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="327"/>
-      <c r="B12" s="189"/>
-      <c r="C12" s="191"/>
-      <c r="D12" s="259" t="s">
+    <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="201"/>
+      <c r="B12" s="327"/>
+      <c r="C12" s="329"/>
+      <c r="D12" s="188" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="262">
+      <c r="G12" s="191">
         <v>48</v>
       </c>
       <c r="H12" s="34">
@@ -3472,7 +3472,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="256">
+      <c r="O12" s="279">
         <f t="shared" ref="O12" si="3">SUM(P12:P15)</f>
         <v>48</v>
       </c>
@@ -3537,16 +3537,16 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="327"/>
-      <c r="B13" s="189"/>
-      <c r="C13" s="191"/>
-      <c r="D13" s="260"/>
+    <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="201"/>
+      <c r="B13" s="327"/>
+      <c r="C13" s="329"/>
+      <c r="D13" s="189"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="263"/>
+      <c r="G13" s="192"/>
       <c r="H13" s="35">
         <v>12</v>
       </c>
@@ -3556,7 +3556,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="257"/>
+      <c r="O13" s="280"/>
       <c r="P13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3578,16 +3578,16 @@
       <c r="AE13" s="179"/>
       <c r="AI13" s="179"/>
     </row>
-    <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="327"/>
-      <c r="B14" s="189"/>
-      <c r="C14" s="191"/>
-      <c r="D14" s="260"/>
+    <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="201"/>
+      <c r="B14" s="327"/>
+      <c r="C14" s="329"/>
+      <c r="D14" s="189"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="263"/>
+      <c r="G14" s="192"/>
       <c r="H14" s="35">
         <v>12</v>
       </c>
@@ -3597,7 +3597,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="257"/>
+      <c r="O14" s="280"/>
       <c r="P14" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3619,16 +3619,16 @@
       <c r="AE14" s="179"/>
       <c r="AI14" s="179"/>
     </row>
-    <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="327"/>
-      <c r="B15" s="189"/>
-      <c r="C15" s="191"/>
-      <c r="D15" s="261"/>
+    <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="201"/>
+      <c r="B15" s="327"/>
+      <c r="C15" s="329"/>
+      <c r="D15" s="190"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="264"/>
+      <c r="G15" s="193"/>
       <c r="H15" s="36">
         <v>12</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="258"/>
+      <c r="O15" s="281"/>
       <c r="P15" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3660,14 +3660,14 @@
       <c r="AE15" s="179"/>
       <c r="AI15" s="179"/>
     </row>
-    <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="327"/>
-      <c r="B16" s="189"/>
-      <c r="C16" s="191"/>
-      <c r="D16" s="194"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="196"/>
+    <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="201"/>
+      <c r="B16" s="327"/>
+      <c r="C16" s="329"/>
+      <c r="D16" s="331"/>
+      <c r="E16" s="332"/>
+      <c r="F16" s="332"/>
+      <c r="G16" s="333"/>
       <c r="H16" s="56">
         <f>SUM(H12:H15)</f>
         <v>48</v>
@@ -3728,18 +3728,18 @@
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
     </row>
-    <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="327"/>
-      <c r="B17" s="189"/>
-      <c r="C17" s="191"/>
-      <c r="D17" s="321" t="s">
+    <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="201"/>
+      <c r="B17" s="327"/>
+      <c r="C17" s="329"/>
+      <c r="D17" s="194" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="323">
+      <c r="G17" s="197">
         <v>48</v>
       </c>
       <c r="H17" s="44"/>
@@ -3827,16 +3827,16 @@
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
     </row>
-    <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="327"/>
-      <c r="B18" s="189"/>
-      <c r="C18" s="191"/>
-      <c r="D18" s="322"/>
+    <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="201"/>
+      <c r="B18" s="327"/>
+      <c r="C18" s="329"/>
+      <c r="D18" s="195"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="324"/>
+      <c r="G18" s="198"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45">
         <v>12</v>
@@ -3881,16 +3881,16 @@
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
     </row>
-    <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="327"/>
-      <c r="B19" s="189"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="322"/>
+    <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="201"/>
+      <c r="B19" s="327"/>
+      <c r="C19" s="329"/>
+      <c r="D19" s="195"/>
       <c r="E19" s="39"/>
       <c r="F19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="324"/>
+      <c r="G19" s="198"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45">
         <v>12</v>
@@ -3935,16 +3935,16 @@
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
     </row>
-    <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="327"/>
-      <c r="B20" s="189"/>
-      <c r="C20" s="191"/>
-      <c r="D20" s="219"/>
+    <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="201"/>
+      <c r="B20" s="327"/>
+      <c r="C20" s="329"/>
+      <c r="D20" s="196"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="325"/>
+      <c r="G20" s="199"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46">
         <v>12</v>
@@ -3989,14 +3989,14 @@
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
     </row>
-    <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="327"/>
-      <c r="B21" s="189"/>
-      <c r="C21" s="191"/>
-      <c r="D21" s="200"/>
-      <c r="E21" s="201"/>
-      <c r="F21" s="201"/>
-      <c r="G21" s="202"/>
+    <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="201"/>
+      <c r="B21" s="327"/>
+      <c r="C21" s="329"/>
+      <c r="D21" s="337"/>
+      <c r="E21" s="338"/>
+      <c r="F21" s="338"/>
+      <c r="G21" s="339"/>
       <c r="H21" s="62">
         <f>SUM(H17:H20)</f>
         <v>0</v>
@@ -4057,11 +4057,11 @@
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
     </row>
-    <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="327"/>
-      <c r="B22" s="189"/>
-      <c r="C22" s="191"/>
-      <c r="D22" s="318" t="s">
+    <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="201"/>
+      <c r="B22" s="327"/>
+      <c r="C22" s="329"/>
+      <c r="D22" s="209" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="47">
@@ -4070,7 +4070,7 @@
       <c r="F22" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="306">
+      <c r="G22" s="212">
         <v>336</v>
       </c>
       <c r="H22" s="53"/>
@@ -4080,7 +4080,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="53"/>
       <c r="N22" s="53"/>
-      <c r="O22" s="271">
+      <c r="O22" s="268">
         <f t="shared" ref="O22" si="13">SUM(P22:P25)</f>
         <v>336</v>
       </c>
@@ -4166,18 +4166,18 @@
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
     </row>
-    <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="327"/>
-      <c r="B23" s="189"/>
-      <c r="C23" s="191"/>
-      <c r="D23" s="319"/>
+    <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="201"/>
+      <c r="B23" s="327"/>
+      <c r="C23" s="329"/>
+      <c r="D23" s="210"/>
       <c r="E23" s="49">
         <v>2</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="307"/>
+      <c r="G23" s="213"/>
       <c r="H23" s="54">
         <v>72</v>
       </c>
@@ -4187,7 +4187,7 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="272"/>
+      <c r="O23" s="269"/>
       <c r="P23" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4222,18 +4222,18 @@
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
     </row>
-    <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="327"/>
-      <c r="B24" s="189"/>
-      <c r="C24" s="191"/>
-      <c r="D24" s="319"/>
+    <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="201"/>
+      <c r="B24" s="327"/>
+      <c r="C24" s="329"/>
+      <c r="D24" s="210"/>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="307"/>
+      <c r="G24" s="213"/>
       <c r="H24" s="54">
         <v>72</v>
       </c>
@@ -4243,7 +4243,7 @@
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
-      <c r="O24" s="272"/>
+      <c r="O24" s="269"/>
       <c r="P24" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4278,18 +4278,18 @@
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
     </row>
-    <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="327"/>
-      <c r="B25" s="189"/>
-      <c r="C25" s="191"/>
-      <c r="D25" s="320"/>
+    <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="201"/>
+      <c r="B25" s="327"/>
+      <c r="C25" s="329"/>
+      <c r="D25" s="211"/>
       <c r="E25" s="51">
         <v>3</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="308"/>
+      <c r="G25" s="214"/>
       <c r="H25" s="55"/>
       <c r="I25" s="55">
         <v>72</v>
@@ -4301,7 +4301,7 @@
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
-      <c r="O25" s="273"/>
+      <c r="O25" s="270"/>
       <c r="P25" s="9">
         <f t="shared" si="4"/>
         <v>192</v>
@@ -4336,14 +4336,14 @@
       <c r="AR25" s="3"/>
       <c r="AS25" s="3"/>
     </row>
-    <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="327"/>
-      <c r="B26" s="189"/>
-      <c r="C26" s="191"/>
-      <c r="D26" s="203"/>
-      <c r="E26" s="204"/>
-      <c r="F26" s="204"/>
-      <c r="G26" s="205"/>
+    <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="201"/>
+      <c r="B26" s="327"/>
+      <c r="C26" s="329"/>
+      <c r="D26" s="340"/>
+      <c r="E26" s="341"/>
+      <c r="F26" s="341"/>
+      <c r="G26" s="342"/>
       <c r="H26" s="64">
         <f>SUM(H22:H25)</f>
         <v>144</v>
@@ -4404,11 +4404,11 @@
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
     </row>
-    <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="327"/>
-      <c r="B27" s="189"/>
-      <c r="C27" s="191"/>
-      <c r="D27" s="353" t="s">
+    <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="201"/>
+      <c r="B27" s="327"/>
+      <c r="C27" s="329"/>
+      <c r="D27" s="233" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="65">
@@ -4417,7 +4417,7 @@
       <c r="F27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="341">
+      <c r="G27" s="221">
         <v>576</v>
       </c>
       <c r="H27" s="73"/>
@@ -4515,18 +4515,18 @@
       <c r="AR27" s="3"/>
       <c r="AS27" s="3"/>
     </row>
-    <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="327"/>
-      <c r="B28" s="189"/>
-      <c r="C28" s="191"/>
-      <c r="D28" s="354"/>
+    <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="201"/>
+      <c r="B28" s="327"/>
+      <c r="C28" s="329"/>
+      <c r="D28" s="234"/>
       <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="342"/>
+      <c r="G28" s="222"/>
       <c r="H28" s="74"/>
       <c r="I28" s="74">
         <v>72</v>
@@ -4571,18 +4571,18 @@
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
     </row>
-    <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="327"/>
-      <c r="B29" s="189"/>
-      <c r="C29" s="191"/>
-      <c r="D29" s="354"/>
+    <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="201"/>
+      <c r="B29" s="327"/>
+      <c r="C29" s="329"/>
+      <c r="D29" s="234"/>
       <c r="E29" s="67">
         <v>1</v>
       </c>
       <c r="F29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="342"/>
+      <c r="G29" s="222"/>
       <c r="H29" s="74">
         <v>72</v>
       </c>
@@ -4627,18 +4627,18 @@
       <c r="AR29" s="3"/>
       <c r="AS29" s="3"/>
     </row>
-    <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="327"/>
-      <c r="B30" s="189"/>
-      <c r="C30" s="191"/>
-      <c r="D30" s="355"/>
+    <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="201"/>
+      <c r="B30" s="327"/>
+      <c r="C30" s="329"/>
+      <c r="D30" s="235"/>
       <c r="E30" s="69">
         <v>3</v>
       </c>
       <c r="F30" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="343"/>
+      <c r="G30" s="223"/>
       <c r="H30" s="75"/>
       <c r="I30" s="75">
         <v>72</v>
@@ -4689,14 +4689,14 @@
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
     </row>
-    <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="327"/>
-      <c r="B31" s="189"/>
-      <c r="C31" s="191"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="207"/>
-      <c r="F31" s="207"/>
-      <c r="G31" s="208"/>
+    <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="201"/>
+      <c r="B31" s="327"/>
+      <c r="C31" s="329"/>
+      <c r="D31" s="343"/>
+      <c r="E31" s="344"/>
+      <c r="F31" s="344"/>
+      <c r="G31" s="345"/>
       <c r="H31" s="71">
         <f>SUM(H27:H30)</f>
         <v>72</v>
@@ -4757,18 +4757,18 @@
       <c r="AR31" s="2"/>
       <c r="AS31" s="2"/>
     </row>
-    <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="327"/>
-      <c r="B32" s="189"/>
-      <c r="C32" s="191"/>
-      <c r="D32" s="265" t="s">
+    <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="201"/>
+      <c r="B32" s="327"/>
+      <c r="C32" s="329"/>
+      <c r="D32" s="300" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="344">
+      <c r="G32" s="224">
         <v>48</v>
       </c>
       <c r="H32" s="82"/>
@@ -4780,7 +4780,7 @@
         <v>12</v>
       </c>
       <c r="N32" s="82"/>
-      <c r="O32" s="250">
+      <c r="O32" s="294">
         <f t="shared" ref="O32" si="27">SUM(P32:P35)</f>
         <v>48</v>
       </c>
@@ -4845,16 +4845,16 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="327"/>
-      <c r="B33" s="189"/>
-      <c r="C33" s="191"/>
-      <c r="D33" s="266"/>
+    <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="201"/>
+      <c r="B33" s="327"/>
+      <c r="C33" s="329"/>
+      <c r="D33" s="301"/>
       <c r="E33" s="78"/>
       <c r="F33" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="345"/>
+      <c r="G33" s="225"/>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -4864,7 +4864,7 @@
         <v>12</v>
       </c>
       <c r="N33" s="83"/>
-      <c r="O33" s="251"/>
+      <c r="O33" s="295"/>
       <c r="P33" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4885,16 +4885,16 @@
       <c r="AD33" s="179"/>
       <c r="AE33" s="179"/>
     </row>
-    <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="327"/>
-      <c r="B34" s="189"/>
-      <c r="C34" s="191"/>
-      <c r="D34" s="266"/>
+    <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="201"/>
+      <c r="B34" s="327"/>
+      <c r="C34" s="329"/>
+      <c r="D34" s="301"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="345"/>
+      <c r="G34" s="225"/>
       <c r="H34" s="83"/>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -4904,7 +4904,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="83"/>
-      <c r="O34" s="251"/>
+      <c r="O34" s="295"/>
       <c r="P34" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4925,16 +4925,16 @@
       <c r="AD34" s="179"/>
       <c r="AE34" s="179"/>
     </row>
-    <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="327"/>
-      <c r="B35" s="189"/>
-      <c r="C35" s="191"/>
-      <c r="D35" s="267"/>
+    <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="201"/>
+      <c r="B35" s="327"/>
+      <c r="C35" s="329"/>
+      <c r="D35" s="302"/>
       <c r="E35" s="80"/>
       <c r="F35" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="346"/>
+      <c r="G35" s="226"/>
       <c r="H35" s="84"/>
       <c r="I35" s="84"/>
       <c r="J35" s="84"/>
@@ -4944,7 +4944,7 @@
         <v>12</v>
       </c>
       <c r="N35" s="84"/>
-      <c r="O35" s="252"/>
+      <c r="O35" s="296"/>
       <c r="P35" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4965,14 +4965,14 @@
       <c r="AD35" s="179"/>
       <c r="AE35" s="179"/>
     </row>
-    <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="327"/>
-      <c r="B36" s="189"/>
-      <c r="C36" s="191"/>
-      <c r="D36" s="244"/>
-      <c r="E36" s="245"/>
-      <c r="F36" s="245"/>
-      <c r="G36" s="246"/>
+    <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="201"/>
+      <c r="B36" s="327"/>
+      <c r="C36" s="329"/>
+      <c r="D36" s="288"/>
+      <c r="E36" s="289"/>
+      <c r="F36" s="289"/>
+      <c r="G36" s="290"/>
       <c r="H36" s="86">
         <f>SUM(H32:H35)</f>
         <v>0</v>
@@ -5033,18 +5033,18 @@
       <c r="AR36" s="2"/>
       <c r="AS36" s="2"/>
     </row>
-    <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="327"/>
-      <c r="B37" s="189"/>
-      <c r="C37" s="191"/>
-      <c r="D37" s="347" t="s">
+    <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="201"/>
+      <c r="B37" s="327"/>
+      <c r="C37" s="329"/>
+      <c r="D37" s="227" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="350">
+      <c r="G37" s="230">
         <v>48</v>
       </c>
       <c r="H37" s="95"/>
@@ -5056,7 +5056,7 @@
       <c r="N37" s="95">
         <v>12</v>
       </c>
-      <c r="O37" s="253">
+      <c r="O37" s="297">
         <f t="shared" ref="O37" si="34">SUM(P37:P40)</f>
         <v>48</v>
       </c>
@@ -5108,16 +5108,16 @@
       <c r="AR37" s="3"/>
       <c r="AS37" s="3"/>
     </row>
-    <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="327"/>
-      <c r="B38" s="189"/>
-      <c r="C38" s="191"/>
-      <c r="D38" s="348"/>
+    <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="201"/>
+      <c r="B38" s="327"/>
+      <c r="C38" s="329"/>
+      <c r="D38" s="228"/>
       <c r="E38" s="89"/>
       <c r="F38" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="351"/>
+      <c r="G38" s="231"/>
       <c r="H38" s="96"/>
       <c r="I38" s="96"/>
       <c r="J38" s="96"/>
@@ -5127,7 +5127,7 @@
       <c r="N38" s="96">
         <v>12</v>
       </c>
-      <c r="O38" s="254"/>
+      <c r="O38" s="298"/>
       <c r="P38" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5162,16 +5162,16 @@
       <c r="AR38" s="3"/>
       <c r="AS38" s="3"/>
     </row>
-    <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="327"/>
-      <c r="B39" s="189"/>
-      <c r="C39" s="191"/>
-      <c r="D39" s="348"/>
+    <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="201"/>
+      <c r="B39" s="327"/>
+      <c r="C39" s="329"/>
+      <c r="D39" s="228"/>
       <c r="E39" s="89"/>
       <c r="F39" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="351"/>
+      <c r="G39" s="231"/>
       <c r="H39" s="96"/>
       <c r="I39" s="96"/>
       <c r="J39" s="96"/>
@@ -5181,7 +5181,7 @@
       <c r="N39" s="96">
         <v>12</v>
       </c>
-      <c r="O39" s="254"/>
+      <c r="O39" s="298"/>
       <c r="P39" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5216,16 +5216,16 @@
       <c r="AR39" s="3"/>
       <c r="AS39" s="3"/>
     </row>
-    <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="327"/>
-      <c r="B40" s="189"/>
-      <c r="C40" s="191"/>
-      <c r="D40" s="349"/>
+    <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="201"/>
+      <c r="B40" s="327"/>
+      <c r="C40" s="329"/>
+      <c r="D40" s="229"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="352"/>
+      <c r="G40" s="232"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
       <c r="J40" s="97"/>
@@ -5235,7 +5235,7 @@
       <c r="N40" s="97">
         <v>12</v>
       </c>
-      <c r="O40" s="255"/>
+      <c r="O40" s="299"/>
       <c r="P40" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5270,14 +5270,14 @@
       <c r="AR40" s="3"/>
       <c r="AS40" s="3"/>
     </row>
-    <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="327"/>
-      <c r="B41" s="189"/>
-      <c r="C41" s="191"/>
-      <c r="D41" s="247"/>
-      <c r="E41" s="248"/>
-      <c r="F41" s="248"/>
-      <c r="G41" s="249"/>
+    <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="201"/>
+      <c r="B41" s="327"/>
+      <c r="C41" s="329"/>
+      <c r="D41" s="291"/>
+      <c r="E41" s="292"/>
+      <c r="F41" s="292"/>
+      <c r="G41" s="293"/>
       <c r="H41" s="93">
         <f>SUM(H37:H40)</f>
         <v>0</v>
@@ -5338,18 +5338,18 @@
       <c r="AR41" s="2"/>
       <c r="AS41" s="2"/>
     </row>
-    <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="327"/>
-      <c r="B42" s="189"/>
-      <c r="C42" s="191"/>
-      <c r="D42" s="259" t="s">
+    <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="201"/>
+      <c r="B42" s="327"/>
+      <c r="C42" s="329"/>
+      <c r="D42" s="188" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="262">
+      <c r="G42" s="191">
         <v>48</v>
       </c>
       <c r="H42" s="34">
@@ -5361,7 +5361,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
-      <c r="O42" s="256">
+      <c r="O42" s="279">
         <f t="shared" ref="O42" si="41">SUM(P42:P45)</f>
         <v>48</v>
       </c>
@@ -5413,16 +5413,16 @@
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
     </row>
-    <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="327"/>
-      <c r="B43" s="189"/>
-      <c r="C43" s="191"/>
-      <c r="D43" s="260"/>
+    <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="201"/>
+      <c r="B43" s="327"/>
+      <c r="C43" s="329"/>
+      <c r="D43" s="189"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="263"/>
+      <c r="G43" s="192"/>
       <c r="H43" s="35">
         <v>12</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="L43" s="35"/>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="257"/>
+      <c r="O43" s="280"/>
       <c r="P43" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5467,16 +5467,16 @@
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
     </row>
-    <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="327"/>
-      <c r="B44" s="189"/>
-      <c r="C44" s="191"/>
-      <c r="D44" s="260"/>
+    <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="201"/>
+      <c r="B44" s="327"/>
+      <c r="C44" s="329"/>
+      <c r="D44" s="189"/>
       <c r="E44" s="30"/>
       <c r="F44" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="263"/>
+      <c r="G44" s="192"/>
       <c r="H44" s="35">
         <v>12</v>
       </c>
@@ -5486,7 +5486,7 @@
       <c r="L44" s="35"/>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
-      <c r="O44" s="257"/>
+      <c r="O44" s="280"/>
       <c r="P44" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5521,16 +5521,16 @@
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
     </row>
-    <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="327"/>
-      <c r="B45" s="189"/>
-      <c r="C45" s="191"/>
-      <c r="D45" s="261"/>
+    <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="201"/>
+      <c r="B45" s="327"/>
+      <c r="C45" s="329"/>
+      <c r="D45" s="190"/>
       <c r="E45" s="32"/>
       <c r="F45" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="264"/>
+      <c r="G45" s="193"/>
       <c r="H45" s="36">
         <v>12</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
-      <c r="O45" s="258"/>
+      <c r="O45" s="281"/>
       <c r="P45" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5575,14 +5575,14 @@
       <c r="AR45" s="3"/>
       <c r="AS45" s="3"/>
     </row>
-    <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="327"/>
-      <c r="B46" s="189"/>
-      <c r="C46" s="191"/>
-      <c r="D46" s="309"/>
-      <c r="E46" s="310"/>
-      <c r="F46" s="310"/>
-      <c r="G46" s="311"/>
+    <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="201"/>
+      <c r="B46" s="327"/>
+      <c r="C46" s="329"/>
+      <c r="D46" s="239"/>
+      <c r="E46" s="240"/>
+      <c r="F46" s="240"/>
+      <c r="G46" s="241"/>
       <c r="H46" s="98">
         <f>SUM(H42:H45)</f>
         <v>48</v>
@@ -5643,18 +5643,18 @@
       <c r="AR46" s="2"/>
       <c r="AS46" s="2"/>
     </row>
-    <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="327"/>
-      <c r="B47" s="189"/>
-      <c r="C47" s="191"/>
-      <c r="D47" s="315" t="s">
+    <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="201"/>
+      <c r="B47" s="327"/>
+      <c r="C47" s="329"/>
+      <c r="D47" s="245" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="99"/>
       <c r="F47" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="303">
+      <c r="G47" s="236">
         <v>48</v>
       </c>
       <c r="H47" s="107"/>
@@ -5666,7 +5666,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
-      <c r="O47" s="268">
+      <c r="O47" s="265">
         <f t="shared" ref="O47" si="48">SUM(P47:P50)</f>
         <v>48</v>
       </c>
@@ -5707,16 +5707,16 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="327"/>
-      <c r="B48" s="189"/>
-      <c r="C48" s="191"/>
-      <c r="D48" s="316"/>
+    <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="201"/>
+      <c r="B48" s="327"/>
+      <c r="C48" s="329"/>
+      <c r="D48" s="246"/>
       <c r="E48" s="101"/>
       <c r="F48" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="304"/>
+      <c r="G48" s="237"/>
       <c r="H48" s="108"/>
       <c r="I48" s="108">
         <v>12</v>
@@ -5726,7 +5726,7 @@
       <c r="L48" s="108"/>
       <c r="M48" s="108"/>
       <c r="N48" s="108"/>
-      <c r="O48" s="269"/>
+      <c r="O48" s="266"/>
       <c r="P48" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5747,16 +5747,16 @@
       <c r="AD48" s="179"/>
       <c r="AE48" s="179"/>
     </row>
-    <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="327"/>
-      <c r="B49" s="189"/>
-      <c r="C49" s="191"/>
-      <c r="D49" s="316"/>
+    <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="201"/>
+      <c r="B49" s="327"/>
+      <c r="C49" s="329"/>
+      <c r="D49" s="246"/>
       <c r="E49" s="101"/>
       <c r="F49" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="304"/>
+      <c r="G49" s="237"/>
       <c r="H49" s="108"/>
       <c r="I49" s="108">
         <v>12</v>
@@ -5766,7 +5766,7 @@
       <c r="L49" s="108"/>
       <c r="M49" s="108"/>
       <c r="N49" s="108"/>
-      <c r="O49" s="269"/>
+      <c r="O49" s="266"/>
       <c r="P49" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5787,16 +5787,16 @@
       <c r="AD49" s="179"/>
       <c r="AE49" s="179"/>
     </row>
-    <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="327"/>
-      <c r="B50" s="189"/>
-      <c r="C50" s="191"/>
-      <c r="D50" s="317"/>
+    <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="201"/>
+      <c r="B50" s="327"/>
+      <c r="C50" s="329"/>
+      <c r="D50" s="247"/>
       <c r="E50" s="103"/>
       <c r="F50" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="G50" s="305"/>
+      <c r="G50" s="238"/>
       <c r="H50" s="109"/>
       <c r="I50" s="109">
         <v>12</v>
@@ -5806,7 +5806,7 @@
       <c r="L50" s="109"/>
       <c r="M50" s="109"/>
       <c r="N50" s="109"/>
-      <c r="O50" s="270"/>
+      <c r="O50" s="267"/>
       <c r="P50" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5827,14 +5827,14 @@
       <c r="AD50" s="179"/>
       <c r="AE50" s="179"/>
     </row>
-    <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="327"/>
-      <c r="B51" s="189"/>
-      <c r="C51" s="191"/>
-      <c r="D51" s="312"/>
-      <c r="E51" s="313"/>
-      <c r="F51" s="313"/>
-      <c r="G51" s="314"/>
+    <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="201"/>
+      <c r="B51" s="327"/>
+      <c r="C51" s="329"/>
+      <c r="D51" s="242"/>
+      <c r="E51" s="243"/>
+      <c r="F51" s="243"/>
+      <c r="G51" s="244"/>
       <c r="H51" s="106">
         <f>SUM(H47:H50)</f>
         <v>0</v>
@@ -5895,18 +5895,18 @@
       <c r="AR51" s="2"/>
       <c r="AS51" s="2"/>
     </row>
-    <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="327"/>
-      <c r="B52" s="189"/>
-      <c r="C52" s="191"/>
-      <c r="D52" s="318" t="s">
+    <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="201"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="329"/>
+      <c r="D52" s="209" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="47"/>
       <c r="F52" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G52" s="306">
+      <c r="G52" s="212">
         <v>48</v>
       </c>
       <c r="H52" s="53"/>
@@ -5918,7 +5918,7 @@
       <c r="N52" s="53">
         <v>12</v>
       </c>
-      <c r="O52" s="271">
+      <c r="O52" s="268">
         <f t="shared" ref="O52" si="55">SUM(P52:P55)</f>
         <v>48</v>
       </c>
@@ -5970,16 +5970,16 @@
       <c r="AR52" s="3"/>
       <c r="AS52" s="3"/>
     </row>
-    <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="327"/>
-      <c r="B53" s="189"/>
-      <c r="C53" s="191"/>
-      <c r="D53" s="319"/>
+    <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="201"/>
+      <c r="B53" s="327"/>
+      <c r="C53" s="329"/>
+      <c r="D53" s="210"/>
       <c r="E53" s="49"/>
       <c r="F53" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G53" s="307"/>
+      <c r="G53" s="213"/>
       <c r="H53" s="54"/>
       <c r="I53" s="54"/>
       <c r="J53" s="54"/>
@@ -5989,7 +5989,7 @@
       <c r="N53" s="54">
         <v>12</v>
       </c>
-      <c r="O53" s="272"/>
+      <c r="O53" s="269"/>
       <c r="P53" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6024,16 +6024,16 @@
       <c r="AR53" s="3"/>
       <c r="AS53" s="3"/>
     </row>
-    <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="327"/>
-      <c r="B54" s="189"/>
-      <c r="C54" s="191"/>
-      <c r="D54" s="319"/>
+    <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="201"/>
+      <c r="B54" s="327"/>
+      <c r="C54" s="329"/>
+      <c r="D54" s="210"/>
       <c r="E54" s="49"/>
       <c r="F54" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="307"/>
+      <c r="G54" s="213"/>
       <c r="H54" s="54"/>
       <c r="I54" s="54"/>
       <c r="J54" s="54"/>
@@ -6043,7 +6043,7 @@
       <c r="N54" s="54">
         <v>12</v>
       </c>
-      <c r="O54" s="272"/>
+      <c r="O54" s="269"/>
       <c r="P54" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6078,16 +6078,16 @@
       <c r="AR54" s="3"/>
       <c r="AS54" s="3"/>
     </row>
-    <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="327"/>
-      <c r="B55" s="189"/>
-      <c r="C55" s="191"/>
-      <c r="D55" s="320"/>
+    <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="201"/>
+      <c r="B55" s="327"/>
+      <c r="C55" s="329"/>
+      <c r="D55" s="211"/>
       <c r="E55" s="51"/>
       <c r="F55" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="308"/>
+      <c r="G55" s="214"/>
       <c r="H55" s="55"/>
       <c r="I55" s="55"/>
       <c r="J55" s="55"/>
@@ -6097,7 +6097,7 @@
       <c r="N55" s="55">
         <v>12</v>
       </c>
-      <c r="O55" s="273"/>
+      <c r="O55" s="270"/>
       <c r="P55" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6132,14 +6132,14 @@
       <c r="AR55" s="3"/>
       <c r="AS55" s="3"/>
     </row>
-    <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="327"/>
-      <c r="B56" s="189"/>
-      <c r="C56" s="191"/>
-      <c r="D56" s="288"/>
-      <c r="E56" s="289"/>
-      <c r="F56" s="289"/>
-      <c r="G56" s="290"/>
+    <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="201"/>
+      <c r="B56" s="327"/>
+      <c r="C56" s="329"/>
+      <c r="D56" s="248"/>
+      <c r="E56" s="249"/>
+      <c r="F56" s="249"/>
+      <c r="G56" s="250"/>
       <c r="H56" s="64">
         <f>SUM(H52:H55)</f>
         <v>0</v>
@@ -6200,11 +6200,11 @@
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
     </row>
-    <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="327"/>
-      <c r="B57" s="189"/>
-      <c r="C57" s="191"/>
-      <c r="D57" s="297" t="s">
+    <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="201"/>
+      <c r="B57" s="327"/>
+      <c r="C57" s="329"/>
+      <c r="D57" s="257" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="149">
@@ -6213,7 +6213,7 @@
       <c r="F57" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="298">
+      <c r="G57" s="259">
         <v>96</v>
       </c>
       <c r="H57" s="114"/>
@@ -6225,7 +6225,7 @@
       <c r="L57" s="114"/>
       <c r="M57" s="114"/>
       <c r="N57" s="114"/>
-      <c r="O57" s="274">
+      <c r="O57" s="271">
         <f t="shared" ref="O57" si="62">SUM(P57:P60)</f>
         <v>96</v>
       </c>
@@ -6302,18 +6302,18 @@
       <c r="AR57" s="3"/>
       <c r="AS57" s="3"/>
     </row>
-    <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="327"/>
-      <c r="B58" s="189"/>
-      <c r="C58" s="191"/>
-      <c r="D58" s="242"/>
+    <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="201"/>
+      <c r="B58" s="327"/>
+      <c r="C58" s="329"/>
+      <c r="D58" s="258"/>
       <c r="E58" s="145">
         <v>2</v>
       </c>
       <c r="F58" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="G58" s="299"/>
+      <c r="G58" s="260"/>
       <c r="H58" s="115"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115">
@@ -6323,7 +6323,7 @@
       <c r="L58" s="115"/>
       <c r="M58" s="115"/>
       <c r="N58" s="115"/>
-      <c r="O58" s="275"/>
+      <c r="O58" s="272"/>
       <c r="P58" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6358,18 +6358,18 @@
       <c r="AR58" s="7"/>
       <c r="AS58" s="7"/>
     </row>
-    <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="327"/>
-      <c r="B59" s="189"/>
-      <c r="C59" s="191"/>
-      <c r="D59" s="242"/>
+    <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="201"/>
+      <c r="B59" s="327"/>
+      <c r="C59" s="329"/>
+      <c r="D59" s="258"/>
       <c r="E59" s="145">
         <v>4</v>
       </c>
       <c r="F59" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="299"/>
+      <c r="G59" s="260"/>
       <c r="H59" s="115"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115">
@@ -6379,7 +6379,7 @@
       <c r="L59" s="115"/>
       <c r="M59" s="115"/>
       <c r="N59" s="115"/>
-      <c r="O59" s="275"/>
+      <c r="O59" s="272"/>
       <c r="P59" s="9">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -6414,18 +6414,18 @@
       <c r="AR59" s="7"/>
       <c r="AS59" s="7"/>
     </row>
-    <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="327"/>
-      <c r="B60" s="189"/>
-      <c r="C60" s="191"/>
-      <c r="D60" s="242"/>
+    <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="201"/>
+      <c r="B60" s="327"/>
+      <c r="C60" s="329"/>
+      <c r="D60" s="258"/>
       <c r="E60" s="145">
         <v>1</v>
       </c>
       <c r="F60" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="299"/>
+      <c r="G60" s="260"/>
       <c r="H60" s="115"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115">
@@ -6435,7 +6435,7 @@
       <c r="L60" s="115"/>
       <c r="M60" s="115"/>
       <c r="N60" s="115"/>
-      <c r="O60" s="275"/>
+      <c r="O60" s="272"/>
       <c r="P60" s="9">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -6470,14 +6470,14 @@
       <c r="AR60" s="7"/>
       <c r="AS60" s="7"/>
     </row>
-    <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="327"/>
-      <c r="B61" s="189"/>
-      <c r="C61" s="191"/>
-      <c r="D61" s="243"/>
-      <c r="E61" s="300"/>
-      <c r="F61" s="300"/>
-      <c r="G61" s="300"/>
+    <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="201"/>
+      <c r="B61" s="327"/>
+      <c r="C61" s="329"/>
+      <c r="D61" s="261"/>
+      <c r="E61" s="262"/>
+      <c r="F61" s="262"/>
+      <c r="G61" s="262"/>
       <c r="H61" s="150">
         <f>SUM(H57:H60)</f>
         <v>0</v>
@@ -6538,11 +6538,11 @@
       <c r="AR61" s="2"/>
       <c r="AS61" s="2"/>
     </row>
-    <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="327"/>
-      <c r="B62" s="189"/>
-      <c r="C62" s="191"/>
-      <c r="D62" s="293" t="s">
+    <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="201"/>
+      <c r="B62" s="327"/>
+      <c r="C62" s="329"/>
+      <c r="D62" s="253" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="142">
@@ -6551,7 +6551,7 @@
       <c r="F62" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="G62" s="294">
+      <c r="G62" s="254">
         <v>288</v>
       </c>
       <c r="H62" s="132"/>
@@ -6563,7 +6563,7 @@
         <v>72</v>
       </c>
       <c r="N62" s="132"/>
-      <c r="O62" s="215">
+      <c r="O62" s="352">
         <f t="shared" ref="O62" si="69">SUM(P62:P65)</f>
         <v>288</v>
       </c>
@@ -6638,18 +6638,18 @@
       <c r="AR62" s="3"/>
       <c r="AS62" s="3"/>
     </row>
-    <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="327"/>
-      <c r="B63" s="189"/>
-      <c r="C63" s="191"/>
-      <c r="D63" s="260"/>
+    <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="201"/>
+      <c r="B63" s="327"/>
+      <c r="C63" s="329"/>
+      <c r="D63" s="189"/>
       <c r="E63" s="116">
         <v>1</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="263"/>
+      <c r="G63" s="192"/>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
@@ -6659,7 +6659,7 @@
       <c r="L63" s="35"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
-      <c r="O63" s="216"/>
+      <c r="O63" s="353"/>
       <c r="P63" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6694,18 +6694,18 @@
       <c r="AR63" s="3"/>
       <c r="AS63" s="3"/>
     </row>
-    <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="327"/>
-      <c r="B64" s="189"/>
-      <c r="C64" s="191"/>
-      <c r="D64" s="260"/>
+    <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="201"/>
+      <c r="B64" s="327"/>
+      <c r="C64" s="329"/>
+      <c r="D64" s="189"/>
       <c r="E64" s="116">
         <v>2</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="263"/>
+      <c r="G64" s="192"/>
       <c r="H64" s="35"/>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
@@ -6715,7 +6715,7 @@
       <c r="L64" s="35"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
-      <c r="O64" s="216"/>
+      <c r="O64" s="353"/>
       <c r="P64" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6750,18 +6750,18 @@
       <c r="AR64" s="3"/>
       <c r="AS64" s="3"/>
     </row>
-    <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="327"/>
-      <c r="B65" s="189"/>
-      <c r="C65" s="191"/>
-      <c r="D65" s="260"/>
+    <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="201"/>
+      <c r="B65" s="327"/>
+      <c r="C65" s="329"/>
+      <c r="D65" s="189"/>
       <c r="E65" s="116">
         <v>3</v>
       </c>
       <c r="F65" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G65" s="263"/>
+      <c r="G65" s="192"/>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
       <c r="J65" s="35"/>
@@ -6773,7 +6773,7 @@
       </c>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
-      <c r="O65" s="216"/>
+      <c r="O65" s="353"/>
       <c r="P65" s="9">
         <f t="shared" si="4"/>
         <v>168</v>
@@ -6808,14 +6808,14 @@
       <c r="AR65" s="3"/>
       <c r="AS65" s="3"/>
     </row>
-    <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="327"/>
-      <c r="B66" s="189"/>
-      <c r="C66" s="191"/>
-      <c r="D66" s="301"/>
-      <c r="E66" s="302"/>
-      <c r="F66" s="302"/>
-      <c r="G66" s="302"/>
+    <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="201"/>
+      <c r="B66" s="327"/>
+      <c r="C66" s="329"/>
+      <c r="D66" s="263"/>
+      <c r="E66" s="264"/>
+      <c r="F66" s="264"/>
+      <c r="G66" s="264"/>
       <c r="H66" s="152">
         <f>SUM(H62:H65)</f>
         <v>0</v>
@@ -6876,18 +6876,18 @@
       <c r="AR66" s="2"/>
       <c r="AS66" s="2"/>
     </row>
-    <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="327"/>
-      <c r="B67" s="189"/>
-      <c r="C67" s="191"/>
-      <c r="D67" s="291" t="s">
+    <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="201"/>
+      <c r="B67" s="327"/>
+      <c r="C67" s="329"/>
+      <c r="D67" s="251" t="s">
         <v>49</v>
       </c>
       <c r="E67" s="134"/>
       <c r="F67" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="295">
+      <c r="G67" s="255">
         <v>384</v>
       </c>
       <c r="H67" s="128">
@@ -6899,7 +6899,7 @@
       <c r="L67" s="128"/>
       <c r="M67" s="128"/>
       <c r="N67" s="128"/>
-      <c r="O67" s="217">
+      <c r="O67" s="354">
         <f>SUM(P67:P72)</f>
         <v>384</v>
       </c>
@@ -6951,16 +6951,16 @@
       <c r="AR67" s="3"/>
       <c r="AS67" s="3"/>
     </row>
-    <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="327"/>
-      <c r="B68" s="189"/>
-      <c r="C68" s="191"/>
-      <c r="D68" s="292"/>
+    <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="201"/>
+      <c r="B68" s="327"/>
+      <c r="C68" s="329"/>
+      <c r="D68" s="252"/>
       <c r="E68" s="133"/>
       <c r="F68" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="296"/>
+      <c r="G68" s="256"/>
       <c r="H68" s="130"/>
       <c r="I68" s="130">
         <v>72</v>
@@ -6970,7 +6970,7 @@
       <c r="L68" s="130"/>
       <c r="M68" s="130"/>
       <c r="N68" s="130"/>
-      <c r="O68" s="218"/>
+      <c r="O68" s="355"/>
       <c r="P68" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7005,16 +7005,16 @@
       <c r="AR68" s="3"/>
       <c r="AS68" s="3"/>
     </row>
-    <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="327"/>
-      <c r="B69" s="189"/>
-      <c r="C69" s="191"/>
-      <c r="D69" s="292"/>
+    <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="201"/>
+      <c r="B69" s="327"/>
+      <c r="C69" s="329"/>
+      <c r="D69" s="252"/>
       <c r="E69" s="133"/>
       <c r="F69" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="296"/>
+      <c r="G69" s="256"/>
       <c r="H69" s="130"/>
       <c r="I69" s="130"/>
       <c r="J69" s="130">
@@ -7024,7 +7024,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="130"/>
       <c r="N69" s="130"/>
-      <c r="O69" s="218"/>
+      <c r="O69" s="355"/>
       <c r="P69" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7059,16 +7059,16 @@
       <c r="AR69" s="3"/>
       <c r="AS69" s="3"/>
     </row>
-    <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="327"/>
-      <c r="B70" s="189"/>
-      <c r="C70" s="191"/>
-      <c r="D70" s="292"/>
+    <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="201"/>
+      <c r="B70" s="327"/>
+      <c r="C70" s="329"/>
+      <c r="D70" s="252"/>
       <c r="E70" s="133"/>
       <c r="F70" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="296"/>
+      <c r="G70" s="256"/>
       <c r="H70" s="130"/>
       <c r="I70" s="130"/>
       <c r="J70" s="130"/>
@@ -7078,7 +7078,7 @@
       <c r="L70" s="130"/>
       <c r="M70" s="130"/>
       <c r="N70" s="130"/>
-      <c r="O70" s="218"/>
+      <c r="O70" s="355"/>
       <c r="P70" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7113,16 +7113,16 @@
       <c r="AR70" s="3"/>
       <c r="AS70" s="3"/>
     </row>
-    <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="327"/>
-      <c r="B71" s="189"/>
-      <c r="C71" s="191"/>
-      <c r="D71" s="292"/>
+    <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="201"/>
+      <c r="B71" s="327"/>
+      <c r="C71" s="329"/>
+      <c r="D71" s="252"/>
       <c r="E71" s="133"/>
       <c r="F71" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="296"/>
+      <c r="G71" s="256"/>
       <c r="H71" s="130"/>
       <c r="I71" s="130"/>
       <c r="J71" s="130"/>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="M71" s="130"/>
       <c r="N71" s="130"/>
-      <c r="O71" s="218"/>
+      <c r="O71" s="355"/>
       <c r="P71" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7167,16 +7167,16 @@
       <c r="AR71" s="3"/>
       <c r="AS71" s="3"/>
     </row>
-    <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="327"/>
-      <c r="B72" s="189"/>
-      <c r="C72" s="191"/>
-      <c r="D72" s="292"/>
+    <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="201"/>
+      <c r="B72" s="327"/>
+      <c r="C72" s="329"/>
+      <c r="D72" s="252"/>
       <c r="E72" s="133"/>
       <c r="F72" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="296"/>
+      <c r="G72" s="256"/>
       <c r="H72" s="130"/>
       <c r="I72" s="130"/>
       <c r="J72" s="130"/>
@@ -7186,7 +7186,7 @@
         <v>24</v>
       </c>
       <c r="N72" s="130"/>
-      <c r="O72" s="218"/>
+      <c r="O72" s="355"/>
       <c r="P72" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7221,14 +7221,14 @@
       <c r="AR72" s="3"/>
       <c r="AS72" s="3"/>
     </row>
-    <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="327"/>
-      <c r="B73" s="189"/>
-      <c r="C73" s="191"/>
-      <c r="D73" s="221"/>
-      <c r="E73" s="222"/>
-      <c r="F73" s="222"/>
-      <c r="G73" s="222"/>
+    <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="201"/>
+      <c r="B73" s="327"/>
+      <c r="C73" s="329"/>
+      <c r="D73" s="305"/>
+      <c r="E73" s="306"/>
+      <c r="F73" s="306"/>
+      <c r="G73" s="306"/>
       <c r="H73" s="135">
         <f>SUM(H67:H72)</f>
         <v>72</v>
@@ -7289,18 +7289,18 @@
       <c r="AR73" s="2"/>
       <c r="AS73" s="2"/>
     </row>
-    <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="327"/>
-      <c r="B74" s="189"/>
-      <c r="C74" s="191"/>
-      <c r="D74" s="241" t="s">
+    <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="201"/>
+      <c r="B74" s="327"/>
+      <c r="C74" s="329"/>
+      <c r="D74" s="325" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="146"/>
       <c r="F74" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="231">
+      <c r="G74" s="315">
         <v>48</v>
       </c>
       <c r="H74" s="148"/>
@@ -7312,7 +7312,7 @@
       <c r="N74" s="148">
         <v>12</v>
       </c>
-      <c r="O74" s="209">
+      <c r="O74" s="346">
         <f>SUM(P74:P77)</f>
         <v>48</v>
       </c>
@@ -7364,16 +7364,16 @@
       <c r="AR74" s="3"/>
       <c r="AS74" s="3"/>
     </row>
-    <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="327"/>
-      <c r="B75" s="189"/>
-      <c r="C75" s="191"/>
-      <c r="D75" s="242"/>
+    <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="201"/>
+      <c r="B75" s="327"/>
+      <c r="C75" s="329"/>
+      <c r="D75" s="258"/>
       <c r="E75" s="145"/>
       <c r="F75" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="231"/>
+      <c r="G75" s="315"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117"/>
       <c r="J75" s="117"/>
@@ -7383,7 +7383,7 @@
       <c r="N75" s="117">
         <v>12</v>
       </c>
-      <c r="O75" s="209"/>
+      <c r="O75" s="346"/>
       <c r="P75" s="9">
         <f t="shared" ref="P75:P77" si="81">SUM(H75:N75)</f>
         <v>12</v>
@@ -7418,16 +7418,16 @@
       <c r="AR75" s="3"/>
       <c r="AS75" s="3"/>
     </row>
-    <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="327"/>
-      <c r="B76" s="189"/>
-      <c r="C76" s="191"/>
-      <c r="D76" s="242"/>
+    <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="201"/>
+      <c r="B76" s="327"/>
+      <c r="C76" s="329"/>
+      <c r="D76" s="258"/>
       <c r="E76" s="145"/>
       <c r="F76" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="231"/>
+      <c r="G76" s="315"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117"/>
       <c r="J76" s="117"/>
@@ -7437,7 +7437,7 @@
       <c r="N76" s="117">
         <v>12</v>
       </c>
-      <c r="O76" s="209"/>
+      <c r="O76" s="346"/>
       <c r="P76" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7472,16 +7472,16 @@
       <c r="AR76" s="3"/>
       <c r="AS76" s="3"/>
     </row>
-    <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="327"/>
-      <c r="B77" s="189"/>
-      <c r="C77" s="191"/>
-      <c r="D77" s="243"/>
+    <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="201"/>
+      <c r="B77" s="327"/>
+      <c r="C77" s="329"/>
+      <c r="D77" s="261"/>
       <c r="E77" s="145"/>
       <c r="F77" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G77" s="232"/>
+      <c r="G77" s="316"/>
       <c r="H77" s="118"/>
       <c r="I77" s="118"/>
       <c r="J77" s="118"/>
@@ -7491,7 +7491,7 @@
       <c r="N77" s="118">
         <v>12</v>
       </c>
-      <c r="O77" s="210"/>
+      <c r="O77" s="347"/>
       <c r="P77" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7526,14 +7526,14 @@
       <c r="AR77" s="3"/>
       <c r="AS77" s="3"/>
     </row>
-    <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="327"/>
-      <c r="B78" s="189"/>
-      <c r="C78" s="191"/>
-      <c r="D78" s="223"/>
-      <c r="E78" s="224"/>
-      <c r="F78" s="225"/>
-      <c r="G78" s="226"/>
+    <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="201"/>
+      <c r="B78" s="327"/>
+      <c r="C78" s="329"/>
+      <c r="D78" s="307"/>
+      <c r="E78" s="308"/>
+      <c r="F78" s="309"/>
+      <c r="G78" s="310"/>
       <c r="H78" s="112">
         <f>SUM(H74:H77)</f>
         <v>0</v>
@@ -7594,18 +7594,18 @@
       <c r="AR78" s="2"/>
       <c r="AS78" s="2"/>
     </row>
-    <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="327"/>
-      <c r="B79" s="189"/>
-      <c r="C79" s="191"/>
-      <c r="D79" s="239" t="s">
+    <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="201"/>
+      <c r="B79" s="327"/>
+      <c r="C79" s="329"/>
+      <c r="D79" s="323" t="s">
         <v>50</v>
       </c>
       <c r="E79" s="157"/>
       <c r="F79" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="G79" s="233">
+      <c r="G79" s="317">
         <v>48</v>
       </c>
       <c r="H79" s="159">
@@ -7617,7 +7617,7 @@
       <c r="L79" s="159"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
-      <c r="O79" s="213">
+      <c r="O79" s="350">
         <f>SUM(P79:P82)</f>
         <v>48</v>
       </c>
@@ -7663,16 +7663,16 @@
       <c r="AR79" s="3"/>
       <c r="AS79" s="3"/>
     </row>
-    <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="327"/>
-      <c r="B80" s="189"/>
-      <c r="C80" s="191"/>
-      <c r="D80" s="240"/>
+    <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="201"/>
+      <c r="B80" s="327"/>
+      <c r="C80" s="329"/>
+      <c r="D80" s="324"/>
       <c r="E80" s="154"/>
       <c r="F80" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G80" s="234"/>
+      <c r="G80" s="318"/>
       <c r="H80" s="156">
         <v>12</v>
       </c>
@@ -7682,7 +7682,7 @@
       <c r="L80" s="156"/>
       <c r="M80" s="156"/>
       <c r="N80" s="156"/>
-      <c r="O80" s="214"/>
+      <c r="O80" s="351"/>
       <c r="P80" s="9">
         <f t="shared" ref="P80:P82" si="83">SUM(H80:N80)</f>
         <v>12</v>
@@ -7717,16 +7717,16 @@
       <c r="AR80" s="3"/>
       <c r="AS80" s="3"/>
     </row>
-    <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="327"/>
-      <c r="B81" s="189"/>
-      <c r="C81" s="191"/>
-      <c r="D81" s="240"/>
+    <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="201"/>
+      <c r="B81" s="327"/>
+      <c r="C81" s="329"/>
+      <c r="D81" s="324"/>
       <c r="E81" s="154"/>
       <c r="F81" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G81" s="234"/>
+      <c r="G81" s="318"/>
       <c r="H81" s="156">
         <v>12</v>
       </c>
@@ -7736,7 +7736,7 @@
       <c r="L81" s="156"/>
       <c r="M81" s="156"/>
       <c r="N81" s="156"/>
-      <c r="O81" s="214"/>
+      <c r="O81" s="351"/>
       <c r="P81" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7771,16 +7771,16 @@
       <c r="AR81" s="3"/>
       <c r="AS81" s="3"/>
     </row>
-    <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="327"/>
-      <c r="B82" s="189"/>
-      <c r="C82" s="191"/>
-      <c r="D82" s="240"/>
+    <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="201"/>
+      <c r="B82" s="327"/>
+      <c r="C82" s="329"/>
+      <c r="D82" s="324"/>
       <c r="E82" s="154"/>
       <c r="F82" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="G82" s="234"/>
+      <c r="G82" s="318"/>
       <c r="H82" s="156">
         <v>12</v>
       </c>
@@ -7790,7 +7790,7 @@
       <c r="L82" s="156"/>
       <c r="M82" s="156"/>
       <c r="N82" s="156"/>
-      <c r="O82" s="214"/>
+      <c r="O82" s="351"/>
       <c r="P82" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7825,14 +7825,14 @@
       <c r="AR82" s="3"/>
       <c r="AS82" s="3"/>
     </row>
-    <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="327"/>
-      <c r="B83" s="189"/>
-      <c r="C83" s="191"/>
-      <c r="D83" s="227"/>
-      <c r="E83" s="228"/>
-      <c r="F83" s="228"/>
-      <c r="G83" s="228"/>
+    <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="201"/>
+      <c r="B83" s="327"/>
+      <c r="C83" s="329"/>
+      <c r="D83" s="311"/>
+      <c r="E83" s="312"/>
+      <c r="F83" s="312"/>
+      <c r="G83" s="312"/>
       <c r="H83" s="160">
         <f>SUM(H79:H82)</f>
         <v>48</v>
@@ -7893,18 +7893,18 @@
       <c r="AR83" s="2"/>
       <c r="AS83" s="2"/>
     </row>
-    <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="327"/>
-      <c r="B84" s="189"/>
-      <c r="C84" s="192"/>
-      <c r="D84" s="237" t="s">
+    <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="201"/>
+      <c r="B84" s="327"/>
+      <c r="C84" s="330"/>
+      <c r="D84" s="321" t="s">
         <v>51</v>
       </c>
       <c r="E84" s="125"/>
       <c r="F84" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="235">
+      <c r="G84" s="319">
         <v>48</v>
       </c>
       <c r="H84" s="126"/>
@@ -7916,7 +7916,7 @@
       <c r="L84" s="126"/>
       <c r="M84" s="126"/>
       <c r="N84" s="126"/>
-      <c r="O84" s="211">
+      <c r="O84" s="348">
         <f>SUM(P84:P87)</f>
         <v>48</v>
       </c>
@@ -7962,16 +7962,16 @@
       <c r="AR84" s="3"/>
       <c r="AS84" s="3"/>
     </row>
-    <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="327"/>
-      <c r="B85" s="189"/>
-      <c r="C85" s="192"/>
-      <c r="D85" s="238"/>
+    <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="201"/>
+      <c r="B85" s="327"/>
+      <c r="C85" s="330"/>
+      <c r="D85" s="322"/>
       <c r="E85" s="123"/>
       <c r="F85" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="G85" s="236"/>
+      <c r="G85" s="320"/>
       <c r="H85" s="124"/>
       <c r="I85" s="124">
         <v>12</v>
@@ -7981,7 +7981,7 @@
       <c r="L85" s="124"/>
       <c r="M85" s="124"/>
       <c r="N85" s="124"/>
-      <c r="O85" s="212"/>
+      <c r="O85" s="349"/>
       <c r="P85" s="9">
         <f t="shared" ref="P85:P87" si="90">SUM(H85:N85)</f>
         <v>12</v>
@@ -8016,16 +8016,16 @@
       <c r="AR85" s="3"/>
       <c r="AS85" s="3"/>
     </row>
-    <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="327"/>
-      <c r="B86" s="189"/>
-      <c r="C86" s="192"/>
-      <c r="D86" s="238"/>
+    <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="201"/>
+      <c r="B86" s="327"/>
+      <c r="C86" s="330"/>
+      <c r="D86" s="322"/>
       <c r="E86" s="123"/>
       <c r="F86" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="236"/>
+      <c r="G86" s="320"/>
       <c r="H86" s="124"/>
       <c r="I86" s="124">
         <v>12</v>
@@ -8035,7 +8035,7 @@
       <c r="L86" s="124"/>
       <c r="M86" s="124"/>
       <c r="N86" s="124"/>
-      <c r="O86" s="212"/>
+      <c r="O86" s="349"/>
       <c r="P86" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8070,16 +8070,16 @@
       <c r="AR86" s="3"/>
       <c r="AS86" s="3"/>
     </row>
-    <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="328"/>
-      <c r="B87" s="189"/>
-      <c r="C87" s="192"/>
-      <c r="D87" s="238"/>
+    <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="202"/>
+      <c r="B87" s="327"/>
+      <c r="C87" s="330"/>
+      <c r="D87" s="322"/>
       <c r="E87" s="123"/>
       <c r="F87" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="236"/>
+      <c r="G87" s="320"/>
       <c r="H87" s="124"/>
       <c r="I87" s="124">
         <v>12</v>
@@ -8089,7 +8089,7 @@
       <c r="L87" s="124"/>
       <c r="M87" s="124"/>
       <c r="N87" s="124"/>
-      <c r="O87" s="212"/>
+      <c r="O87" s="349"/>
       <c r="P87" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8124,14 +8124,14 @@
       <c r="AR87" s="3"/>
       <c r="AS87" s="3"/>
     </row>
-    <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
-      <c r="B88" s="189"/>
-      <c r="C88" s="192"/>
-      <c r="D88" s="229"/>
-      <c r="E88" s="230"/>
-      <c r="F88" s="230"/>
-      <c r="G88" s="230"/>
+      <c r="B88" s="327"/>
+      <c r="C88" s="330"/>
+      <c r="D88" s="313"/>
+      <c r="E88" s="314"/>
+      <c r="F88" s="314"/>
+      <c r="G88" s="314"/>
       <c r="H88" s="162">
         <f>SUM(H84:H87)</f>
         <v>0</v>
@@ -8192,10 +8192,10 @@
       <c r="AR88" s="2"/>
       <c r="AS88" s="2"/>
     </row>
-    <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
-      <c r="B89" s="189"/>
-      <c r="C89" s="192"/>
+      <c r="B89" s="327"/>
+      <c r="C89" s="330"/>
       <c r="D89" s="122" t="s">
         <v>17</v>
       </c>
@@ -8261,14 +8261,14 @@
       <c r="AR89" s="3"/>
       <c r="AS89" s="3"/>
     </row>
-    <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
-      <c r="B90" s="189"/>
-      <c r="C90" s="192"/>
-      <c r="D90" s="219"/>
-      <c r="E90" s="220"/>
-      <c r="F90" s="220"/>
-      <c r="G90" s="220"/>
+      <c r="B90" s="327"/>
+      <c r="C90" s="330"/>
+      <c r="D90" s="196"/>
+      <c r="E90" s="304"/>
+      <c r="F90" s="304"/>
+      <c r="G90" s="304"/>
       <c r="H90" s="140">
         <f t="shared" ref="H90:N90" si="97">SUM(H89:H89)</f>
         <v>48</v>
@@ -8329,7 +8329,7 @@
       <c r="AR90" s="2"/>
       <c r="AS90" s="2"/>
     </row>
-    <row r="91" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H91" s="164">
         <f t="shared" ref="H91:N91" si="98">SUM(H6+H11+H16+H21+H26+H31+H36+H41+H46+H51+H56+H61+H66+H73+H78+H83+H88+H90)</f>
         <v>480</v>
@@ -8364,7 +8364,7 @@
       </c>
       <c r="Q91" s="121"/>
     </row>
-    <row r="93" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H93" s="166">
         <f t="shared" ref="H93:N93" si="99">IF(H91=0,"SIN HORAS",432-H91)</f>
         <v>-48</v>
@@ -8394,32 +8394,91 @@
         <v>-48</v>
       </c>
     </row>
-    <row r="97" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H97" s="193" t="s">
+    <row r="97" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H97" s="303" t="s">
         <v>104</v>
       </c>
-      <c r="I97" s="193"/>
-      <c r="J97" s="193"/>
-    </row>
-    <row r="99" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="I99" s="193" t="s">
+      <c r="I97" s="303"/>
+      <c r="J97" s="303"/>
+    </row>
+    <row r="99" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="I99" s="303" t="s">
         <v>105</v>
       </c>
-      <c r="J99" s="193"/>
-      <c r="K99" s="193"/>
-      <c r="L99" s="193"/>
-    </row>
-    <row r="101" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="K101" s="193" t="s">
+      <c r="J99" s="303"/>
+      <c r="K99" s="303"/>
+      <c r="L99" s="303"/>
+    </row>
+    <row r="101" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="K101" s="303" t="s">
         <v>106</v>
       </c>
-      <c r="L101" s="193"/>
-      <c r="M101" s="193"/>
-      <c r="N101" s="193"/>
+      <c r="L101" s="303"/>
+      <c r="M101" s="303"/>
+      <c r="N101" s="303"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS91" xr:uid="{44B9DB88-0080-4900-9B58-5C638DC6AAB3}"/>
   <mergeCells count="75">
+    <mergeCell ref="O74:O77"/>
+    <mergeCell ref="O84:O87"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="O67:O72"/>
+    <mergeCell ref="B2:B90"/>
+    <mergeCell ref="C2:C90"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="O32:O35"/>
+    <mergeCell ref="O37:O40"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O52:O55"/>
+    <mergeCell ref="O57:O60"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="G12:G15"/>
     <mergeCell ref="D17:D20"/>
@@ -8436,65 +8495,6 @@
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="G37:G40"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O52:O55"/>
-    <mergeCell ref="O57:O60"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="O32:O35"/>
-    <mergeCell ref="O37:O40"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="K101:N101"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="B2:B90"/>
-    <mergeCell ref="C2:C90"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="O74:O77"/>
-    <mergeCell ref="O84:O87"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="O67:O72"/>
   </mergeCells>
   <conditionalFormatting sqref="H93:N93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Se modifico el controlador del la extracion del excel y se agrego el filto de competencias y resultados de aprendizaje para que se muestren un triemestre adelante del que ya esta la ficha
</commit_message>
<xml_diff>
--- a/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
+++ b/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919AAABB-E5C9-4E23-8F90-20831E169821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37981CEF-84DD-4AB1-9DAB-A0813A16FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="113">
   <si>
     <t>DENOMINACION</t>
   </si>
@@ -376,50 +376,14 @@
     <t>INSTRUCTOR</t>
   </si>
   <si>
-    <t>LUIS F GARCIA</t>
-  </si>
-  <si>
-    <t>BEATRIZ ALFARO</t>
-  </si>
-  <si>
-    <t>ANEDIA GONZALEZ</t>
-  </si>
-  <si>
-    <t>DAVID ARRIETA</t>
-  </si>
-  <si>
-    <t>FERNANDO FLOREZ</t>
-  </si>
-  <si>
-    <t>PILAR PRADA</t>
-  </si>
-  <si>
-    <t>LUIS PEREZ</t>
-  </si>
-  <si>
-    <t>YOVANNI URREGO</t>
-  </si>
-  <si>
-    <t>OSMEIDA RAMIREZ</t>
-  </si>
-  <si>
-    <t>ANDRES MARQUEZ</t>
-  </si>
-  <si>
-    <t>LUZ E CARRIAZO</t>
-  </si>
-  <si>
-    <t>JORGE VASQUEZ</t>
-  </si>
-  <si>
-    <t>ENADITH HERNANDEZ</t>
+    <t>MARRUGO LEYVA  WILLIAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +465,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1219,7 +1197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1780,24 +1758,435 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1873,416 +2262,12 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2633,11 +2618,11 @@
   <dimension ref="A1:AS101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K83" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="AJ87" sqref="AJ87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,16 +2743,16 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="326" t="s">
+      <c r="A2" s="200" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="188">
+      <c r="B2" s="326">
         <v>228183</v>
       </c>
-      <c r="C2" s="190">
+      <c r="C2" s="328">
         <v>2</v>
       </c>
-      <c r="D2" s="329" t="s">
+      <c r="D2" s="203" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
@@ -2776,7 +2761,7 @@
       <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="332">
+      <c r="G2" s="206">
         <v>528</v>
       </c>
       <c r="H2" s="12"/>
@@ -2788,7 +2773,7 @@
       <c r="N2" s="12">
         <v>72</v>
       </c>
-      <c r="O2" s="276">
+      <c r="O2" s="273">
         <f>SUM(P2:P5)</f>
         <v>528</v>
       </c>
@@ -2854,7 +2839,7 @@
         <f>AG2/O2</f>
         <v>1</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AI2" s="356" t="s">
         <v>112</v>
       </c>
       <c r="AJ2" s="2"/>
@@ -2869,17 +2854,17 @@
       <c r="AS2" s="2"/>
     </row>
     <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="327"/>
-      <c r="B3" s="189"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="330"/>
+      <c r="A3" s="201"/>
+      <c r="B3" s="327"/>
+      <c r="C3" s="329"/>
+      <c r="D3" s="204"/>
       <c r="E3" s="13">
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="333"/>
+      <c r="G3" s="207"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -2889,7 +2874,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="277"/>
+      <c r="O3" s="274"/>
       <c r="P3" s="9">
         <f>SUM(H3:N3)</f>
         <v>64</v>
@@ -2925,17 +2910,17 @@
       <c r="AS3" s="2"/>
     </row>
     <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="327"/>
-      <c r="B4" s="189"/>
-      <c r="C4" s="191"/>
-      <c r="D4" s="330"/>
+      <c r="A4" s="201"/>
+      <c r="B4" s="327"/>
+      <c r="C4" s="329"/>
+      <c r="D4" s="204"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="333"/>
+      <c r="G4" s="207"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2945,7 +2930,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="277"/>
+      <c r="O4" s="274"/>
       <c r="P4" s="9">
         <f>SUM(H4:N4)</f>
         <v>80</v>
@@ -2981,17 +2966,17 @@
       <c r="AS4" s="2"/>
     </row>
     <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="327"/>
-      <c r="B5" s="189"/>
-      <c r="C5" s="191"/>
-      <c r="D5" s="331"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="327"/>
+      <c r="C5" s="329"/>
+      <c r="D5" s="205"/>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="334"/>
+      <c r="G5" s="208"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -3005,7 +2990,7 @@
       <c r="N5" s="18">
         <v>168</v>
       </c>
-      <c r="O5" s="278"/>
+      <c r="O5" s="275"/>
       <c r="P5" s="9">
         <f>SUM(H5:N5)</f>
         <v>312</v>
@@ -3041,13 +3026,13 @@
       <c r="AS5" s="2"/>
     </row>
     <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="327"/>
-      <c r="B6" s="189"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="196"/>
+      <c r="A6" s="201"/>
+      <c r="B6" s="327"/>
+      <c r="C6" s="329"/>
+      <c r="D6" s="331"/>
+      <c r="E6" s="332"/>
+      <c r="F6" s="332"/>
+      <c r="G6" s="333"/>
       <c r="H6" s="56">
         <f>SUM(H2:H5)</f>
         <v>0</v>
@@ -3109,10 +3094,10 @@
       <c r="AS6" s="2"/>
     </row>
     <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="327"/>
-      <c r="B7" s="189"/>
-      <c r="C7" s="191"/>
-      <c r="D7" s="335" t="s">
+      <c r="A7" s="201"/>
+      <c r="B7" s="327"/>
+      <c r="C7" s="329"/>
+      <c r="D7" s="215" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="19">
@@ -3121,7 +3106,7 @@
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="338">
+      <c r="G7" s="218">
         <v>384</v>
       </c>
       <c r="H7" s="25"/>
@@ -3133,7 +3118,7 @@
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="279">
+      <c r="O7" s="276">
         <f>SUM(P7:P10)</f>
         <v>384</v>
       </c>
@@ -3199,8 +3184,8 @@
         <f>AG7/O7</f>
         <v>1</v>
       </c>
-      <c r="AI7" s="3" t="s">
-        <v>113</v>
+      <c r="AI7" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
@@ -3214,17 +3199,17 @@
       <c r="AS7" s="3"/>
     </row>
     <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="327"/>
-      <c r="B8" s="189"/>
-      <c r="C8" s="191"/>
-      <c r="D8" s="336"/>
+      <c r="A8" s="201"/>
+      <c r="B8" s="327"/>
+      <c r="C8" s="329"/>
+      <c r="D8" s="216"/>
       <c r="E8" s="21">
         <v>3</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="339"/>
+      <c r="G8" s="219"/>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
@@ -3234,7 +3219,7 @@
         <v>144</v>
       </c>
       <c r="N8" s="26"/>
-      <c r="O8" s="280"/>
+      <c r="O8" s="277"/>
       <c r="P8" s="9">
         <f t="shared" ref="P8:P10" si="1">SUM(H8:N8)</f>
         <v>144</v>
@@ -3270,17 +3255,17 @@
       <c r="AS8" s="3"/>
     </row>
     <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="327"/>
-      <c r="B9" s="189"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="336"/>
+      <c r="A9" s="201"/>
+      <c r="B9" s="327"/>
+      <c r="C9" s="329"/>
+      <c r="D9" s="216"/>
       <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="339"/>
+      <c r="G9" s="219"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -3290,7 +3275,7 @@
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="280"/>
+      <c r="O9" s="277"/>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3326,17 +3311,17 @@
       <c r="AS9" s="3"/>
     </row>
     <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="327"/>
-      <c r="B10" s="189"/>
-      <c r="C10" s="191"/>
-      <c r="D10" s="337"/>
+      <c r="A10" s="201"/>
+      <c r="B10" s="327"/>
+      <c r="C10" s="329"/>
+      <c r="D10" s="217"/>
       <c r="E10" s="23">
         <v>4</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="340"/>
+      <c r="G10" s="220"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -3346,7 +3331,7 @@
       <c r="N10" s="27">
         <v>96</v>
       </c>
-      <c r="O10" s="281"/>
+      <c r="O10" s="278"/>
       <c r="P10" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3382,13 +3367,13 @@
       <c r="AS10" s="3"/>
     </row>
     <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="327"/>
-      <c r="B11" s="189"/>
-      <c r="C11" s="191"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="198"/>
-      <c r="F11" s="198"/>
-      <c r="G11" s="199"/>
+      <c r="A11" s="201"/>
+      <c r="B11" s="327"/>
+      <c r="C11" s="329"/>
+      <c r="D11" s="334"/>
+      <c r="E11" s="335"/>
+      <c r="F11" s="335"/>
+      <c r="G11" s="336"/>
       <c r="H11" s="61">
         <f>SUM(H7:H10)</f>
         <v>0</v>
@@ -3450,17 +3435,17 @@
       <c r="AS11" s="2"/>
     </row>
     <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="327"/>
-      <c r="B12" s="189"/>
-      <c r="C12" s="191"/>
-      <c r="D12" s="259" t="s">
+      <c r="A12" s="201"/>
+      <c r="B12" s="327"/>
+      <c r="C12" s="329"/>
+      <c r="D12" s="188" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="262">
+      <c r="G12" s="191">
         <v>48</v>
       </c>
       <c r="H12" s="34">
@@ -3472,7 +3457,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="256">
+      <c r="O12" s="279">
         <f t="shared" ref="O12" si="3">SUM(P12:P15)</f>
         <v>48</v>
       </c>
@@ -3533,20 +3518,20 @@
         <f>AG12/O12</f>
         <v>1</v>
       </c>
-      <c r="AI12" s="179" t="s">
+      <c r="AI12" s="356" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="327"/>
-      <c r="B13" s="189"/>
-      <c r="C13" s="191"/>
-      <c r="D13" s="260"/>
+      <c r="A13" s="201"/>
+      <c r="B13" s="327"/>
+      <c r="C13" s="329"/>
+      <c r="D13" s="189"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="263"/>
+      <c r="G13" s="192"/>
       <c r="H13" s="35">
         <v>12</v>
       </c>
@@ -3556,7 +3541,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="257"/>
+      <c r="O13" s="280"/>
       <c r="P13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3579,15 +3564,15 @@
       <c r="AI13" s="179"/>
     </row>
     <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="327"/>
-      <c r="B14" s="189"/>
-      <c r="C14" s="191"/>
-      <c r="D14" s="260"/>
+      <c r="A14" s="201"/>
+      <c r="B14" s="327"/>
+      <c r="C14" s="329"/>
+      <c r="D14" s="189"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="263"/>
+      <c r="G14" s="192"/>
       <c r="H14" s="35">
         <v>12</v>
       </c>
@@ -3597,7 +3582,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="257"/>
+      <c r="O14" s="280"/>
       <c r="P14" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3620,15 +3605,15 @@
       <c r="AI14" s="179"/>
     </row>
     <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="327"/>
-      <c r="B15" s="189"/>
-      <c r="C15" s="191"/>
-      <c r="D15" s="261"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="327"/>
+      <c r="C15" s="329"/>
+      <c r="D15" s="190"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="264"/>
+      <c r="G15" s="193"/>
       <c r="H15" s="36">
         <v>12</v>
       </c>
@@ -3638,7 +3623,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="258"/>
+      <c r="O15" s="281"/>
       <c r="P15" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3661,13 +3646,13 @@
       <c r="AI15" s="179"/>
     </row>
     <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="327"/>
-      <c r="B16" s="189"/>
-      <c r="C16" s="191"/>
-      <c r="D16" s="194"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="196"/>
+      <c r="A16" s="201"/>
+      <c r="B16" s="327"/>
+      <c r="C16" s="329"/>
+      <c r="D16" s="331"/>
+      <c r="E16" s="332"/>
+      <c r="F16" s="332"/>
+      <c r="G16" s="333"/>
       <c r="H16" s="56">
         <f>SUM(H12:H15)</f>
         <v>48</v>
@@ -3729,17 +3714,17 @@
       <c r="AS16" s="2"/>
     </row>
     <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="327"/>
-      <c r="B17" s="189"/>
-      <c r="C17" s="191"/>
-      <c r="D17" s="321" t="s">
+      <c r="A17" s="201"/>
+      <c r="B17" s="327"/>
+      <c r="C17" s="329"/>
+      <c r="D17" s="194" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="323">
+      <c r="G17" s="197">
         <v>48</v>
       </c>
       <c r="H17" s="44"/>
@@ -3813,8 +3798,8 @@
         <f>AG17/O17</f>
         <v>1</v>
       </c>
-      <c r="AI17" s="3" t="s">
-        <v>117</v>
+      <c r="AI17" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
@@ -3828,15 +3813,15 @@
       <c r="AS17" s="3"/>
     </row>
     <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="327"/>
-      <c r="B18" s="189"/>
-      <c r="C18" s="191"/>
-      <c r="D18" s="322"/>
+      <c r="A18" s="201"/>
+      <c r="B18" s="327"/>
+      <c r="C18" s="329"/>
+      <c r="D18" s="195"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="324"/>
+      <c r="G18" s="198"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45">
         <v>12</v>
@@ -3882,15 +3867,15 @@
       <c r="AS18" s="3"/>
     </row>
     <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="327"/>
-      <c r="B19" s="189"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="322"/>
+      <c r="A19" s="201"/>
+      <c r="B19" s="327"/>
+      <c r="C19" s="329"/>
+      <c r="D19" s="195"/>
       <c r="E19" s="39"/>
       <c r="F19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="324"/>
+      <c r="G19" s="198"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45">
         <v>12</v>
@@ -3936,15 +3921,15 @@
       <c r="AS19" s="3"/>
     </row>
     <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="327"/>
-      <c r="B20" s="189"/>
-      <c r="C20" s="191"/>
-      <c r="D20" s="219"/>
+      <c r="A20" s="201"/>
+      <c r="B20" s="327"/>
+      <c r="C20" s="329"/>
+      <c r="D20" s="196"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="325"/>
+      <c r="G20" s="199"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46">
         <v>12</v>
@@ -3990,13 +3975,13 @@
       <c r="AS20" s="3"/>
     </row>
     <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="327"/>
-      <c r="B21" s="189"/>
-      <c r="C21" s="191"/>
-      <c r="D21" s="200"/>
-      <c r="E21" s="201"/>
-      <c r="F21" s="201"/>
-      <c r="G21" s="202"/>
+      <c r="A21" s="201"/>
+      <c r="B21" s="327"/>
+      <c r="C21" s="329"/>
+      <c r="D21" s="337"/>
+      <c r="E21" s="338"/>
+      <c r="F21" s="338"/>
+      <c r="G21" s="339"/>
       <c r="H21" s="62">
         <f>SUM(H17:H20)</f>
         <v>0</v>
@@ -4058,10 +4043,10 @@
       <c r="AS21" s="2"/>
     </row>
     <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="327"/>
-      <c r="B22" s="189"/>
-      <c r="C22" s="191"/>
-      <c r="D22" s="318" t="s">
+      <c r="A22" s="201"/>
+      <c r="B22" s="327"/>
+      <c r="C22" s="329"/>
+      <c r="D22" s="209" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="47">
@@ -4070,7 +4055,7 @@
       <c r="F22" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="306">
+      <c r="G22" s="212">
         <v>336</v>
       </c>
       <c r="H22" s="53"/>
@@ -4080,7 +4065,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="53"/>
       <c r="N22" s="53"/>
-      <c r="O22" s="271">
+      <c r="O22" s="268">
         <f t="shared" ref="O22" si="13">SUM(P22:P25)</f>
         <v>336</v>
       </c>
@@ -4152,8 +4137,8 @@
         <f>AG22/O22</f>
         <v>1</v>
       </c>
-      <c r="AI22" s="3" t="s">
-        <v>118</v>
+      <c r="AI22" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
@@ -4167,17 +4152,17 @@
       <c r="AS22" s="3"/>
     </row>
     <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="327"/>
-      <c r="B23" s="189"/>
-      <c r="C23" s="191"/>
-      <c r="D23" s="319"/>
+      <c r="A23" s="201"/>
+      <c r="B23" s="327"/>
+      <c r="C23" s="329"/>
+      <c r="D23" s="210"/>
       <c r="E23" s="49">
         <v>2</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="307"/>
+      <c r="G23" s="213"/>
       <c r="H23" s="54">
         <v>72</v>
       </c>
@@ -4187,7 +4172,7 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="272"/>
+      <c r="O23" s="269"/>
       <c r="P23" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4223,17 +4208,17 @@
       <c r="AS23" s="3"/>
     </row>
     <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="327"/>
-      <c r="B24" s="189"/>
-      <c r="C24" s="191"/>
-      <c r="D24" s="319"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="327"/>
+      <c r="C24" s="329"/>
+      <c r="D24" s="210"/>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="307"/>
+      <c r="G24" s="213"/>
       <c r="H24" s="54">
         <v>72</v>
       </c>
@@ -4243,7 +4228,7 @@
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
-      <c r="O24" s="272"/>
+      <c r="O24" s="269"/>
       <c r="P24" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4279,17 +4264,17 @@
       <c r="AS24" s="3"/>
     </row>
     <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="327"/>
-      <c r="B25" s="189"/>
-      <c r="C25" s="191"/>
-      <c r="D25" s="320"/>
+      <c r="A25" s="201"/>
+      <c r="B25" s="327"/>
+      <c r="C25" s="329"/>
+      <c r="D25" s="211"/>
       <c r="E25" s="51">
         <v>3</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="308"/>
+      <c r="G25" s="214"/>
       <c r="H25" s="55"/>
       <c r="I25" s="55">
         <v>72</v>
@@ -4301,7 +4286,7 @@
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
-      <c r="O25" s="273"/>
+      <c r="O25" s="270"/>
       <c r="P25" s="9">
         <f t="shared" si="4"/>
         <v>192</v>
@@ -4337,13 +4322,13 @@
       <c r="AS25" s="3"/>
     </row>
     <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="327"/>
-      <c r="B26" s="189"/>
-      <c r="C26" s="191"/>
-      <c r="D26" s="203"/>
-      <c r="E26" s="204"/>
-      <c r="F26" s="204"/>
-      <c r="G26" s="205"/>
+      <c r="A26" s="201"/>
+      <c r="B26" s="327"/>
+      <c r="C26" s="329"/>
+      <c r="D26" s="340"/>
+      <c r="E26" s="341"/>
+      <c r="F26" s="341"/>
+      <c r="G26" s="342"/>
       <c r="H26" s="64">
         <f>SUM(H22:H25)</f>
         <v>144</v>
@@ -4405,10 +4390,10 @@
       <c r="AS26" s="2"/>
     </row>
     <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="327"/>
-      <c r="B27" s="189"/>
-      <c r="C27" s="191"/>
-      <c r="D27" s="353" t="s">
+      <c r="A27" s="201"/>
+      <c r="B27" s="327"/>
+      <c r="C27" s="329"/>
+      <c r="D27" s="233" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="65">
@@ -4417,7 +4402,7 @@
       <c r="F27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="341">
+      <c r="G27" s="221">
         <v>576</v>
       </c>
       <c r="H27" s="73"/>
@@ -4501,7 +4486,7 @@
         <f>AG27/O27</f>
         <v>1</v>
       </c>
-      <c r="AI27" s="3" t="s">
+      <c r="AI27" s="356" t="s">
         <v>112</v>
       </c>
       <c r="AJ27" s="3"/>
@@ -4516,17 +4501,17 @@
       <c r="AS27" s="3"/>
     </row>
     <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="327"/>
-      <c r="B28" s="189"/>
-      <c r="C28" s="191"/>
-      <c r="D28" s="354"/>
+      <c r="A28" s="201"/>
+      <c r="B28" s="327"/>
+      <c r="C28" s="329"/>
+      <c r="D28" s="234"/>
       <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="342"/>
+      <c r="G28" s="222"/>
       <c r="H28" s="74"/>
       <c r="I28" s="74">
         <v>72</v>
@@ -4572,17 +4557,17 @@
       <c r="AS28" s="3"/>
     </row>
     <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="327"/>
-      <c r="B29" s="189"/>
-      <c r="C29" s="191"/>
-      <c r="D29" s="354"/>
+      <c r="A29" s="201"/>
+      <c r="B29" s="327"/>
+      <c r="C29" s="329"/>
+      <c r="D29" s="234"/>
       <c r="E29" s="67">
         <v>1</v>
       </c>
       <c r="F29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="342"/>
+      <c r="G29" s="222"/>
       <c r="H29" s="74">
         <v>72</v>
       </c>
@@ -4628,17 +4613,17 @@
       <c r="AS29" s="3"/>
     </row>
     <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="327"/>
-      <c r="B30" s="189"/>
-      <c r="C30" s="191"/>
-      <c r="D30" s="355"/>
+      <c r="A30" s="201"/>
+      <c r="B30" s="327"/>
+      <c r="C30" s="329"/>
+      <c r="D30" s="235"/>
       <c r="E30" s="69">
         <v>3</v>
       </c>
       <c r="F30" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="343"/>
+      <c r="G30" s="223"/>
       <c r="H30" s="75"/>
       <c r="I30" s="75">
         <v>72</v>
@@ -4690,13 +4675,13 @@
       <c r="AS30" s="3"/>
     </row>
     <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="327"/>
-      <c r="B31" s="189"/>
-      <c r="C31" s="191"/>
-      <c r="D31" s="206"/>
-      <c r="E31" s="207"/>
-      <c r="F31" s="207"/>
-      <c r="G31" s="208"/>
+      <c r="A31" s="201"/>
+      <c r="B31" s="327"/>
+      <c r="C31" s="329"/>
+      <c r="D31" s="343"/>
+      <c r="E31" s="344"/>
+      <c r="F31" s="344"/>
+      <c r="G31" s="345"/>
       <c r="H31" s="71">
         <f>SUM(H27:H30)</f>
         <v>72</v>
@@ -4758,17 +4743,17 @@
       <c r="AS31" s="2"/>
     </row>
     <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="327"/>
-      <c r="B32" s="189"/>
-      <c r="C32" s="191"/>
-      <c r="D32" s="265" t="s">
+      <c r="A32" s="201"/>
+      <c r="B32" s="327"/>
+      <c r="C32" s="329"/>
+      <c r="D32" s="300" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="344">
+      <c r="G32" s="224">
         <v>48</v>
       </c>
       <c r="H32" s="82"/>
@@ -4780,7 +4765,7 @@
         <v>12</v>
       </c>
       <c r="N32" s="82"/>
-      <c r="O32" s="250">
+      <c r="O32" s="294">
         <f t="shared" ref="O32" si="27">SUM(P32:P35)</f>
         <v>48</v>
       </c>
@@ -4841,20 +4826,20 @@
         <f>AG32/O32</f>
         <v>1</v>
       </c>
-      <c r="AI32" t="s">
-        <v>119</v>
+      <c r="AI32" s="356" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="327"/>
-      <c r="B33" s="189"/>
-      <c r="C33" s="191"/>
-      <c r="D33" s="266"/>
+      <c r="A33" s="201"/>
+      <c r="B33" s="327"/>
+      <c r="C33" s="329"/>
+      <c r="D33" s="301"/>
       <c r="E33" s="78"/>
       <c r="F33" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="345"/>
+      <c r="G33" s="225"/>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -4864,7 +4849,7 @@
         <v>12</v>
       </c>
       <c r="N33" s="83"/>
-      <c r="O33" s="251"/>
+      <c r="O33" s="295"/>
       <c r="P33" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4886,15 +4871,15 @@
       <c r="AE33" s="179"/>
     </row>
     <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="327"/>
-      <c r="B34" s="189"/>
-      <c r="C34" s="191"/>
-      <c r="D34" s="266"/>
+      <c r="A34" s="201"/>
+      <c r="B34" s="327"/>
+      <c r="C34" s="329"/>
+      <c r="D34" s="301"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="345"/>
+      <c r="G34" s="225"/>
       <c r="H34" s="83"/>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -4904,7 +4889,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="83"/>
-      <c r="O34" s="251"/>
+      <c r="O34" s="295"/>
       <c r="P34" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4926,15 +4911,15 @@
       <c r="AE34" s="179"/>
     </row>
     <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="327"/>
-      <c r="B35" s="189"/>
-      <c r="C35" s="191"/>
-      <c r="D35" s="267"/>
+      <c r="A35" s="201"/>
+      <c r="B35" s="327"/>
+      <c r="C35" s="329"/>
+      <c r="D35" s="302"/>
       <c r="E35" s="80"/>
       <c r="F35" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="346"/>
+      <c r="G35" s="226"/>
       <c r="H35" s="84"/>
       <c r="I35" s="84"/>
       <c r="J35" s="84"/>
@@ -4944,7 +4929,7 @@
         <v>12</v>
       </c>
       <c r="N35" s="84"/>
-      <c r="O35" s="252"/>
+      <c r="O35" s="296"/>
       <c r="P35" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4966,13 +4951,13 @@
       <c r="AE35" s="179"/>
     </row>
     <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="327"/>
-      <c r="B36" s="189"/>
-      <c r="C36" s="191"/>
-      <c r="D36" s="244"/>
-      <c r="E36" s="245"/>
-      <c r="F36" s="245"/>
-      <c r="G36" s="246"/>
+      <c r="A36" s="201"/>
+      <c r="B36" s="327"/>
+      <c r="C36" s="329"/>
+      <c r="D36" s="288"/>
+      <c r="E36" s="289"/>
+      <c r="F36" s="289"/>
+      <c r="G36" s="290"/>
       <c r="H36" s="86">
         <f>SUM(H32:H35)</f>
         <v>0</v>
@@ -5034,17 +5019,17 @@
       <c r="AS36" s="2"/>
     </row>
     <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="327"/>
-      <c r="B37" s="189"/>
-      <c r="C37" s="191"/>
-      <c r="D37" s="347" t="s">
+      <c r="A37" s="201"/>
+      <c r="B37" s="327"/>
+      <c r="C37" s="329"/>
+      <c r="D37" s="227" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="350">
+      <c r="G37" s="230">
         <v>48</v>
       </c>
       <c r="H37" s="95"/>
@@ -5056,7 +5041,7 @@
       <c r="N37" s="95">
         <v>12</v>
       </c>
-      <c r="O37" s="253">
+      <c r="O37" s="297">
         <f t="shared" ref="O37" si="34">SUM(P37:P40)</f>
         <v>48</v>
       </c>
@@ -5094,8 +5079,8 @@
         <f>AG37/O37</f>
         <v>1</v>
       </c>
-      <c r="AI37" s="3" t="s">
-        <v>114</v>
+      <c r="AI37" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
@@ -5109,15 +5094,15 @@
       <c r="AS37" s="3"/>
     </row>
     <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="327"/>
-      <c r="B38" s="189"/>
-      <c r="C38" s="191"/>
-      <c r="D38" s="348"/>
+      <c r="A38" s="201"/>
+      <c r="B38" s="327"/>
+      <c r="C38" s="329"/>
+      <c r="D38" s="228"/>
       <c r="E38" s="89"/>
       <c r="F38" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="351"/>
+      <c r="G38" s="231"/>
       <c r="H38" s="96"/>
       <c r="I38" s="96"/>
       <c r="J38" s="96"/>
@@ -5127,7 +5112,7 @@
       <c r="N38" s="96">
         <v>12</v>
       </c>
-      <c r="O38" s="254"/>
+      <c r="O38" s="298"/>
       <c r="P38" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5163,15 +5148,15 @@
       <c r="AS38" s="3"/>
     </row>
     <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="327"/>
-      <c r="B39" s="189"/>
-      <c r="C39" s="191"/>
-      <c r="D39" s="348"/>
+      <c r="A39" s="201"/>
+      <c r="B39" s="327"/>
+      <c r="C39" s="329"/>
+      <c r="D39" s="228"/>
       <c r="E39" s="89"/>
       <c r="F39" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="351"/>
+      <c r="G39" s="231"/>
       <c r="H39" s="96"/>
       <c r="I39" s="96"/>
       <c r="J39" s="96"/>
@@ -5181,7 +5166,7 @@
       <c r="N39" s="96">
         <v>12</v>
       </c>
-      <c r="O39" s="254"/>
+      <c r="O39" s="298"/>
       <c r="P39" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5217,15 +5202,15 @@
       <c r="AS39" s="3"/>
     </row>
     <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="327"/>
-      <c r="B40" s="189"/>
-      <c r="C40" s="191"/>
-      <c r="D40" s="349"/>
+      <c r="A40" s="201"/>
+      <c r="B40" s="327"/>
+      <c r="C40" s="329"/>
+      <c r="D40" s="229"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="352"/>
+      <c r="G40" s="232"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
       <c r="J40" s="97"/>
@@ -5235,7 +5220,7 @@
       <c r="N40" s="97">
         <v>12</v>
       </c>
-      <c r="O40" s="255"/>
+      <c r="O40" s="299"/>
       <c r="P40" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5271,13 +5256,13 @@
       <c r="AS40" s="3"/>
     </row>
     <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="327"/>
-      <c r="B41" s="189"/>
-      <c r="C41" s="191"/>
-      <c r="D41" s="247"/>
-      <c r="E41" s="248"/>
-      <c r="F41" s="248"/>
-      <c r="G41" s="249"/>
+      <c r="A41" s="201"/>
+      <c r="B41" s="327"/>
+      <c r="C41" s="329"/>
+      <c r="D41" s="291"/>
+      <c r="E41" s="292"/>
+      <c r="F41" s="292"/>
+      <c r="G41" s="293"/>
       <c r="H41" s="93">
         <f>SUM(H37:H40)</f>
         <v>0</v>
@@ -5339,17 +5324,17 @@
       <c r="AS41" s="2"/>
     </row>
     <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="327"/>
-      <c r="B42" s="189"/>
-      <c r="C42" s="191"/>
-      <c r="D42" s="259" t="s">
+      <c r="A42" s="201"/>
+      <c r="B42" s="327"/>
+      <c r="C42" s="329"/>
+      <c r="D42" s="188" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="262">
+      <c r="G42" s="191">
         <v>48</v>
       </c>
       <c r="H42" s="34">
@@ -5361,7 +5346,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
-      <c r="O42" s="256">
+      <c r="O42" s="279">
         <f t="shared" ref="O42" si="41">SUM(P42:P45)</f>
         <v>48</v>
       </c>
@@ -5399,8 +5384,8 @@
         <f>AG42/O42</f>
         <v>1</v>
       </c>
-      <c r="AI42" s="3" t="s">
-        <v>120</v>
+      <c r="AI42" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -5414,15 +5399,15 @@
       <c r="AS42" s="3"/>
     </row>
     <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="327"/>
-      <c r="B43" s="189"/>
-      <c r="C43" s="191"/>
-      <c r="D43" s="260"/>
+      <c r="A43" s="201"/>
+      <c r="B43" s="327"/>
+      <c r="C43" s="329"/>
+      <c r="D43" s="189"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="263"/>
+      <c r="G43" s="192"/>
       <c r="H43" s="35">
         <v>12</v>
       </c>
@@ -5432,7 +5417,7 @@
       <c r="L43" s="35"/>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="257"/>
+      <c r="O43" s="280"/>
       <c r="P43" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5468,15 +5453,15 @@
       <c r="AS43" s="3"/>
     </row>
     <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="327"/>
-      <c r="B44" s="189"/>
-      <c r="C44" s="191"/>
-      <c r="D44" s="260"/>
+      <c r="A44" s="201"/>
+      <c r="B44" s="327"/>
+      <c r="C44" s="329"/>
+      <c r="D44" s="189"/>
       <c r="E44" s="30"/>
       <c r="F44" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="263"/>
+      <c r="G44" s="192"/>
       <c r="H44" s="35">
         <v>12</v>
       </c>
@@ -5486,7 +5471,7 @@
       <c r="L44" s="35"/>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
-      <c r="O44" s="257"/>
+      <c r="O44" s="280"/>
       <c r="P44" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5522,15 +5507,15 @@
       <c r="AS44" s="3"/>
     </row>
     <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="327"/>
-      <c r="B45" s="189"/>
-      <c r="C45" s="191"/>
-      <c r="D45" s="261"/>
+      <c r="A45" s="201"/>
+      <c r="B45" s="327"/>
+      <c r="C45" s="329"/>
+      <c r="D45" s="190"/>
       <c r="E45" s="32"/>
       <c r="F45" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="264"/>
+      <c r="G45" s="193"/>
       <c r="H45" s="36">
         <v>12</v>
       </c>
@@ -5540,7 +5525,7 @@
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
-      <c r="O45" s="258"/>
+      <c r="O45" s="281"/>
       <c r="P45" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5576,13 +5561,13 @@
       <c r="AS45" s="3"/>
     </row>
     <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="327"/>
-      <c r="B46" s="189"/>
-      <c r="C46" s="191"/>
-      <c r="D46" s="309"/>
-      <c r="E46" s="310"/>
-      <c r="F46" s="310"/>
-      <c r="G46" s="311"/>
+      <c r="A46" s="201"/>
+      <c r="B46" s="327"/>
+      <c r="C46" s="329"/>
+      <c r="D46" s="239"/>
+      <c r="E46" s="240"/>
+      <c r="F46" s="240"/>
+      <c r="G46" s="241"/>
       <c r="H46" s="98">
         <f>SUM(H42:H45)</f>
         <v>48</v>
@@ -5644,17 +5629,17 @@
       <c r="AS46" s="2"/>
     </row>
     <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="327"/>
-      <c r="B47" s="189"/>
-      <c r="C47" s="191"/>
-      <c r="D47" s="315" t="s">
+      <c r="A47" s="201"/>
+      <c r="B47" s="327"/>
+      <c r="C47" s="329"/>
+      <c r="D47" s="245" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="99"/>
       <c r="F47" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="303">
+      <c r="G47" s="236">
         <v>48</v>
       </c>
       <c r="H47" s="107"/>
@@ -5666,7 +5651,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
-      <c r="O47" s="268">
+      <c r="O47" s="265">
         <f t="shared" ref="O47" si="48">SUM(P47:P50)</f>
         <v>48</v>
       </c>
@@ -5703,20 +5688,20 @@
         <f>AG47/O47</f>
         <v>1</v>
       </c>
-      <c r="AI47" t="s">
-        <v>121</v>
+      <c r="AI47" s="356" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="327"/>
-      <c r="B48" s="189"/>
-      <c r="C48" s="191"/>
-      <c r="D48" s="316"/>
+      <c r="A48" s="201"/>
+      <c r="B48" s="327"/>
+      <c r="C48" s="329"/>
+      <c r="D48" s="246"/>
       <c r="E48" s="101"/>
       <c r="F48" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="304"/>
+      <c r="G48" s="237"/>
       <c r="H48" s="108"/>
       <c r="I48" s="108">
         <v>12</v>
@@ -5726,7 +5711,7 @@
       <c r="L48" s="108"/>
       <c r="M48" s="108"/>
       <c r="N48" s="108"/>
-      <c r="O48" s="269"/>
+      <c r="O48" s="266"/>
       <c r="P48" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5748,15 +5733,15 @@
       <c r="AE48" s="179"/>
     </row>
     <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="327"/>
-      <c r="B49" s="189"/>
-      <c r="C49" s="191"/>
-      <c r="D49" s="316"/>
+      <c r="A49" s="201"/>
+      <c r="B49" s="327"/>
+      <c r="C49" s="329"/>
+      <c r="D49" s="246"/>
       <c r="E49" s="101"/>
       <c r="F49" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="304"/>
+      <c r="G49" s="237"/>
       <c r="H49" s="108"/>
       <c r="I49" s="108">
         <v>12</v>
@@ -5766,7 +5751,7 @@
       <c r="L49" s="108"/>
       <c r="M49" s="108"/>
       <c r="N49" s="108"/>
-      <c r="O49" s="269"/>
+      <c r="O49" s="266"/>
       <c r="P49" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5788,15 +5773,15 @@
       <c r="AE49" s="179"/>
     </row>
     <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="327"/>
-      <c r="B50" s="189"/>
-      <c r="C50" s="191"/>
-      <c r="D50" s="317"/>
+      <c r="A50" s="201"/>
+      <c r="B50" s="327"/>
+      <c r="C50" s="329"/>
+      <c r="D50" s="247"/>
       <c r="E50" s="103"/>
       <c r="F50" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="G50" s="305"/>
+      <c r="G50" s="238"/>
       <c r="H50" s="109"/>
       <c r="I50" s="109">
         <v>12</v>
@@ -5806,7 +5791,7 @@
       <c r="L50" s="109"/>
       <c r="M50" s="109"/>
       <c r="N50" s="109"/>
-      <c r="O50" s="270"/>
+      <c r="O50" s="267"/>
       <c r="P50" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5828,13 +5813,13 @@
       <c r="AE50" s="179"/>
     </row>
     <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="327"/>
-      <c r="B51" s="189"/>
-      <c r="C51" s="191"/>
-      <c r="D51" s="312"/>
-      <c r="E51" s="313"/>
-      <c r="F51" s="313"/>
-      <c r="G51" s="314"/>
+      <c r="A51" s="201"/>
+      <c r="B51" s="327"/>
+      <c r="C51" s="329"/>
+      <c r="D51" s="242"/>
+      <c r="E51" s="243"/>
+      <c r="F51" s="243"/>
+      <c r="G51" s="244"/>
       <c r="H51" s="106">
         <f>SUM(H47:H50)</f>
         <v>0</v>
@@ -5896,17 +5881,17 @@
       <c r="AS51" s="2"/>
     </row>
     <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="327"/>
-      <c r="B52" s="189"/>
-      <c r="C52" s="191"/>
-      <c r="D52" s="318" t="s">
+      <c r="A52" s="201"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="329"/>
+      <c r="D52" s="209" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="47"/>
       <c r="F52" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G52" s="306">
+      <c r="G52" s="212">
         <v>48</v>
       </c>
       <c r="H52" s="53"/>
@@ -5918,7 +5903,7 @@
       <c r="N52" s="53">
         <v>12</v>
       </c>
-      <c r="O52" s="271">
+      <c r="O52" s="268">
         <f t="shared" ref="O52" si="55">SUM(P52:P55)</f>
         <v>48</v>
       </c>
@@ -5956,8 +5941,8 @@
         <f>AG52/O52</f>
         <v>1</v>
       </c>
-      <c r="AI52" s="3" t="s">
-        <v>115</v>
+      <c r="AI52" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
@@ -5971,15 +5956,15 @@
       <c r="AS52" s="3"/>
     </row>
     <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="327"/>
-      <c r="B53" s="189"/>
-      <c r="C53" s="191"/>
-      <c r="D53" s="319"/>
+      <c r="A53" s="201"/>
+      <c r="B53" s="327"/>
+      <c r="C53" s="329"/>
+      <c r="D53" s="210"/>
       <c r="E53" s="49"/>
       <c r="F53" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G53" s="307"/>
+      <c r="G53" s="213"/>
       <c r="H53" s="54"/>
       <c r="I53" s="54"/>
       <c r="J53" s="54"/>
@@ -5989,7 +5974,7 @@
       <c r="N53" s="54">
         <v>12</v>
       </c>
-      <c r="O53" s="272"/>
+      <c r="O53" s="269"/>
       <c r="P53" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6025,15 +6010,15 @@
       <c r="AS53" s="3"/>
     </row>
     <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="327"/>
-      <c r="B54" s="189"/>
-      <c r="C54" s="191"/>
-      <c r="D54" s="319"/>
+      <c r="A54" s="201"/>
+      <c r="B54" s="327"/>
+      <c r="C54" s="329"/>
+      <c r="D54" s="210"/>
       <c r="E54" s="49"/>
       <c r="F54" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="307"/>
+      <c r="G54" s="213"/>
       <c r="H54" s="54"/>
       <c r="I54" s="54"/>
       <c r="J54" s="54"/>
@@ -6043,7 +6028,7 @@
       <c r="N54" s="54">
         <v>12</v>
       </c>
-      <c r="O54" s="272"/>
+      <c r="O54" s="269"/>
       <c r="P54" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6079,15 +6064,15 @@
       <c r="AS54" s="3"/>
     </row>
     <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="327"/>
-      <c r="B55" s="189"/>
-      <c r="C55" s="191"/>
-      <c r="D55" s="320"/>
+      <c r="A55" s="201"/>
+      <c r="B55" s="327"/>
+      <c r="C55" s="329"/>
+      <c r="D55" s="211"/>
       <c r="E55" s="51"/>
       <c r="F55" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="308"/>
+      <c r="G55" s="214"/>
       <c r="H55" s="55"/>
       <c r="I55" s="55"/>
       <c r="J55" s="55"/>
@@ -6097,7 +6082,7 @@
       <c r="N55" s="55">
         <v>12</v>
       </c>
-      <c r="O55" s="273"/>
+      <c r="O55" s="270"/>
       <c r="P55" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6133,13 +6118,13 @@
       <c r="AS55" s="3"/>
     </row>
     <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="327"/>
-      <c r="B56" s="189"/>
-      <c r="C56" s="191"/>
-      <c r="D56" s="288"/>
-      <c r="E56" s="289"/>
-      <c r="F56" s="289"/>
-      <c r="G56" s="290"/>
+      <c r="A56" s="201"/>
+      <c r="B56" s="327"/>
+      <c r="C56" s="329"/>
+      <c r="D56" s="248"/>
+      <c r="E56" s="249"/>
+      <c r="F56" s="249"/>
+      <c r="G56" s="250"/>
       <c r="H56" s="64">
         <f>SUM(H52:H55)</f>
         <v>0</v>
@@ -6201,10 +6186,10 @@
       <c r="AS56" s="2"/>
     </row>
     <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="327"/>
-      <c r="B57" s="189"/>
-      <c r="C57" s="191"/>
-      <c r="D57" s="297" t="s">
+      <c r="A57" s="201"/>
+      <c r="B57" s="327"/>
+      <c r="C57" s="329"/>
+      <c r="D57" s="257" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="149">
@@ -6213,7 +6198,7 @@
       <c r="F57" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="298">
+      <c r="G57" s="259">
         <v>96</v>
       </c>
       <c r="H57" s="114"/>
@@ -6225,7 +6210,7 @@
       <c r="L57" s="114"/>
       <c r="M57" s="114"/>
       <c r="N57" s="114"/>
-      <c r="O57" s="274">
+      <c r="O57" s="271">
         <f t="shared" ref="O57" si="62">SUM(P57:P60)</f>
         <v>96</v>
       </c>
@@ -6288,8 +6273,8 @@
         <f>AG57/O57</f>
         <v>1</v>
       </c>
-      <c r="AI57" s="3" t="s">
-        <v>118</v>
+      <c r="AI57" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
@@ -6303,17 +6288,17 @@
       <c r="AS57" s="3"/>
     </row>
     <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="327"/>
-      <c r="B58" s="189"/>
-      <c r="C58" s="191"/>
-      <c r="D58" s="242"/>
+      <c r="A58" s="201"/>
+      <c r="B58" s="327"/>
+      <c r="C58" s="329"/>
+      <c r="D58" s="258"/>
       <c r="E58" s="145">
         <v>2</v>
       </c>
       <c r="F58" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="G58" s="299"/>
+      <c r="G58" s="260"/>
       <c r="H58" s="115"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115">
@@ -6323,7 +6308,7 @@
       <c r="L58" s="115"/>
       <c r="M58" s="115"/>
       <c r="N58" s="115"/>
-      <c r="O58" s="275"/>
+      <c r="O58" s="272"/>
       <c r="P58" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6359,17 +6344,17 @@
       <c r="AS58" s="7"/>
     </row>
     <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="327"/>
-      <c r="B59" s="189"/>
-      <c r="C59" s="191"/>
-      <c r="D59" s="242"/>
+      <c r="A59" s="201"/>
+      <c r="B59" s="327"/>
+      <c r="C59" s="329"/>
+      <c r="D59" s="258"/>
       <c r="E59" s="145">
         <v>4</v>
       </c>
       <c r="F59" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="299"/>
+      <c r="G59" s="260"/>
       <c r="H59" s="115"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115">
@@ -6379,7 +6364,7 @@
       <c r="L59" s="115"/>
       <c r="M59" s="115"/>
       <c r="N59" s="115"/>
-      <c r="O59" s="275"/>
+      <c r="O59" s="272"/>
       <c r="P59" s="9">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -6415,17 +6400,17 @@
       <c r="AS59" s="7"/>
     </row>
     <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="327"/>
-      <c r="B60" s="189"/>
-      <c r="C60" s="191"/>
-      <c r="D60" s="242"/>
+      <c r="A60" s="201"/>
+      <c r="B60" s="327"/>
+      <c r="C60" s="329"/>
+      <c r="D60" s="258"/>
       <c r="E60" s="145">
         <v>1</v>
       </c>
       <c r="F60" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="299"/>
+      <c r="G60" s="260"/>
       <c r="H60" s="115"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115">
@@ -6435,7 +6420,7 @@
       <c r="L60" s="115"/>
       <c r="M60" s="115"/>
       <c r="N60" s="115"/>
-      <c r="O60" s="275"/>
+      <c r="O60" s="272"/>
       <c r="P60" s="9">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -6471,13 +6456,13 @@
       <c r="AS60" s="7"/>
     </row>
     <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="327"/>
-      <c r="B61" s="189"/>
-      <c r="C61" s="191"/>
-      <c r="D61" s="243"/>
-      <c r="E61" s="300"/>
-      <c r="F61" s="300"/>
-      <c r="G61" s="300"/>
+      <c r="A61" s="201"/>
+      <c r="B61" s="327"/>
+      <c r="C61" s="329"/>
+      <c r="D61" s="261"/>
+      <c r="E61" s="262"/>
+      <c r="F61" s="262"/>
+      <c r="G61" s="262"/>
       <c r="H61" s="150">
         <f>SUM(H57:H60)</f>
         <v>0</v>
@@ -6539,10 +6524,10 @@
       <c r="AS61" s="2"/>
     </row>
     <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="327"/>
-      <c r="B62" s="189"/>
-      <c r="C62" s="191"/>
-      <c r="D62" s="293" t="s">
+      <c r="A62" s="201"/>
+      <c r="B62" s="327"/>
+      <c r="C62" s="329"/>
+      <c r="D62" s="253" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="142">
@@ -6551,7 +6536,7 @@
       <c r="F62" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="G62" s="294">
+      <c r="G62" s="254">
         <v>288</v>
       </c>
       <c r="H62" s="132"/>
@@ -6563,7 +6548,7 @@
         <v>72</v>
       </c>
       <c r="N62" s="132"/>
-      <c r="O62" s="215">
+      <c r="O62" s="352">
         <f t="shared" ref="O62" si="69">SUM(P62:P65)</f>
         <v>288</v>
       </c>
@@ -6624,8 +6609,8 @@
         <f>AG62/O62</f>
         <v>1</v>
       </c>
-      <c r="AI62" s="3" t="s">
-        <v>113</v>
+      <c r="AI62" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
@@ -6639,17 +6624,17 @@
       <c r="AS62" s="3"/>
     </row>
     <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="327"/>
-      <c r="B63" s="189"/>
-      <c r="C63" s="191"/>
-      <c r="D63" s="260"/>
+      <c r="A63" s="201"/>
+      <c r="B63" s="327"/>
+      <c r="C63" s="329"/>
+      <c r="D63" s="189"/>
       <c r="E63" s="116">
         <v>1</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="263"/>
+      <c r="G63" s="192"/>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
@@ -6659,7 +6644,7 @@
       <c r="L63" s="35"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
-      <c r="O63" s="216"/>
+      <c r="O63" s="353"/>
       <c r="P63" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6695,17 +6680,17 @@
       <c r="AS63" s="3"/>
     </row>
     <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="327"/>
-      <c r="B64" s="189"/>
-      <c r="C64" s="191"/>
-      <c r="D64" s="260"/>
+      <c r="A64" s="201"/>
+      <c r="B64" s="327"/>
+      <c r="C64" s="329"/>
+      <c r="D64" s="189"/>
       <c r="E64" s="116">
         <v>2</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="263"/>
+      <c r="G64" s="192"/>
       <c r="H64" s="35"/>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
@@ -6715,7 +6700,7 @@
       <c r="L64" s="35"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
-      <c r="O64" s="216"/>
+      <c r="O64" s="353"/>
       <c r="P64" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6751,17 +6736,17 @@
       <c r="AS64" s="3"/>
     </row>
     <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="327"/>
-      <c r="B65" s="189"/>
-      <c r="C65" s="191"/>
-      <c r="D65" s="260"/>
+      <c r="A65" s="201"/>
+      <c r="B65" s="327"/>
+      <c r="C65" s="329"/>
+      <c r="D65" s="189"/>
       <c r="E65" s="116">
         <v>3</v>
       </c>
       <c r="F65" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G65" s="263"/>
+      <c r="G65" s="192"/>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
       <c r="J65" s="35"/>
@@ -6773,7 +6758,7 @@
       </c>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
-      <c r="O65" s="216"/>
+      <c r="O65" s="353"/>
       <c r="P65" s="9">
         <f t="shared" si="4"/>
         <v>168</v>
@@ -6809,13 +6794,13 @@
       <c r="AS65" s="3"/>
     </row>
     <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="327"/>
-      <c r="B66" s="189"/>
-      <c r="C66" s="191"/>
-      <c r="D66" s="301"/>
-      <c r="E66" s="302"/>
-      <c r="F66" s="302"/>
-      <c r="G66" s="302"/>
+      <c r="A66" s="201"/>
+      <c r="B66" s="327"/>
+      <c r="C66" s="329"/>
+      <c r="D66" s="263"/>
+      <c r="E66" s="264"/>
+      <c r="F66" s="264"/>
+      <c r="G66" s="264"/>
       <c r="H66" s="152">
         <f>SUM(H62:H65)</f>
         <v>0</v>
@@ -6877,17 +6862,17 @@
       <c r="AS66" s="2"/>
     </row>
     <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="327"/>
-      <c r="B67" s="189"/>
-      <c r="C67" s="191"/>
-      <c r="D67" s="291" t="s">
+      <c r="A67" s="201"/>
+      <c r="B67" s="327"/>
+      <c r="C67" s="329"/>
+      <c r="D67" s="251" t="s">
         <v>49</v>
       </c>
       <c r="E67" s="134"/>
       <c r="F67" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="295">
+      <c r="G67" s="255">
         <v>384</v>
       </c>
       <c r="H67" s="128">
@@ -6899,7 +6884,7 @@
       <c r="L67" s="128"/>
       <c r="M67" s="128"/>
       <c r="N67" s="128"/>
-      <c r="O67" s="217">
+      <c r="O67" s="354">
         <f>SUM(P67:P72)</f>
         <v>384</v>
       </c>
@@ -6937,8 +6922,8 @@
         <f>AG67/O67</f>
         <v>1</v>
       </c>
-      <c r="AI67" s="3" t="s">
-        <v>122</v>
+      <c r="AI67" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
@@ -6952,15 +6937,15 @@
       <c r="AS67" s="3"/>
     </row>
     <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="327"/>
-      <c r="B68" s="189"/>
-      <c r="C68" s="191"/>
-      <c r="D68" s="292"/>
+      <c r="A68" s="201"/>
+      <c r="B68" s="327"/>
+      <c r="C68" s="329"/>
+      <c r="D68" s="252"/>
       <c r="E68" s="133"/>
       <c r="F68" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="296"/>
+      <c r="G68" s="256"/>
       <c r="H68" s="130"/>
       <c r="I68" s="130">
         <v>72</v>
@@ -6970,7 +6955,7 @@
       <c r="L68" s="130"/>
       <c r="M68" s="130"/>
       <c r="N68" s="130"/>
-      <c r="O68" s="218"/>
+      <c r="O68" s="355"/>
       <c r="P68" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7006,15 +6991,15 @@
       <c r="AS68" s="3"/>
     </row>
     <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="327"/>
-      <c r="B69" s="189"/>
-      <c r="C69" s="191"/>
-      <c r="D69" s="292"/>
+      <c r="A69" s="201"/>
+      <c r="B69" s="327"/>
+      <c r="C69" s="329"/>
+      <c r="D69" s="252"/>
       <c r="E69" s="133"/>
       <c r="F69" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="296"/>
+      <c r="G69" s="256"/>
       <c r="H69" s="130"/>
       <c r="I69" s="130"/>
       <c r="J69" s="130">
@@ -7024,7 +7009,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="130"/>
       <c r="N69" s="130"/>
-      <c r="O69" s="218"/>
+      <c r="O69" s="355"/>
       <c r="P69" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7060,15 +7045,15 @@
       <c r="AS69" s="3"/>
     </row>
     <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="327"/>
-      <c r="B70" s="189"/>
-      <c r="C70" s="191"/>
-      <c r="D70" s="292"/>
+      <c r="A70" s="201"/>
+      <c r="B70" s="327"/>
+      <c r="C70" s="329"/>
+      <c r="D70" s="252"/>
       <c r="E70" s="133"/>
       <c r="F70" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="296"/>
+      <c r="G70" s="256"/>
       <c r="H70" s="130"/>
       <c r="I70" s="130"/>
       <c r="J70" s="130"/>
@@ -7078,7 +7063,7 @@
       <c r="L70" s="130"/>
       <c r="M70" s="130"/>
       <c r="N70" s="130"/>
-      <c r="O70" s="218"/>
+      <c r="O70" s="355"/>
       <c r="P70" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7114,15 +7099,15 @@
       <c r="AS70" s="3"/>
     </row>
     <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="327"/>
-      <c r="B71" s="189"/>
-      <c r="C71" s="191"/>
-      <c r="D71" s="292"/>
+      <c r="A71" s="201"/>
+      <c r="B71" s="327"/>
+      <c r="C71" s="329"/>
+      <c r="D71" s="252"/>
       <c r="E71" s="133"/>
       <c r="F71" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="296"/>
+      <c r="G71" s="256"/>
       <c r="H71" s="130"/>
       <c r="I71" s="130"/>
       <c r="J71" s="130"/>
@@ -7132,7 +7117,7 @@
       </c>
       <c r="M71" s="130"/>
       <c r="N71" s="130"/>
-      <c r="O71" s="218"/>
+      <c r="O71" s="355"/>
       <c r="P71" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7168,15 +7153,15 @@
       <c r="AS71" s="3"/>
     </row>
     <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="327"/>
-      <c r="B72" s="189"/>
-      <c r="C72" s="191"/>
-      <c r="D72" s="292"/>
+      <c r="A72" s="201"/>
+      <c r="B72" s="327"/>
+      <c r="C72" s="329"/>
+      <c r="D72" s="252"/>
       <c r="E72" s="133"/>
       <c r="F72" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="296"/>
+      <c r="G72" s="256"/>
       <c r="H72" s="130"/>
       <c r="I72" s="130"/>
       <c r="J72" s="130"/>
@@ -7186,7 +7171,7 @@
         <v>24</v>
       </c>
       <c r="N72" s="130"/>
-      <c r="O72" s="218"/>
+      <c r="O72" s="355"/>
       <c r="P72" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7222,13 +7207,13 @@
       <c r="AS72" s="3"/>
     </row>
     <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="327"/>
-      <c r="B73" s="189"/>
-      <c r="C73" s="191"/>
-      <c r="D73" s="221"/>
-      <c r="E73" s="222"/>
-      <c r="F73" s="222"/>
-      <c r="G73" s="222"/>
+      <c r="A73" s="201"/>
+      <c r="B73" s="327"/>
+      <c r="C73" s="329"/>
+      <c r="D73" s="305"/>
+      <c r="E73" s="306"/>
+      <c r="F73" s="306"/>
+      <c r="G73" s="306"/>
       <c r="H73" s="135">
         <f>SUM(H67:H72)</f>
         <v>72</v>
@@ -7290,17 +7275,17 @@
       <c r="AS73" s="2"/>
     </row>
     <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="327"/>
-      <c r="B74" s="189"/>
-      <c r="C74" s="191"/>
-      <c r="D74" s="241" t="s">
+      <c r="A74" s="201"/>
+      <c r="B74" s="327"/>
+      <c r="C74" s="329"/>
+      <c r="D74" s="325" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="146"/>
       <c r="F74" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="231">
+      <c r="G74" s="315">
         <v>48</v>
       </c>
       <c r="H74" s="148"/>
@@ -7312,7 +7297,7 @@
       <c r="N74" s="148">
         <v>12</v>
       </c>
-      <c r="O74" s="209">
+      <c r="O74" s="346">
         <f>SUM(P74:P77)</f>
         <v>48</v>
       </c>
@@ -7350,8 +7335,8 @@
         <f>AG74/O74</f>
         <v>1</v>
       </c>
-      <c r="AI74" s="3" t="s">
-        <v>116</v>
+      <c r="AI74" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
@@ -7365,15 +7350,15 @@
       <c r="AS74" s="3"/>
     </row>
     <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="327"/>
-      <c r="B75" s="189"/>
-      <c r="C75" s="191"/>
-      <c r="D75" s="242"/>
+      <c r="A75" s="201"/>
+      <c r="B75" s="327"/>
+      <c r="C75" s="329"/>
+      <c r="D75" s="258"/>
       <c r="E75" s="145"/>
       <c r="F75" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="231"/>
+      <c r="G75" s="315"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117"/>
       <c r="J75" s="117"/>
@@ -7383,7 +7368,7 @@
       <c r="N75" s="117">
         <v>12</v>
       </c>
-      <c r="O75" s="209"/>
+      <c r="O75" s="346"/>
       <c r="P75" s="9">
         <f t="shared" ref="P75:P77" si="81">SUM(H75:N75)</f>
         <v>12</v>
@@ -7419,15 +7404,15 @@
       <c r="AS75" s="3"/>
     </row>
     <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="327"/>
-      <c r="B76" s="189"/>
-      <c r="C76" s="191"/>
-      <c r="D76" s="242"/>
+      <c r="A76" s="201"/>
+      <c r="B76" s="327"/>
+      <c r="C76" s="329"/>
+      <c r="D76" s="258"/>
       <c r="E76" s="145"/>
       <c r="F76" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="231"/>
+      <c r="G76" s="315"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117"/>
       <c r="J76" s="117"/>
@@ -7437,7 +7422,7 @@
       <c r="N76" s="117">
         <v>12</v>
       </c>
-      <c r="O76" s="209"/>
+      <c r="O76" s="346"/>
       <c r="P76" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7473,15 +7458,15 @@
       <c r="AS76" s="3"/>
     </row>
     <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="327"/>
-      <c r="B77" s="189"/>
-      <c r="C77" s="191"/>
-      <c r="D77" s="243"/>
+      <c r="A77" s="201"/>
+      <c r="B77" s="327"/>
+      <c r="C77" s="329"/>
+      <c r="D77" s="261"/>
       <c r="E77" s="145"/>
       <c r="F77" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G77" s="232"/>
+      <c r="G77" s="316"/>
       <c r="H77" s="118"/>
       <c r="I77" s="118"/>
       <c r="J77" s="118"/>
@@ -7491,7 +7476,7 @@
       <c r="N77" s="118">
         <v>12</v>
       </c>
-      <c r="O77" s="210"/>
+      <c r="O77" s="347"/>
       <c r="P77" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7527,13 +7512,13 @@
       <c r="AS77" s="3"/>
     </row>
     <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="327"/>
-      <c r="B78" s="189"/>
-      <c r="C78" s="191"/>
-      <c r="D78" s="223"/>
-      <c r="E78" s="224"/>
-      <c r="F78" s="225"/>
-      <c r="G78" s="226"/>
+      <c r="A78" s="201"/>
+      <c r="B78" s="327"/>
+      <c r="C78" s="329"/>
+      <c r="D78" s="307"/>
+      <c r="E78" s="308"/>
+      <c r="F78" s="309"/>
+      <c r="G78" s="310"/>
       <c r="H78" s="112">
         <f>SUM(H74:H77)</f>
         <v>0</v>
@@ -7595,17 +7580,17 @@
       <c r="AS78" s="2"/>
     </row>
     <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="327"/>
-      <c r="B79" s="189"/>
-      <c r="C79" s="191"/>
-      <c r="D79" s="239" t="s">
+      <c r="A79" s="201"/>
+      <c r="B79" s="327"/>
+      <c r="C79" s="329"/>
+      <c r="D79" s="323" t="s">
         <v>50</v>
       </c>
       <c r="E79" s="157"/>
       <c r="F79" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="G79" s="233">
+      <c r="G79" s="317">
         <v>48</v>
       </c>
       <c r="H79" s="159">
@@ -7617,7 +7602,7 @@
       <c r="L79" s="159"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
-      <c r="O79" s="213">
+      <c r="O79" s="350">
         <f>SUM(P79:P82)</f>
         <v>48</v>
       </c>
@@ -7649,8 +7634,8 @@
         <f>AG79/O79</f>
         <v>1</v>
       </c>
-      <c r="AI79" s="3" t="s">
-        <v>123</v>
+      <c r="AI79" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
@@ -7664,15 +7649,15 @@
       <c r="AS79" s="3"/>
     </row>
     <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="327"/>
-      <c r="B80" s="189"/>
-      <c r="C80" s="191"/>
-      <c r="D80" s="240"/>
+      <c r="A80" s="201"/>
+      <c r="B80" s="327"/>
+      <c r="C80" s="329"/>
+      <c r="D80" s="324"/>
       <c r="E80" s="154"/>
       <c r="F80" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G80" s="234"/>
+      <c r="G80" s="318"/>
       <c r="H80" s="156">
         <v>12</v>
       </c>
@@ -7682,7 +7667,7 @@
       <c r="L80" s="156"/>
       <c r="M80" s="156"/>
       <c r="N80" s="156"/>
-      <c r="O80" s="214"/>
+      <c r="O80" s="351"/>
       <c r="P80" s="9">
         <f t="shared" ref="P80:P82" si="83">SUM(H80:N80)</f>
         <v>12</v>
@@ -7718,15 +7703,15 @@
       <c r="AS80" s="3"/>
     </row>
     <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="327"/>
-      <c r="B81" s="189"/>
-      <c r="C81" s="191"/>
-      <c r="D81" s="240"/>
+      <c r="A81" s="201"/>
+      <c r="B81" s="327"/>
+      <c r="C81" s="329"/>
+      <c r="D81" s="324"/>
       <c r="E81" s="154"/>
       <c r="F81" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G81" s="234"/>
+      <c r="G81" s="318"/>
       <c r="H81" s="156">
         <v>12</v>
       </c>
@@ -7736,7 +7721,7 @@
       <c r="L81" s="156"/>
       <c r="M81" s="156"/>
       <c r="N81" s="156"/>
-      <c r="O81" s="214"/>
+      <c r="O81" s="351"/>
       <c r="P81" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7772,15 +7757,15 @@
       <c r="AS81" s="3"/>
     </row>
     <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="327"/>
-      <c r="B82" s="189"/>
-      <c r="C82" s="191"/>
-      <c r="D82" s="240"/>
+      <c r="A82" s="201"/>
+      <c r="B82" s="327"/>
+      <c r="C82" s="329"/>
+      <c r="D82" s="324"/>
       <c r="E82" s="154"/>
       <c r="F82" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="G82" s="234"/>
+      <c r="G82" s="318"/>
       <c r="H82" s="156">
         <v>12</v>
       </c>
@@ -7790,7 +7775,7 @@
       <c r="L82" s="156"/>
       <c r="M82" s="156"/>
       <c r="N82" s="156"/>
-      <c r="O82" s="214"/>
+      <c r="O82" s="351"/>
       <c r="P82" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7826,13 +7811,13 @@
       <c r="AS82" s="3"/>
     </row>
     <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="327"/>
-      <c r="B83" s="189"/>
-      <c r="C83" s="191"/>
-      <c r="D83" s="227"/>
-      <c r="E83" s="228"/>
-      <c r="F83" s="228"/>
-      <c r="G83" s="228"/>
+      <c r="A83" s="201"/>
+      <c r="B83" s="327"/>
+      <c r="C83" s="329"/>
+      <c r="D83" s="311"/>
+      <c r="E83" s="312"/>
+      <c r="F83" s="312"/>
+      <c r="G83" s="312"/>
       <c r="H83" s="160">
         <f>SUM(H79:H82)</f>
         <v>48</v>
@@ -7894,17 +7879,17 @@
       <c r="AS83" s="2"/>
     </row>
     <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="327"/>
-      <c r="B84" s="189"/>
-      <c r="C84" s="192"/>
-      <c r="D84" s="237" t="s">
+      <c r="A84" s="201"/>
+      <c r="B84" s="327"/>
+      <c r="C84" s="330"/>
+      <c r="D84" s="321" t="s">
         <v>51</v>
       </c>
       <c r="E84" s="125"/>
       <c r="F84" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="235">
+      <c r="G84" s="319">
         <v>48</v>
       </c>
       <c r="H84" s="126"/>
@@ -7916,7 +7901,7 @@
       <c r="L84" s="126"/>
       <c r="M84" s="126"/>
       <c r="N84" s="126"/>
-      <c r="O84" s="211">
+      <c r="O84" s="348">
         <f>SUM(P84:P87)</f>
         <v>48</v>
       </c>
@@ -7948,8 +7933,8 @@
         <f>AG84/O84</f>
         <v>1</v>
       </c>
-      <c r="AI84" s="3" t="s">
-        <v>124</v>
+      <c r="AI84" s="356" t="s">
+        <v>112</v>
       </c>
       <c r="AJ84" s="3"/>
       <c r="AK84" s="3"/>
@@ -7963,15 +7948,15 @@
       <c r="AS84" s="3"/>
     </row>
     <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="327"/>
-      <c r="B85" s="189"/>
-      <c r="C85" s="192"/>
-      <c r="D85" s="238"/>
+      <c r="A85" s="201"/>
+      <c r="B85" s="327"/>
+      <c r="C85" s="330"/>
+      <c r="D85" s="322"/>
       <c r="E85" s="123"/>
       <c r="F85" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="G85" s="236"/>
+      <c r="G85" s="320"/>
       <c r="H85" s="124"/>
       <c r="I85" s="124">
         <v>12</v>
@@ -7981,7 +7966,7 @@
       <c r="L85" s="124"/>
       <c r="M85" s="124"/>
       <c r="N85" s="124"/>
-      <c r="O85" s="212"/>
+      <c r="O85" s="349"/>
       <c r="P85" s="9">
         <f t="shared" ref="P85:P87" si="90">SUM(H85:N85)</f>
         <v>12</v>
@@ -8002,7 +7987,7 @@
       <c r="AD85" s="3"/>
       <c r="AE85" s="3"/>
       <c r="AF85" s="3"/>
-      <c r="AG85" s="3"/>
+      <c r="AG85" s="358"/>
       <c r="AH85" s="3"/>
       <c r="AI85" s="3"/>
       <c r="AJ85" s="3"/>
@@ -8017,15 +8002,15 @@
       <c r="AS85" s="3"/>
     </row>
     <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="327"/>
-      <c r="B86" s="189"/>
-      <c r="C86" s="192"/>
-      <c r="D86" s="238"/>
+      <c r="A86" s="201"/>
+      <c r="B86" s="327"/>
+      <c r="C86" s="330"/>
+      <c r="D86" s="322"/>
       <c r="E86" s="123"/>
       <c r="F86" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="236"/>
+      <c r="G86" s="320"/>
       <c r="H86" s="124"/>
       <c r="I86" s="124">
         <v>12</v>
@@ -8035,7 +8020,7 @@
       <c r="L86" s="124"/>
       <c r="M86" s="124"/>
       <c r="N86" s="124"/>
-      <c r="O86" s="212"/>
+      <c r="O86" s="349"/>
       <c r="P86" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8071,15 +8056,15 @@
       <c r="AS86" s="3"/>
     </row>
     <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="328"/>
-      <c r="B87" s="189"/>
-      <c r="C87" s="192"/>
-      <c r="D87" s="238"/>
+      <c r="A87" s="202"/>
+      <c r="B87" s="327"/>
+      <c r="C87" s="330"/>
+      <c r="D87" s="322"/>
       <c r="E87" s="123"/>
       <c r="F87" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="236"/>
+      <c r="G87" s="320"/>
       <c r="H87" s="124"/>
       <c r="I87" s="124">
         <v>12</v>
@@ -8089,7 +8074,7 @@
       <c r="L87" s="124"/>
       <c r="M87" s="124"/>
       <c r="N87" s="124"/>
-      <c r="O87" s="212"/>
+      <c r="O87" s="349"/>
       <c r="P87" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8126,12 +8111,12 @@
     </row>
     <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
-      <c r="B88" s="189"/>
-      <c r="C88" s="192"/>
-      <c r="D88" s="229"/>
-      <c r="E88" s="230"/>
-      <c r="F88" s="230"/>
-      <c r="G88" s="230"/>
+      <c r="B88" s="327"/>
+      <c r="C88" s="330"/>
+      <c r="D88" s="313"/>
+      <c r="E88" s="314"/>
+      <c r="F88" s="314"/>
+      <c r="G88" s="314"/>
       <c r="H88" s="162">
         <f>SUM(H84:H87)</f>
         <v>0</v>
@@ -8194,8 +8179,8 @@
     </row>
     <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
-      <c r="B89" s="189"/>
-      <c r="C89" s="192"/>
+      <c r="B89" s="327"/>
+      <c r="C89" s="330"/>
       <c r="D89" s="122" t="s">
         <v>17</v>
       </c>
@@ -8247,7 +8232,7 @@
         <f>AG89/O89</f>
         <v>1</v>
       </c>
-      <c r="AI89" s="3" t="s">
+      <c r="AI89" s="356" t="s">
         <v>112</v>
       </c>
       <c r="AJ89" s="3"/>
@@ -8263,12 +8248,12 @@
     </row>
     <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
-      <c r="B90" s="189"/>
-      <c r="C90" s="192"/>
-      <c r="D90" s="219"/>
-      <c r="E90" s="220"/>
-      <c r="F90" s="220"/>
-      <c r="G90" s="220"/>
+      <c r="B90" s="327"/>
+      <c r="C90" s="330"/>
+      <c r="D90" s="196"/>
+      <c r="E90" s="304"/>
+      <c r="F90" s="304"/>
+      <c r="G90" s="304"/>
       <c r="H90" s="140">
         <f t="shared" ref="H90:N90" si="97">SUM(H89:H89)</f>
         <v>48</v>
@@ -8393,33 +8378,93 @@
         <f t="shared" si="99"/>
         <v>-48</v>
       </c>
+      <c r="AI93" s="357"/>
     </row>
     <row r="97" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H97" s="193" t="s">
+      <c r="H97" s="303" t="s">
         <v>104</v>
       </c>
-      <c r="I97" s="193"/>
-      <c r="J97" s="193"/>
+      <c r="I97" s="303"/>
+      <c r="J97" s="303"/>
     </row>
     <row r="99" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="I99" s="193" t="s">
+      <c r="I99" s="303" t="s">
         <v>105</v>
       </c>
-      <c r="J99" s="193"/>
-      <c r="K99" s="193"/>
-      <c r="L99" s="193"/>
+      <c r="J99" s="303"/>
+      <c r="K99" s="303"/>
+      <c r="L99" s="303"/>
     </row>
     <row r="101" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="K101" s="193" t="s">
+      <c r="K101" s="303" t="s">
         <v>106</v>
       </c>
-      <c r="L101" s="193"/>
-      <c r="M101" s="193"/>
-      <c r="N101" s="193"/>
+      <c r="L101" s="303"/>
+      <c r="M101" s="303"/>
+      <c r="N101" s="303"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS91" xr:uid="{44B9DB88-0080-4900-9B58-5C638DC6AAB3}"/>
   <mergeCells count="75">
+    <mergeCell ref="O74:O77"/>
+    <mergeCell ref="O84:O87"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="O67:O72"/>
+    <mergeCell ref="B2:B90"/>
+    <mergeCell ref="C2:C90"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="O32:O35"/>
+    <mergeCell ref="O37:O40"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O52:O55"/>
+    <mergeCell ref="O57:O60"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="G12:G15"/>
     <mergeCell ref="D17:D20"/>
@@ -8436,65 +8481,6 @@
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="G37:G40"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O52:O55"/>
-    <mergeCell ref="O57:O60"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="O32:O35"/>
-    <mergeCell ref="O37:O40"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="K101:N101"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="B2:B90"/>
-    <mergeCell ref="C2:C90"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="O74:O77"/>
-    <mergeCell ref="O84:O87"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="O67:O72"/>
   </mergeCells>
   <conditionalFormatting sqref="H93:N93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Cambio en front - end de div
</commit_message>
<xml_diff>
--- a/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
+++ b/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Desktop\PROYECTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1234\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37981CEF-84DD-4AB1-9DAB-A0813A16FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8EB1A3-61D5-4E01-8979-F67FC9E6B9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
   <si>
     <t>DENOMINACION</t>
   </si>
@@ -376,14 +376,50 @@
     <t>INSTRUCTOR</t>
   </si>
   <si>
-    <t>MARRUGO LEYVA  WILLIAM</t>
+    <t>LUIS F GARCIA</t>
+  </si>
+  <si>
+    <t>BEATRIZ ALFARO</t>
+  </si>
+  <si>
+    <t>ANEDIA GONZALEZ</t>
+  </si>
+  <si>
+    <t>DAVID ARRIETA</t>
+  </si>
+  <si>
+    <t>FERNANDO FLOREZ</t>
+  </si>
+  <si>
+    <t>PILAR PRADA</t>
+  </si>
+  <si>
+    <t>LUIS PEREZ</t>
+  </si>
+  <si>
+    <t>YOVANNI URREGO</t>
+  </si>
+  <si>
+    <t>OSMEIDA RAMIREZ</t>
+  </si>
+  <si>
+    <t>ANDRES MARQUEZ</t>
+  </si>
+  <si>
+    <t>LUZ E CARRIAZO</t>
+  </si>
+  <si>
+    <t>JORGE VASQUEZ</t>
+  </si>
+  <si>
+    <t>ENADITH HERNANDEZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,20 +501,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -588,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1192,12 +1214,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="362">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1755,357 +1801,102 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2172,103 +1963,367 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2618,27 +2673,27 @@
   <dimension ref="A1:AS101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="AJ87" sqref="AJ87"/>
+      <selection pane="bottomRight" activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="31" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1"/>
+    <col min="7" max="15" width="11.44140625" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="31" width="11.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2742,17 +2797,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="200" t="s">
+    <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="325" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="326">
+      <c r="B2" s="197">
         <v>228183</v>
       </c>
-      <c r="C2" s="328">
+      <c r="C2" s="199">
         <v>2</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="D2" s="328" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
@@ -2761,7 +2816,7 @@
       <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="206">
+      <c r="G2" s="331">
         <v>528</v>
       </c>
       <c r="H2" s="12"/>
@@ -2773,7 +2828,7 @@
       <c r="N2" s="12">
         <v>72</v>
       </c>
-      <c r="O2" s="273">
+      <c r="O2" s="275">
         <f>SUM(P2:P5)</f>
         <v>528</v>
       </c>
@@ -2839,7 +2894,7 @@
         <f>AG2/O2</f>
         <v>1</v>
       </c>
-      <c r="AI2" s="356" t="s">
+      <c r="AI2" s="3" t="s">
         <v>112</v>
       </c>
       <c r="AJ2" s="2"/>
@@ -2853,18 +2908,18 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="201"/>
-      <c r="B3" s="327"/>
-      <c r="C3" s="329"/>
-      <c r="D3" s="204"/>
+    <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="326"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="329"/>
       <c r="E3" s="13">
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="207"/>
+      <c r="G3" s="332"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -2874,7 +2929,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="274"/>
+      <c r="O3" s="276"/>
       <c r="P3" s="9">
         <f>SUM(H3:N3)</f>
         <v>64</v>
@@ -2897,7 +2952,9 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
+      <c r="AI3" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
@@ -2909,18 +2966,18 @@
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201"/>
-      <c r="B4" s="327"/>
-      <c r="C4" s="329"/>
-      <c r="D4" s="204"/>
+    <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="326"/>
+      <c r="B4" s="198"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="329"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="207"/>
+      <c r="G4" s="332"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2930,7 +2987,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="274"/>
+      <c r="O4" s="276"/>
       <c r="P4" s="9">
         <f>SUM(H4:N4)</f>
         <v>80</v>
@@ -2953,7 +3010,9 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
+      <c r="AI4" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
@@ -2965,18 +3024,18 @@
       <c r="AR4" s="2"/>
       <c r="AS4" s="2"/>
     </row>
-    <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="201"/>
-      <c r="B5" s="327"/>
-      <c r="C5" s="329"/>
-      <c r="D5" s="205"/>
+    <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="326"/>
+      <c r="B5" s="198"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="330"/>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="208"/>
+      <c r="G5" s="333"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -2990,7 +3049,7 @@
       <c r="N5" s="18">
         <v>168</v>
       </c>
-      <c r="O5" s="275"/>
+      <c r="O5" s="277"/>
       <c r="P5" s="9">
         <f>SUM(H5:N5)</f>
         <v>312</v>
@@ -3013,7 +3072,9 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
+      <c r="AI5" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
@@ -3025,14 +3086,14 @@
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
     </row>
-    <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="201"/>
-      <c r="B6" s="327"/>
-      <c r="C6" s="329"/>
-      <c r="D6" s="331"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="332"/>
-      <c r="G6" s="333"/>
+    <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="326"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="200"/>
+      <c r="D6" s="203"/>
+      <c r="E6" s="204"/>
+      <c r="F6" s="204"/>
+      <c r="G6" s="205"/>
       <c r="H6" s="56">
         <f>SUM(H2:H5)</f>
         <v>0</v>
@@ -3093,11 +3154,11 @@
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
     </row>
-    <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="201"/>
-      <c r="B7" s="327"/>
-      <c r="C7" s="329"/>
-      <c r="D7" s="215" t="s">
+    <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="326"/>
+      <c r="B7" s="198"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="334" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="19">
@@ -3106,7 +3167,7 @@
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="218">
+      <c r="G7" s="337">
         <v>384</v>
       </c>
       <c r="H7" s="25"/>
@@ -3118,7 +3179,7 @@
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="276">
+      <c r="O7" s="278">
         <f>SUM(P7:P10)</f>
         <v>384</v>
       </c>
@@ -3184,8 +3245,8 @@
         <f>AG7/O7</f>
         <v>1</v>
       </c>
-      <c r="AI7" s="356" t="s">
-        <v>112</v>
+      <c r="AI7" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
@@ -3198,18 +3259,18 @@
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
     </row>
-    <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="201"/>
-      <c r="B8" s="327"/>
-      <c r="C8" s="329"/>
-      <c r="D8" s="216"/>
+    <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="326"/>
+      <c r="B8" s="198"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="335"/>
       <c r="E8" s="21">
         <v>3</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="219"/>
+      <c r="G8" s="338"/>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
@@ -3219,7 +3280,7 @@
         <v>144</v>
       </c>
       <c r="N8" s="26"/>
-      <c r="O8" s="277"/>
+      <c r="O8" s="279"/>
       <c r="P8" s="9">
         <f t="shared" ref="P8:P10" si="1">SUM(H8:N8)</f>
         <v>144</v>
@@ -3242,7 +3303,9 @@
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
+      <c r="AI8" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
@@ -3254,18 +3317,18 @@
       <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
     </row>
-    <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="201"/>
-      <c r="B9" s="327"/>
-      <c r="C9" s="329"/>
-      <c r="D9" s="216"/>
+    <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="326"/>
+      <c r="B9" s="198"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="335"/>
       <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="219"/>
+      <c r="G9" s="338"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -3275,7 +3338,7 @@
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="277"/>
+      <c r="O9" s="279"/>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3298,7 +3361,9 @@
       <c r="AF9" s="3"/>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
+      <c r="AI9" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
@@ -3310,18 +3375,18 @@
       <c r="AR9" s="3"/>
       <c r="AS9" s="3"/>
     </row>
-    <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
-      <c r="B10" s="327"/>
-      <c r="C10" s="329"/>
-      <c r="D10" s="217"/>
+    <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="326"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="336"/>
       <c r="E10" s="23">
         <v>4</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="220"/>
+      <c r="G10" s="339"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -3331,7 +3396,7 @@
       <c r="N10" s="27">
         <v>96</v>
       </c>
-      <c r="O10" s="278"/>
+      <c r="O10" s="280"/>
       <c r="P10" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3354,7 +3419,9 @@
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
+      <c r="AI10" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
@@ -3366,14 +3433,14 @@
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
     </row>
-    <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
-      <c r="B11" s="327"/>
-      <c r="C11" s="329"/>
-      <c r="D11" s="334"/>
-      <c r="E11" s="335"/>
-      <c r="F11" s="335"/>
-      <c r="G11" s="336"/>
+    <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="326"/>
+      <c r="B11" s="198"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="206"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="207"/>
+      <c r="G11" s="208"/>
       <c r="H11" s="61">
         <f>SUM(H7:H10)</f>
         <v>0</v>
@@ -3419,9 +3486,9 @@
       <c r="AC11" s="180"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
+      <c r="AF11" s="120"/>
+      <c r="AG11" s="120"/>
+      <c r="AH11" s="120"/>
       <c r="AI11" s="120"/>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
@@ -3434,18 +3501,18 @@
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
     </row>
-    <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="201"/>
-      <c r="B12" s="327"/>
-      <c r="C12" s="329"/>
-      <c r="D12" s="188" t="s">
+    <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="326"/>
+      <c r="B12" s="198"/>
+      <c r="C12" s="200"/>
+      <c r="D12" s="258" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="191">
+      <c r="G12" s="261">
         <v>48</v>
       </c>
       <c r="H12" s="34">
@@ -3457,7 +3524,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="279">
+      <c r="O12" s="255">
         <f t="shared" ref="O12" si="3">SUM(P12:P15)</f>
         <v>48</v>
       </c>
@@ -3506,32 +3573,33 @@
         <f>O12-AC12</f>
         <v>48</v>
       </c>
-      <c r="AE12" s="175">
+      <c r="AE12" s="360">
         <f>AD12/O12</f>
         <v>1</v>
       </c>
-      <c r="AG12" s="184">
+      <c r="AF12" s="179"/>
+      <c r="AG12" s="355">
         <f>O12-AF12</f>
         <v>48</v>
       </c>
-      <c r="AH12" s="187">
+      <c r="AH12" s="356">
         <f>AG12/O12</f>
         <v>1</v>
       </c>
-      <c r="AI12" s="356" t="s">
+      <c r="AI12" s="357" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="201"/>
-      <c r="B13" s="327"/>
-      <c r="C13" s="329"/>
-      <c r="D13" s="189"/>
+    <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="326"/>
+      <c r="B13" s="198"/>
+      <c r="C13" s="200"/>
+      <c r="D13" s="259"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="192"/>
+      <c r="G13" s="262"/>
       <c r="H13" s="35">
         <v>12</v>
       </c>
@@ -3541,7 +3609,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="280"/>
+      <c r="O13" s="256"/>
       <c r="P13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3560,19 +3628,24 @@
       <c r="AB13" s="178"/>
       <c r="AC13" s="179"/>
       <c r="AD13" s="179"/>
-      <c r="AE13" s="179"/>
-      <c r="AI13" s="179"/>
-    </row>
-    <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="201"/>
-      <c r="B14" s="327"/>
-      <c r="C14" s="329"/>
-      <c r="D14" s="189"/>
+      <c r="AE13" s="361"/>
+      <c r="AF13" s="179"/>
+      <c r="AG13" s="179"/>
+      <c r="AH13" s="179"/>
+      <c r="AI13" s="357" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="326"/>
+      <c r="B14" s="198"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="259"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="192"/>
+      <c r="G14" s="262"/>
       <c r="H14" s="35">
         <v>12</v>
       </c>
@@ -3582,7 +3655,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="280"/>
+      <c r="O14" s="256"/>
       <c r="P14" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3601,19 +3674,24 @@
       <c r="AB14" s="178"/>
       <c r="AC14" s="179"/>
       <c r="AD14" s="179"/>
-      <c r="AE14" s="179"/>
-      <c r="AI14" s="179"/>
-    </row>
-    <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201"/>
-      <c r="B15" s="327"/>
-      <c r="C15" s="329"/>
-      <c r="D15" s="190"/>
+      <c r="AE14" s="361"/>
+      <c r="AF14" s="179"/>
+      <c r="AG14" s="179"/>
+      <c r="AH14" s="179"/>
+      <c r="AI14" s="357" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="326"/>
+      <c r="B15" s="198"/>
+      <c r="C15" s="200"/>
+      <c r="D15" s="260"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="193"/>
+      <c r="G15" s="263"/>
       <c r="H15" s="36">
         <v>12</v>
       </c>
@@ -3623,7 +3701,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="281"/>
+      <c r="O15" s="257"/>
       <c r="P15" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3642,17 +3720,22 @@
       <c r="AB15" s="178"/>
       <c r="AC15" s="179"/>
       <c r="AD15" s="179"/>
-      <c r="AE15" s="179"/>
-      <c r="AI15" s="179"/>
-    </row>
-    <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
-      <c r="B16" s="327"/>
-      <c r="C16" s="329"/>
-      <c r="D16" s="331"/>
-      <c r="E16" s="332"/>
-      <c r="F16" s="332"/>
-      <c r="G16" s="333"/>
+      <c r="AE15" s="361"/>
+      <c r="AF15" s="179"/>
+      <c r="AG15" s="179"/>
+      <c r="AH15" s="179"/>
+      <c r="AI15" s="357" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="326"/>
+      <c r="B16" s="198"/>
+      <c r="C16" s="200"/>
+      <c r="D16" s="203"/>
+      <c r="E16" s="204"/>
+      <c r="F16" s="204"/>
+      <c r="G16" s="205"/>
       <c r="H16" s="56">
         <f>SUM(H12:H15)</f>
         <v>48</v>
@@ -3698,9 +3781,9 @@
       <c r="AC16" s="182"/>
       <c r="AD16" s="168"/>
       <c r="AE16" s="168"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
+      <c r="AF16" s="168"/>
+      <c r="AG16" s="168"/>
+      <c r="AH16" s="168"/>
       <c r="AI16" s="168"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
@@ -3713,18 +3796,18 @@
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
     </row>
-    <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="201"/>
-      <c r="B17" s="327"/>
-      <c r="C17" s="329"/>
-      <c r="D17" s="194" t="s">
+    <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="326"/>
+      <c r="B17" s="198"/>
+      <c r="C17" s="200"/>
+      <c r="D17" s="320" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="197">
+      <c r="G17" s="322">
         <v>48</v>
       </c>
       <c r="H17" s="44"/>
@@ -3736,7 +3819,7 @@
       <c r="L17" s="44"/>
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
-      <c r="O17" s="282">
+      <c r="O17" s="281">
         <f t="shared" ref="O17" si="6">SUM(P17:P20)</f>
         <v>48</v>
       </c>
@@ -3798,8 +3881,8 @@
         <f>AG17/O17</f>
         <v>1</v>
       </c>
-      <c r="AI17" s="356" t="s">
-        <v>112</v>
+      <c r="AI17" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
@@ -3812,16 +3895,16 @@
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
     </row>
-    <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="201"/>
-      <c r="B18" s="327"/>
-      <c r="C18" s="329"/>
-      <c r="D18" s="195"/>
+    <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="326"/>
+      <c r="B18" s="198"/>
+      <c r="C18" s="200"/>
+      <c r="D18" s="321"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="198"/>
+      <c r="G18" s="323"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45">
         <v>12</v>
@@ -3831,7 +3914,7 @@
       <c r="L18" s="45"/>
       <c r="M18" s="45"/>
       <c r="N18" s="45"/>
-      <c r="O18" s="283"/>
+      <c r="O18" s="282"/>
       <c r="P18" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3854,7 +3937,9 @@
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
+      <c r="AI18" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
       <c r="AL18" s="3"/>
@@ -3866,16 +3951,16 @@
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
     </row>
-    <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="201"/>
-      <c r="B19" s="327"/>
-      <c r="C19" s="329"/>
-      <c r="D19" s="195"/>
+    <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="326"/>
+      <c r="B19" s="198"/>
+      <c r="C19" s="200"/>
+      <c r="D19" s="321"/>
       <c r="E19" s="39"/>
       <c r="F19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="198"/>
+      <c r="G19" s="323"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45">
         <v>12</v>
@@ -3885,7 +3970,7 @@
       <c r="L19" s="45"/>
       <c r="M19" s="45"/>
       <c r="N19" s="45"/>
-      <c r="O19" s="283"/>
+      <c r="O19" s="282"/>
       <c r="P19" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3908,7 +3993,9 @@
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
+      <c r="AI19" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
       <c r="AL19" s="3"/>
@@ -3920,16 +4007,16 @@
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
     </row>
-    <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="201"/>
-      <c r="B20" s="327"/>
-      <c r="C20" s="329"/>
-      <c r="D20" s="196"/>
+    <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="326"/>
+      <c r="B20" s="198"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="218"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="199"/>
+      <c r="G20" s="324"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46">
         <v>12</v>
@@ -3939,7 +4026,7 @@
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
       <c r="N20" s="46"/>
-      <c r="O20" s="284"/>
+      <c r="O20" s="283"/>
       <c r="P20" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3962,7 +4049,9 @@
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
+      <c r="AI20" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
       <c r="AL20" s="3"/>
@@ -3974,14 +4063,14 @@
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
     </row>
-    <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="201"/>
-      <c r="B21" s="327"/>
-      <c r="C21" s="329"/>
-      <c r="D21" s="337"/>
-      <c r="E21" s="338"/>
-      <c r="F21" s="338"/>
-      <c r="G21" s="339"/>
+    <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="326"/>
+      <c r="B21" s="198"/>
+      <c r="C21" s="200"/>
+      <c r="D21" s="209"/>
+      <c r="E21" s="210"/>
+      <c r="F21" s="210"/>
+      <c r="G21" s="211"/>
       <c r="H21" s="62">
         <f>SUM(H17:H20)</f>
         <v>0</v>
@@ -4042,11 +4131,11 @@
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
     </row>
-    <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="201"/>
-      <c r="B22" s="327"/>
-      <c r="C22" s="329"/>
-      <c r="D22" s="209" t="s">
+    <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="326"/>
+      <c r="B22" s="198"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="317" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="47">
@@ -4055,7 +4144,7 @@
       <c r="F22" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="212">
+      <c r="G22" s="305">
         <v>336</v>
       </c>
       <c r="H22" s="53"/>
@@ -4065,7 +4154,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="53"/>
       <c r="N22" s="53"/>
-      <c r="O22" s="268">
+      <c r="O22" s="270">
         <f t="shared" ref="O22" si="13">SUM(P22:P25)</f>
         <v>336</v>
       </c>
@@ -4137,8 +4226,8 @@
         <f>AG22/O22</f>
         <v>1</v>
       </c>
-      <c r="AI22" s="356" t="s">
-        <v>112</v>
+      <c r="AI22" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
@@ -4151,18 +4240,18 @@
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
     </row>
-    <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="201"/>
-      <c r="B23" s="327"/>
-      <c r="C23" s="329"/>
-      <c r="D23" s="210"/>
+    <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="326"/>
+      <c r="B23" s="198"/>
+      <c r="C23" s="200"/>
+      <c r="D23" s="318"/>
       <c r="E23" s="49">
         <v>2</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="213"/>
+      <c r="G23" s="306"/>
       <c r="H23" s="54">
         <v>72</v>
       </c>
@@ -4172,7 +4261,7 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="269"/>
+      <c r="O23" s="271"/>
       <c r="P23" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4195,7 +4284,9 @@
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
+      <c r="AI23" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
@@ -4207,18 +4298,18 @@
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
     </row>
-    <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="201"/>
-      <c r="B24" s="327"/>
-      <c r="C24" s="329"/>
-      <c r="D24" s="210"/>
+    <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="326"/>
+      <c r="B24" s="198"/>
+      <c r="C24" s="200"/>
+      <c r="D24" s="318"/>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="213"/>
+      <c r="G24" s="306"/>
       <c r="H24" s="54">
         <v>72</v>
       </c>
@@ -4228,7 +4319,7 @@
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
-      <c r="O24" s="269"/>
+      <c r="O24" s="271"/>
       <c r="P24" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4251,7 +4342,9 @@
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
-      <c r="AI24" s="3"/>
+      <c r="AI24" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
       <c r="AL24" s="3"/>
@@ -4263,18 +4356,18 @@
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
     </row>
-    <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="201"/>
-      <c r="B25" s="327"/>
-      <c r="C25" s="329"/>
-      <c r="D25" s="211"/>
+    <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="326"/>
+      <c r="B25" s="198"/>
+      <c r="C25" s="200"/>
+      <c r="D25" s="319"/>
       <c r="E25" s="51">
         <v>3</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="214"/>
+      <c r="G25" s="307"/>
       <c r="H25" s="55"/>
       <c r="I25" s="55">
         <v>72</v>
@@ -4286,7 +4379,7 @@
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
-      <c r="O25" s="270"/>
+      <c r="O25" s="272"/>
       <c r="P25" s="9">
         <f t="shared" si="4"/>
         <v>192</v>
@@ -4309,7 +4402,9 @@
       <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
-      <c r="AI25" s="3"/>
+      <c r="AI25" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
@@ -4321,14 +4416,14 @@
       <c r="AR25" s="3"/>
       <c r="AS25" s="3"/>
     </row>
-    <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="201"/>
-      <c r="B26" s="327"/>
-      <c r="C26" s="329"/>
-      <c r="D26" s="340"/>
-      <c r="E26" s="341"/>
-      <c r="F26" s="341"/>
-      <c r="G26" s="342"/>
+    <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="326"/>
+      <c r="B26" s="198"/>
+      <c r="C26" s="200"/>
+      <c r="D26" s="212"/>
+      <c r="E26" s="213"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="214"/>
       <c r="H26" s="64">
         <f>SUM(H22:H25)</f>
         <v>144</v>
@@ -4389,11 +4484,11 @@
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
     </row>
-    <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="201"/>
-      <c r="B27" s="327"/>
-      <c r="C27" s="329"/>
-      <c r="D27" s="233" t="s">
+    <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="326"/>
+      <c r="B27" s="198"/>
+      <c r="C27" s="200"/>
+      <c r="D27" s="352" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="65">
@@ -4402,7 +4497,7 @@
       <c r="F27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="221">
+      <c r="G27" s="340">
         <v>576</v>
       </c>
       <c r="H27" s="73"/>
@@ -4414,7 +4509,7 @@
         <v>72</v>
       </c>
       <c r="N27" s="73"/>
-      <c r="O27" s="285">
+      <c r="O27" s="284">
         <f t="shared" ref="O27" si="20">SUM(P27:P30)</f>
         <v>576</v>
       </c>
@@ -4486,7 +4581,7 @@
         <f>AG27/O27</f>
         <v>1</v>
       </c>
-      <c r="AI27" s="356" t="s">
+      <c r="AI27" s="3" t="s">
         <v>112</v>
       </c>
       <c r="AJ27" s="3"/>
@@ -4500,18 +4595,18 @@
       <c r="AR27" s="3"/>
       <c r="AS27" s="3"/>
     </row>
-    <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="201"/>
-      <c r="B28" s="327"/>
-      <c r="C28" s="329"/>
-      <c r="D28" s="234"/>
+    <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="326"/>
+      <c r="B28" s="198"/>
+      <c r="C28" s="200"/>
+      <c r="D28" s="353"/>
       <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="222"/>
+      <c r="G28" s="341"/>
       <c r="H28" s="74"/>
       <c r="I28" s="74">
         <v>72</v>
@@ -4521,7 +4616,7 @@
       <c r="L28" s="74"/>
       <c r="M28" s="74"/>
       <c r="N28" s="74"/>
-      <c r="O28" s="286"/>
+      <c r="O28" s="285"/>
       <c r="P28" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4544,7 +4639,9 @@
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
-      <c r="AI28" s="3"/>
+      <c r="AI28" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ28" s="3"/>
       <c r="AK28" s="3"/>
       <c r="AL28" s="3"/>
@@ -4556,18 +4653,18 @@
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
     </row>
-    <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="201"/>
-      <c r="B29" s="327"/>
-      <c r="C29" s="329"/>
-      <c r="D29" s="234"/>
+    <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="326"/>
+      <c r="B29" s="198"/>
+      <c r="C29" s="200"/>
+      <c r="D29" s="353"/>
       <c r="E29" s="67">
         <v>1</v>
       </c>
       <c r="F29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="222"/>
+      <c r="G29" s="341"/>
       <c r="H29" s="74">
         <v>72</v>
       </c>
@@ -4577,7 +4674,7 @@
       <c r="L29" s="74"/>
       <c r="M29" s="74"/>
       <c r="N29" s="74"/>
-      <c r="O29" s="286"/>
+      <c r="O29" s="285"/>
       <c r="P29" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4600,7 +4697,9 @@
       <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
-      <c r="AI29" s="3"/>
+      <c r="AI29" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
       <c r="AL29" s="3"/>
@@ -4612,18 +4711,18 @@
       <c r="AR29" s="3"/>
       <c r="AS29" s="3"/>
     </row>
-    <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="201"/>
-      <c r="B30" s="327"/>
-      <c r="C30" s="329"/>
-      <c r="D30" s="235"/>
+    <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="326"/>
+      <c r="B30" s="198"/>
+      <c r="C30" s="200"/>
+      <c r="D30" s="354"/>
       <c r="E30" s="69">
         <v>3</v>
       </c>
       <c r="F30" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="223"/>
+      <c r="G30" s="342"/>
       <c r="H30" s="75"/>
       <c r="I30" s="75">
         <v>72</v>
@@ -4639,7 +4738,7 @@
       </c>
       <c r="M30" s="75"/>
       <c r="N30" s="75"/>
-      <c r="O30" s="287"/>
+      <c r="O30" s="286"/>
       <c r="P30" s="9">
         <f t="shared" si="4"/>
         <v>360</v>
@@ -4662,7 +4761,9 @@
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
-      <c r="AI30" s="3"/>
+      <c r="AI30" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
@@ -4674,14 +4775,14 @@
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
     </row>
-    <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="201"/>
-      <c r="B31" s="327"/>
-      <c r="C31" s="329"/>
-      <c r="D31" s="343"/>
-      <c r="E31" s="344"/>
-      <c r="F31" s="344"/>
-      <c r="G31" s="345"/>
+    <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="326"/>
+      <c r="B31" s="198"/>
+      <c r="C31" s="200"/>
+      <c r="D31" s="215"/>
+      <c r="E31" s="216"/>
+      <c r="F31" s="216"/>
+      <c r="G31" s="217"/>
       <c r="H31" s="71">
         <f>SUM(H27:H30)</f>
         <v>72</v>
@@ -4727,10 +4828,10 @@
       <c r="AC31" s="180"/>
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
-      <c r="AF31" s="2"/>
-      <c r="AG31" s="2"/>
-      <c r="AH31" s="2"/>
-      <c r="AI31" s="2"/>
+      <c r="AF31" s="120"/>
+      <c r="AG31" s="120"/>
+      <c r="AH31" s="120"/>
+      <c r="AI31" s="120"/>
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="2"/>
@@ -4742,18 +4843,18 @@
       <c r="AR31" s="2"/>
       <c r="AS31" s="2"/>
     </row>
-    <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="201"/>
-      <c r="B32" s="327"/>
-      <c r="C32" s="329"/>
-      <c r="D32" s="300" t="s">
+    <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="326"/>
+      <c r="B32" s="198"/>
+      <c r="C32" s="200"/>
+      <c r="D32" s="264" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="224">
+      <c r="G32" s="343">
         <v>48</v>
       </c>
       <c r="H32" s="82"/>
@@ -4765,7 +4866,7 @@
         <v>12</v>
       </c>
       <c r="N32" s="82"/>
-      <c r="O32" s="294">
+      <c r="O32" s="249">
         <f t="shared" ref="O32" si="27">SUM(P32:P35)</f>
         <v>48</v>
       </c>
@@ -4814,32 +4915,33 @@
         <f>O32-AC32</f>
         <v>48</v>
       </c>
-      <c r="AE32" s="175">
+      <c r="AE32" s="360">
         <f>AD32/O32</f>
         <v>1</v>
       </c>
-      <c r="AG32" s="184">
+      <c r="AF32" s="179"/>
+      <c r="AG32" s="355">
         <f>O32-AF32</f>
         <v>48</v>
       </c>
-      <c r="AH32" s="185">
+      <c r="AH32" s="356">
         <f>AG32/O32</f>
         <v>1</v>
       </c>
-      <c r="AI32" s="356" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="201"/>
-      <c r="B33" s="327"/>
-      <c r="C33" s="329"/>
-      <c r="D33" s="301"/>
+      <c r="AI32" s="357" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="326"/>
+      <c r="B33" s="198"/>
+      <c r="C33" s="200"/>
+      <c r="D33" s="265"/>
       <c r="E33" s="78"/>
       <c r="F33" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="225"/>
+      <c r="G33" s="344"/>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -4849,7 +4951,7 @@
         <v>12</v>
       </c>
       <c r="N33" s="83"/>
-      <c r="O33" s="295"/>
+      <c r="O33" s="250"/>
       <c r="P33" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4868,18 +4970,24 @@
       <c r="AB33" s="178"/>
       <c r="AC33" s="179"/>
       <c r="AD33" s="179"/>
-      <c r="AE33" s="179"/>
-    </row>
-    <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="201"/>
-      <c r="B34" s="327"/>
-      <c r="C34" s="329"/>
-      <c r="D34" s="301"/>
+      <c r="AE33" s="361"/>
+      <c r="AF33" s="179"/>
+      <c r="AG33" s="179"/>
+      <c r="AH33" s="179"/>
+      <c r="AI33" s="357" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="326"/>
+      <c r="B34" s="198"/>
+      <c r="C34" s="200"/>
+      <c r="D34" s="265"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="225"/>
+      <c r="G34" s="344"/>
       <c r="H34" s="83"/>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -4889,7 +4997,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="83"/>
-      <c r="O34" s="295"/>
+      <c r="O34" s="250"/>
       <c r="P34" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4908,18 +5016,24 @@
       <c r="AB34" s="178"/>
       <c r="AC34" s="179"/>
       <c r="AD34" s="179"/>
-      <c r="AE34" s="179"/>
-    </row>
-    <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="201"/>
-      <c r="B35" s="327"/>
-      <c r="C35" s="329"/>
-      <c r="D35" s="302"/>
+      <c r="AE34" s="361"/>
+      <c r="AF34" s="179"/>
+      <c r="AG34" s="179"/>
+      <c r="AH34" s="179"/>
+      <c r="AI34" s="357" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="326"/>
+      <c r="B35" s="198"/>
+      <c r="C35" s="200"/>
+      <c r="D35" s="266"/>
       <c r="E35" s="80"/>
       <c r="F35" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="226"/>
+      <c r="G35" s="345"/>
       <c r="H35" s="84"/>
       <c r="I35" s="84"/>
       <c r="J35" s="84"/>
@@ -4929,7 +5043,7 @@
         <v>12</v>
       </c>
       <c r="N35" s="84"/>
-      <c r="O35" s="296"/>
+      <c r="O35" s="251"/>
       <c r="P35" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4948,16 +5062,22 @@
       <c r="AB35" s="178"/>
       <c r="AC35" s="179"/>
       <c r="AD35" s="179"/>
-      <c r="AE35" s="179"/>
-    </row>
-    <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="201"/>
-      <c r="B36" s="327"/>
-      <c r="C36" s="329"/>
-      <c r="D36" s="288"/>
-      <c r="E36" s="289"/>
-      <c r="F36" s="289"/>
-      <c r="G36" s="290"/>
+      <c r="AE35" s="361"/>
+      <c r="AF35" s="179"/>
+      <c r="AG35" s="179"/>
+      <c r="AH35" s="179"/>
+      <c r="AI35" s="357" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="326"/>
+      <c r="B36" s="198"/>
+      <c r="C36" s="200"/>
+      <c r="D36" s="243"/>
+      <c r="E36" s="244"/>
+      <c r="F36" s="244"/>
+      <c r="G36" s="245"/>
       <c r="H36" s="86">
         <f>SUM(H32:H35)</f>
         <v>0</v>
@@ -5003,10 +5123,10 @@
       <c r="AC36" s="182"/>
       <c r="AD36" s="168"/>
       <c r="AE36" s="168"/>
-      <c r="AF36" s="2"/>
-      <c r="AG36" s="2"/>
-      <c r="AH36" s="2"/>
-      <c r="AI36" s="2"/>
+      <c r="AF36" s="168"/>
+      <c r="AG36" s="168"/>
+      <c r="AH36" s="168"/>
+      <c r="AI36" s="168"/>
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
       <c r="AL36" s="2"/>
@@ -5018,18 +5138,18 @@
       <c r="AR36" s="2"/>
       <c r="AS36" s="2"/>
     </row>
-    <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="201"/>
-      <c r="B37" s="327"/>
-      <c r="C37" s="329"/>
-      <c r="D37" s="227" t="s">
+    <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="326"/>
+      <c r="B37" s="198"/>
+      <c r="C37" s="200"/>
+      <c r="D37" s="346" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="230">
+      <c r="G37" s="349">
         <v>48</v>
       </c>
       <c r="H37" s="95"/>
@@ -5041,7 +5161,7 @@
       <c r="N37" s="95">
         <v>12</v>
       </c>
-      <c r="O37" s="297">
+      <c r="O37" s="252">
         <f t="shared" ref="O37" si="34">SUM(P37:P40)</f>
         <v>48</v>
       </c>
@@ -5079,8 +5199,8 @@
         <f>AG37/O37</f>
         <v>1</v>
       </c>
-      <c r="AI37" s="356" t="s">
-        <v>112</v>
+      <c r="AI37" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
@@ -5093,16 +5213,16 @@
       <c r="AR37" s="3"/>
       <c r="AS37" s="3"/>
     </row>
-    <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="201"/>
-      <c r="B38" s="327"/>
-      <c r="C38" s="329"/>
-      <c r="D38" s="228"/>
+    <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="326"/>
+      <c r="B38" s="198"/>
+      <c r="C38" s="200"/>
+      <c r="D38" s="347"/>
       <c r="E38" s="89"/>
       <c r="F38" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="231"/>
+      <c r="G38" s="350"/>
       <c r="H38" s="96"/>
       <c r="I38" s="96"/>
       <c r="J38" s="96"/>
@@ -5112,7 +5232,7 @@
       <c r="N38" s="96">
         <v>12</v>
       </c>
-      <c r="O38" s="298"/>
+      <c r="O38" s="253"/>
       <c r="P38" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5135,7 +5255,9 @@
       <c r="AF38" s="3"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
-      <c r="AI38" s="3"/>
+      <c r="AI38" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
       <c r="AL38" s="3"/>
@@ -5147,16 +5269,16 @@
       <c r="AR38" s="3"/>
       <c r="AS38" s="3"/>
     </row>
-    <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="201"/>
-      <c r="B39" s="327"/>
-      <c r="C39" s="329"/>
-      <c r="D39" s="228"/>
+    <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="326"/>
+      <c r="B39" s="198"/>
+      <c r="C39" s="200"/>
+      <c r="D39" s="347"/>
       <c r="E39" s="89"/>
       <c r="F39" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="231"/>
+      <c r="G39" s="350"/>
       <c r="H39" s="96"/>
       <c r="I39" s="96"/>
       <c r="J39" s="96"/>
@@ -5166,7 +5288,7 @@
       <c r="N39" s="96">
         <v>12</v>
       </c>
-      <c r="O39" s="298"/>
+      <c r="O39" s="253"/>
       <c r="P39" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5189,7 +5311,9 @@
       <c r="AF39" s="3"/>
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
-      <c r="AI39" s="3"/>
+      <c r="AI39" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
@@ -5201,16 +5325,16 @@
       <c r="AR39" s="3"/>
       <c r="AS39" s="3"/>
     </row>
-    <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="201"/>
-      <c r="B40" s="327"/>
-      <c r="C40" s="329"/>
-      <c r="D40" s="229"/>
+    <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="326"/>
+      <c r="B40" s="198"/>
+      <c r="C40" s="200"/>
+      <c r="D40" s="348"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="232"/>
+      <c r="G40" s="351"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
       <c r="J40" s="97"/>
@@ -5220,7 +5344,7 @@
       <c r="N40" s="97">
         <v>12</v>
       </c>
-      <c r="O40" s="299"/>
+      <c r="O40" s="254"/>
       <c r="P40" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5243,7 +5367,9 @@
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
-      <c r="AI40" s="3"/>
+      <c r="AI40" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
       <c r="AL40" s="3"/>
@@ -5255,14 +5381,14 @@
       <c r="AR40" s="3"/>
       <c r="AS40" s="3"/>
     </row>
-    <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="201"/>
-      <c r="B41" s="327"/>
-      <c r="C41" s="329"/>
-      <c r="D41" s="291"/>
-      <c r="E41" s="292"/>
-      <c r="F41" s="292"/>
-      <c r="G41" s="293"/>
+    <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="326"/>
+      <c r="B41" s="198"/>
+      <c r="C41" s="200"/>
+      <c r="D41" s="246"/>
+      <c r="E41" s="247"/>
+      <c r="F41" s="247"/>
+      <c r="G41" s="248"/>
       <c r="H41" s="93">
         <f>SUM(H37:H40)</f>
         <v>0</v>
@@ -5323,18 +5449,18 @@
       <c r="AR41" s="2"/>
       <c r="AS41" s="2"/>
     </row>
-    <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="201"/>
-      <c r="B42" s="327"/>
-      <c r="C42" s="329"/>
-      <c r="D42" s="188" t="s">
+    <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="326"/>
+      <c r="B42" s="198"/>
+      <c r="C42" s="200"/>
+      <c r="D42" s="258" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="191">
+      <c r="G42" s="261">
         <v>48</v>
       </c>
       <c r="H42" s="34">
@@ -5346,7 +5472,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
-      <c r="O42" s="279">
+      <c r="O42" s="255">
         <f t="shared" ref="O42" si="41">SUM(P42:P45)</f>
         <v>48</v>
       </c>
@@ -5384,8 +5510,8 @@
         <f>AG42/O42</f>
         <v>1</v>
       </c>
-      <c r="AI42" s="356" t="s">
-        <v>112</v>
+      <c r="AI42" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -5398,16 +5524,16 @@
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
     </row>
-    <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="201"/>
-      <c r="B43" s="327"/>
-      <c r="C43" s="329"/>
-      <c r="D43" s="189"/>
+    <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="326"/>
+      <c r="B43" s="198"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="259"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="192"/>
+      <c r="G43" s="262"/>
       <c r="H43" s="35">
         <v>12</v>
       </c>
@@ -5417,7 +5543,7 @@
       <c r="L43" s="35"/>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="280"/>
+      <c r="O43" s="256"/>
       <c r="P43" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5440,7 +5566,9 @@
       <c r="AF43" s="3"/>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
-      <c r="AI43" s="3"/>
+      <c r="AI43" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="AJ43" s="3"/>
       <c r="AK43" s="3"/>
       <c r="AL43" s="3"/>
@@ -5452,16 +5580,16 @@
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
     </row>
-    <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="201"/>
-      <c r="B44" s="327"/>
-      <c r="C44" s="329"/>
-      <c r="D44" s="189"/>
+    <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="326"/>
+      <c r="B44" s="198"/>
+      <c r="C44" s="200"/>
+      <c r="D44" s="259"/>
       <c r="E44" s="30"/>
       <c r="F44" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="192"/>
+      <c r="G44" s="262"/>
       <c r="H44" s="35">
         <v>12</v>
       </c>
@@ -5471,7 +5599,7 @@
       <c r="L44" s="35"/>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
-      <c r="O44" s="280"/>
+      <c r="O44" s="256"/>
       <c r="P44" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5494,7 +5622,9 @@
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
-      <c r="AI44" s="3"/>
+      <c r="AI44" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
@@ -5506,16 +5636,16 @@
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
     </row>
-    <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="201"/>
-      <c r="B45" s="327"/>
-      <c r="C45" s="329"/>
-      <c r="D45" s="190"/>
+    <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="326"/>
+      <c r="B45" s="198"/>
+      <c r="C45" s="200"/>
+      <c r="D45" s="260"/>
       <c r="E45" s="32"/>
       <c r="F45" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="193"/>
+      <c r="G45" s="263"/>
       <c r="H45" s="36">
         <v>12</v>
       </c>
@@ -5525,7 +5655,7 @@
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
-      <c r="O45" s="281"/>
+      <c r="O45" s="257"/>
       <c r="P45" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5548,7 +5678,9 @@
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
-      <c r="AI45" s="3"/>
+      <c r="AI45" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
@@ -5560,14 +5692,14 @@
       <c r="AR45" s="3"/>
       <c r="AS45" s="3"/>
     </row>
-    <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="201"/>
-      <c r="B46" s="327"/>
-      <c r="C46" s="329"/>
-      <c r="D46" s="239"/>
-      <c r="E46" s="240"/>
-      <c r="F46" s="240"/>
-      <c r="G46" s="241"/>
+    <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="326"/>
+      <c r="B46" s="198"/>
+      <c r="C46" s="200"/>
+      <c r="D46" s="308"/>
+      <c r="E46" s="309"/>
+      <c r="F46" s="309"/>
+      <c r="G46" s="310"/>
       <c r="H46" s="98">
         <f>SUM(H42:H45)</f>
         <v>48</v>
@@ -5613,10 +5745,10 @@
       <c r="AC46" s="181"/>
       <c r="AD46" s="120"/>
       <c r="AE46" s="120"/>
-      <c r="AF46" s="2"/>
-      <c r="AG46" s="2"/>
-      <c r="AH46" s="2"/>
-      <c r="AI46" s="2"/>
+      <c r="AF46" s="120"/>
+      <c r="AG46" s="120"/>
+      <c r="AH46" s="120"/>
+      <c r="AI46" s="120"/>
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
@@ -5628,18 +5760,18 @@
       <c r="AR46" s="2"/>
       <c r="AS46" s="2"/>
     </row>
-    <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="201"/>
-      <c r="B47" s="327"/>
-      <c r="C47" s="329"/>
-      <c r="D47" s="245" t="s">
+    <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="326"/>
+      <c r="B47" s="198"/>
+      <c r="C47" s="200"/>
+      <c r="D47" s="314" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="99"/>
       <c r="F47" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="236">
+      <c r="G47" s="302">
         <v>48</v>
       </c>
       <c r="H47" s="107"/>
@@ -5651,7 +5783,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
-      <c r="O47" s="265">
+      <c r="O47" s="267">
         <f t="shared" ref="O47" si="48">SUM(P47:P50)</f>
         <v>48</v>
       </c>
@@ -5680,28 +5812,29 @@
       <c r="AC47" s="179"/>
       <c r="AD47" s="179"/>
       <c r="AE47" s="179"/>
-      <c r="AG47" s="184">
+      <c r="AF47" s="179"/>
+      <c r="AG47" s="355">
         <f>O47-AF47</f>
         <v>48</v>
       </c>
-      <c r="AH47" s="185">
+      <c r="AH47" s="356">
         <f>AG47/O47</f>
         <v>1</v>
       </c>
-      <c r="AI47" s="356" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="201"/>
-      <c r="B48" s="327"/>
-      <c r="C48" s="329"/>
-      <c r="D48" s="246"/>
+      <c r="AI47" s="357" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="326"/>
+      <c r="B48" s="198"/>
+      <c r="C48" s="200"/>
+      <c r="D48" s="315"/>
       <c r="E48" s="101"/>
       <c r="F48" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="237"/>
+      <c r="G48" s="303"/>
       <c r="H48" s="108"/>
       <c r="I48" s="108">
         <v>12</v>
@@ -5711,7 +5844,7 @@
       <c r="L48" s="108"/>
       <c r="M48" s="108"/>
       <c r="N48" s="108"/>
-      <c r="O48" s="266"/>
+      <c r="O48" s="268"/>
       <c r="P48" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5731,17 +5864,23 @@
       <c r="AC48" s="179"/>
       <c r="AD48" s="179"/>
       <c r="AE48" s="179"/>
-    </row>
-    <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="201"/>
-      <c r="B49" s="327"/>
-      <c r="C49" s="329"/>
-      <c r="D49" s="246"/>
+      <c r="AF48" s="179"/>
+      <c r="AG48" s="179"/>
+      <c r="AH48" s="179"/>
+      <c r="AI48" s="357" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="326"/>
+      <c r="B49" s="198"/>
+      <c r="C49" s="200"/>
+      <c r="D49" s="315"/>
       <c r="E49" s="101"/>
       <c r="F49" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="237"/>
+      <c r="G49" s="303"/>
       <c r="H49" s="108"/>
       <c r="I49" s="108">
         <v>12</v>
@@ -5751,7 +5890,7 @@
       <c r="L49" s="108"/>
       <c r="M49" s="108"/>
       <c r="N49" s="108"/>
-      <c r="O49" s="266"/>
+      <c r="O49" s="268"/>
       <c r="P49" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5771,17 +5910,23 @@
       <c r="AC49" s="179"/>
       <c r="AD49" s="179"/>
       <c r="AE49" s="179"/>
-    </row>
-    <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="201"/>
-      <c r="B50" s="327"/>
-      <c r="C50" s="329"/>
-      <c r="D50" s="247"/>
+      <c r="AF49" s="179"/>
+      <c r="AG49" s="179"/>
+      <c r="AH49" s="179"/>
+      <c r="AI49" s="357" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="326"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="200"/>
+      <c r="D50" s="316"/>
       <c r="E50" s="103"/>
       <c r="F50" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="G50" s="238"/>
+      <c r="G50" s="304"/>
       <c r="H50" s="109"/>
       <c r="I50" s="109">
         <v>12</v>
@@ -5791,7 +5936,7 @@
       <c r="L50" s="109"/>
       <c r="M50" s="109"/>
       <c r="N50" s="109"/>
-      <c r="O50" s="267"/>
+      <c r="O50" s="269"/>
       <c r="P50" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5811,15 +5956,21 @@
       <c r="AC50" s="179"/>
       <c r="AD50" s="179"/>
       <c r="AE50" s="179"/>
-    </row>
-    <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="201"/>
-      <c r="B51" s="327"/>
-      <c r="C51" s="329"/>
-      <c r="D51" s="242"/>
-      <c r="E51" s="243"/>
-      <c r="F51" s="243"/>
-      <c r="G51" s="244"/>
+      <c r="AF50" s="179"/>
+      <c r="AG50" s="179"/>
+      <c r="AH50" s="179"/>
+      <c r="AI50" s="357" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="326"/>
+      <c r="B51" s="198"/>
+      <c r="C51" s="200"/>
+      <c r="D51" s="311"/>
+      <c r="E51" s="312"/>
+      <c r="F51" s="312"/>
+      <c r="G51" s="313"/>
       <c r="H51" s="106">
         <f>SUM(H47:H50)</f>
         <v>0</v>
@@ -5865,10 +6016,10 @@
       <c r="AC51" s="182"/>
       <c r="AD51" s="168"/>
       <c r="AE51" s="168"/>
-      <c r="AF51" s="2"/>
-      <c r="AG51" s="2"/>
-      <c r="AH51" s="2"/>
-      <c r="AI51" s="2"/>
+      <c r="AF51" s="168"/>
+      <c r="AG51" s="168"/>
+      <c r="AH51" s="168"/>
+      <c r="AI51" s="168"/>
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
       <c r="AL51" s="2"/>
@@ -5880,18 +6031,18 @@
       <c r="AR51" s="2"/>
       <c r="AS51" s="2"/>
     </row>
-    <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="201"/>
-      <c r="B52" s="327"/>
-      <c r="C52" s="329"/>
-      <c r="D52" s="209" t="s">
+    <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="326"/>
+      <c r="B52" s="198"/>
+      <c r="C52" s="200"/>
+      <c r="D52" s="317" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="47"/>
       <c r="F52" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G52" s="212">
+      <c r="G52" s="305">
         <v>48</v>
       </c>
       <c r="H52" s="53"/>
@@ -5903,7 +6054,7 @@
       <c r="N52" s="53">
         <v>12</v>
       </c>
-      <c r="O52" s="268">
+      <c r="O52" s="270">
         <f t="shared" ref="O52" si="55">SUM(P52:P55)</f>
         <v>48</v>
       </c>
@@ -5941,8 +6092,8 @@
         <f>AG52/O52</f>
         <v>1</v>
       </c>
-      <c r="AI52" s="356" t="s">
-        <v>112</v>
+      <c r="AI52" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
@@ -5955,16 +6106,16 @@
       <c r="AR52" s="3"/>
       <c r="AS52" s="3"/>
     </row>
-    <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="201"/>
-      <c r="B53" s="327"/>
-      <c r="C53" s="329"/>
-      <c r="D53" s="210"/>
+    <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="326"/>
+      <c r="B53" s="198"/>
+      <c r="C53" s="200"/>
+      <c r="D53" s="318"/>
       <c r="E53" s="49"/>
       <c r="F53" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G53" s="213"/>
+      <c r="G53" s="306"/>
       <c r="H53" s="54"/>
       <c r="I53" s="54"/>
       <c r="J53" s="54"/>
@@ -5974,7 +6125,7 @@
       <c r="N53" s="54">
         <v>12</v>
       </c>
-      <c r="O53" s="269"/>
+      <c r="O53" s="271"/>
       <c r="P53" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5997,7 +6148,9 @@
       <c r="AF53" s="3"/>
       <c r="AG53" s="3"/>
       <c r="AH53" s="3"/>
-      <c r="AI53" s="3"/>
+      <c r="AI53" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
@@ -6009,16 +6162,16 @@
       <c r="AR53" s="3"/>
       <c r="AS53" s="3"/>
     </row>
-    <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="201"/>
-      <c r="B54" s="327"/>
-      <c r="C54" s="329"/>
-      <c r="D54" s="210"/>
+    <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="326"/>
+      <c r="B54" s="198"/>
+      <c r="C54" s="200"/>
+      <c r="D54" s="318"/>
       <c r="E54" s="49"/>
       <c r="F54" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="213"/>
+      <c r="G54" s="306"/>
       <c r="H54" s="54"/>
       <c r="I54" s="54"/>
       <c r="J54" s="54"/>
@@ -6028,7 +6181,7 @@
       <c r="N54" s="54">
         <v>12</v>
       </c>
-      <c r="O54" s="269"/>
+      <c r="O54" s="271"/>
       <c r="P54" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6051,7 +6204,9 @@
       <c r="AF54" s="3"/>
       <c r="AG54" s="3"/>
       <c r="AH54" s="3"/>
-      <c r="AI54" s="3"/>
+      <c r="AI54" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
       <c r="AL54" s="3"/>
@@ -6063,16 +6218,16 @@
       <c r="AR54" s="3"/>
       <c r="AS54" s="3"/>
     </row>
-    <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="201"/>
-      <c r="B55" s="327"/>
-      <c r="C55" s="329"/>
-      <c r="D55" s="211"/>
+    <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="326"/>
+      <c r="B55" s="198"/>
+      <c r="C55" s="200"/>
+      <c r="D55" s="319"/>
       <c r="E55" s="51"/>
       <c r="F55" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="214"/>
+      <c r="G55" s="307"/>
       <c r="H55" s="55"/>
       <c r="I55" s="55"/>
       <c r="J55" s="55"/>
@@ -6082,7 +6237,7 @@
       <c r="N55" s="55">
         <v>12</v>
       </c>
-      <c r="O55" s="270"/>
+      <c r="O55" s="272"/>
       <c r="P55" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6105,7 +6260,9 @@
       <c r="AF55" s="3"/>
       <c r="AG55" s="3"/>
       <c r="AH55" s="3"/>
-      <c r="AI55" s="3"/>
+      <c r="AI55" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="AJ55" s="3"/>
       <c r="AK55" s="3"/>
       <c r="AL55" s="3"/>
@@ -6117,14 +6274,14 @@
       <c r="AR55" s="3"/>
       <c r="AS55" s="3"/>
     </row>
-    <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="201"/>
-      <c r="B56" s="327"/>
-      <c r="C56" s="329"/>
-      <c r="D56" s="248"/>
-      <c r="E56" s="249"/>
-      <c r="F56" s="249"/>
-      <c r="G56" s="250"/>
+    <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="326"/>
+      <c r="B56" s="198"/>
+      <c r="C56" s="200"/>
+      <c r="D56" s="287"/>
+      <c r="E56" s="288"/>
+      <c r="F56" s="288"/>
+      <c r="G56" s="289"/>
       <c r="H56" s="64">
         <f>SUM(H52:H55)</f>
         <v>0</v>
@@ -6185,11 +6342,11 @@
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
     </row>
-    <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="201"/>
-      <c r="B57" s="327"/>
-      <c r="C57" s="329"/>
-      <c r="D57" s="257" t="s">
+    <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="326"/>
+      <c r="B57" s="198"/>
+      <c r="C57" s="200"/>
+      <c r="D57" s="296" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="149">
@@ -6198,7 +6355,7 @@
       <c r="F57" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="259">
+      <c r="G57" s="297">
         <v>96</v>
       </c>
       <c r="H57" s="114"/>
@@ -6210,7 +6367,7 @@
       <c r="L57" s="114"/>
       <c r="M57" s="114"/>
       <c r="N57" s="114"/>
-      <c r="O57" s="271">
+      <c r="O57" s="273">
         <f t="shared" ref="O57" si="62">SUM(P57:P60)</f>
         <v>96</v>
       </c>
@@ -6265,16 +6422,16 @@
         <v>0.3125</v>
       </c>
       <c r="AF57" s="176"/>
-      <c r="AG57" s="184">
+      <c r="AG57" s="358">
         <f>O57-AF57</f>
         <v>96</v>
       </c>
-      <c r="AH57" s="185">
+      <c r="AH57" s="359">
         <f>AG57/O57</f>
         <v>1</v>
       </c>
-      <c r="AI57" s="356" t="s">
-        <v>112</v>
+      <c r="AI57" s="176" t="s">
+        <v>118</v>
       </c>
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
@@ -6287,18 +6444,18 @@
       <c r="AR57" s="3"/>
       <c r="AS57" s="3"/>
     </row>
-    <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="201"/>
-      <c r="B58" s="327"/>
-      <c r="C58" s="329"/>
-      <c r="D58" s="258"/>
+    <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="326"/>
+      <c r="B58" s="198"/>
+      <c r="C58" s="200"/>
+      <c r="D58" s="241"/>
       <c r="E58" s="145">
         <v>2</v>
       </c>
       <c r="F58" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="G58" s="260"/>
+      <c r="G58" s="298"/>
       <c r="H58" s="115"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115">
@@ -6308,7 +6465,7 @@
       <c r="L58" s="115"/>
       <c r="M58" s="115"/>
       <c r="N58" s="115"/>
-      <c r="O58" s="272"/>
+      <c r="O58" s="274"/>
       <c r="P58" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6329,9 +6486,11 @@
       <c r="AD58" s="177"/>
       <c r="AE58" s="177"/>
       <c r="AF58" s="177"/>
-      <c r="AG58" s="7"/>
-      <c r="AH58" s="7"/>
-      <c r="AI58" s="7"/>
+      <c r="AG58" s="177"/>
+      <c r="AH58" s="177"/>
+      <c r="AI58" s="176" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ58" s="7"/>
       <c r="AK58" s="7"/>
       <c r="AL58" s="7"/>
@@ -6343,18 +6502,18 @@
       <c r="AR58" s="7"/>
       <c r="AS58" s="7"/>
     </row>
-    <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="201"/>
-      <c r="B59" s="327"/>
-      <c r="C59" s="329"/>
-      <c r="D59" s="258"/>
+    <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="326"/>
+      <c r="B59" s="198"/>
+      <c r="C59" s="200"/>
+      <c r="D59" s="241"/>
       <c r="E59" s="145">
         <v>4</v>
       </c>
       <c r="F59" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="260"/>
+      <c r="G59" s="298"/>
       <c r="H59" s="115"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115">
@@ -6364,7 +6523,7 @@
       <c r="L59" s="115"/>
       <c r="M59" s="115"/>
       <c r="N59" s="115"/>
-      <c r="O59" s="272"/>
+      <c r="O59" s="274"/>
       <c r="P59" s="9">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -6385,9 +6544,11 @@
       <c r="AD59" s="177"/>
       <c r="AE59" s="177"/>
       <c r="AF59" s="177"/>
-      <c r="AG59" s="7"/>
-      <c r="AH59" s="7"/>
-      <c r="AI59" s="7"/>
+      <c r="AG59" s="177"/>
+      <c r="AH59" s="177"/>
+      <c r="AI59" s="176" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ59" s="7"/>
       <c r="AK59" s="7"/>
       <c r="AL59" s="7"/>
@@ -6399,18 +6560,18 @@
       <c r="AR59" s="7"/>
       <c r="AS59" s="7"/>
     </row>
-    <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="201"/>
-      <c r="B60" s="327"/>
-      <c r="C60" s="329"/>
-      <c r="D60" s="258"/>
+    <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="326"/>
+      <c r="B60" s="198"/>
+      <c r="C60" s="200"/>
+      <c r="D60" s="241"/>
       <c r="E60" s="145">
         <v>1</v>
       </c>
       <c r="F60" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="260"/>
+      <c r="G60" s="298"/>
       <c r="H60" s="115"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115">
@@ -6420,7 +6581,7 @@
       <c r="L60" s="115"/>
       <c r="M60" s="115"/>
       <c r="N60" s="115"/>
-      <c r="O60" s="272"/>
+      <c r="O60" s="274"/>
       <c r="P60" s="9">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -6441,9 +6602,11 @@
       <c r="AD60" s="177"/>
       <c r="AE60" s="177"/>
       <c r="AF60" s="177"/>
-      <c r="AG60" s="7"/>
-      <c r="AH60" s="7"/>
-      <c r="AI60" s="7"/>
+      <c r="AG60" s="177"/>
+      <c r="AH60" s="177"/>
+      <c r="AI60" s="176" t="s">
+        <v>118</v>
+      </c>
       <c r="AJ60" s="7"/>
       <c r="AK60" s="7"/>
       <c r="AL60" s="7"/>
@@ -6455,14 +6618,14 @@
       <c r="AR60" s="7"/>
       <c r="AS60" s="7"/>
     </row>
-    <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="201"/>
-      <c r="B61" s="327"/>
-      <c r="C61" s="329"/>
-      <c r="D61" s="261"/>
-      <c r="E61" s="262"/>
-      <c r="F61" s="262"/>
-      <c r="G61" s="262"/>
+    <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="326"/>
+      <c r="B61" s="198"/>
+      <c r="C61" s="200"/>
+      <c r="D61" s="242"/>
+      <c r="E61" s="299"/>
+      <c r="F61" s="299"/>
+      <c r="G61" s="299"/>
       <c r="H61" s="150">
         <f>SUM(H57:H60)</f>
         <v>0</v>
@@ -6509,9 +6672,9 @@
       <c r="AD61" s="168"/>
       <c r="AE61" s="168"/>
       <c r="AF61" s="168"/>
-      <c r="AG61" s="2"/>
-      <c r="AH61" s="2"/>
-      <c r="AI61" s="2"/>
+      <c r="AG61" s="168"/>
+      <c r="AH61" s="168"/>
+      <c r="AI61" s="168"/>
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
       <c r="AL61" s="2"/>
@@ -6523,11 +6686,11 @@
       <c r="AR61" s="2"/>
       <c r="AS61" s="2"/>
     </row>
-    <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="201"/>
-      <c r="B62" s="327"/>
-      <c r="C62" s="329"/>
-      <c r="D62" s="253" t="s">
+    <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="326"/>
+      <c r="B62" s="198"/>
+      <c r="C62" s="200"/>
+      <c r="D62" s="292" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="142">
@@ -6536,7 +6699,7 @@
       <c r="F62" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="G62" s="254">
+      <c r="G62" s="293">
         <v>288</v>
       </c>
       <c r="H62" s="132"/>
@@ -6548,7 +6711,7 @@
         <v>72</v>
       </c>
       <c r="N62" s="132"/>
-      <c r="O62" s="352">
+      <c r="O62" s="193">
         <f t="shared" ref="O62" si="69">SUM(P62:P65)</f>
         <v>288</v>
       </c>
@@ -6609,8 +6772,8 @@
         <f>AG62/O62</f>
         <v>1</v>
       </c>
-      <c r="AI62" s="356" t="s">
-        <v>112</v>
+      <c r="AI62" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
@@ -6623,18 +6786,18 @@
       <c r="AR62" s="3"/>
       <c r="AS62" s="3"/>
     </row>
-    <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="201"/>
-      <c r="B63" s="327"/>
-      <c r="C63" s="329"/>
-      <c r="D63" s="189"/>
+    <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="326"/>
+      <c r="B63" s="198"/>
+      <c r="C63" s="200"/>
+      <c r="D63" s="259"/>
       <c r="E63" s="116">
         <v>1</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="192"/>
+      <c r="G63" s="262"/>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
@@ -6644,7 +6807,7 @@
       <c r="L63" s="35"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
-      <c r="O63" s="353"/>
+      <c r="O63" s="194"/>
       <c r="P63" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6667,7 +6830,9 @@
       <c r="AF63" s="3"/>
       <c r="AG63" s="3"/>
       <c r="AH63" s="3"/>
-      <c r="AI63" s="3"/>
+      <c r="AI63" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ63" s="3"/>
       <c r="AK63" s="3"/>
       <c r="AL63" s="3"/>
@@ -6679,18 +6844,18 @@
       <c r="AR63" s="3"/>
       <c r="AS63" s="3"/>
     </row>
-    <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="201"/>
-      <c r="B64" s="327"/>
-      <c r="C64" s="329"/>
-      <c r="D64" s="189"/>
+    <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="326"/>
+      <c r="B64" s="198"/>
+      <c r="C64" s="200"/>
+      <c r="D64" s="259"/>
       <c r="E64" s="116">
         <v>2</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="192"/>
+      <c r="G64" s="262"/>
       <c r="H64" s="35"/>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
@@ -6700,7 +6865,7 @@
       <c r="L64" s="35"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
-      <c r="O64" s="353"/>
+      <c r="O64" s="194"/>
       <c r="P64" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6723,7 +6888,9 @@
       <c r="AF64" s="3"/>
       <c r="AG64" s="3"/>
       <c r="AH64" s="3"/>
-      <c r="AI64" s="3"/>
+      <c r="AI64" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ64" s="3"/>
       <c r="AK64" s="3"/>
       <c r="AL64" s="3"/>
@@ -6735,18 +6902,18 @@
       <c r="AR64" s="3"/>
       <c r="AS64" s="3"/>
     </row>
-    <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="201"/>
-      <c r="B65" s="327"/>
-      <c r="C65" s="329"/>
-      <c r="D65" s="189"/>
+    <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="326"/>
+      <c r="B65" s="198"/>
+      <c r="C65" s="200"/>
+      <c r="D65" s="259"/>
       <c r="E65" s="116">
         <v>3</v>
       </c>
       <c r="F65" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G65" s="192"/>
+      <c r="G65" s="262"/>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
       <c r="J65" s="35"/>
@@ -6758,7 +6925,7 @@
       </c>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
-      <c r="O65" s="353"/>
+      <c r="O65" s="194"/>
       <c r="P65" s="9">
         <f t="shared" si="4"/>
         <v>168</v>
@@ -6781,7 +6948,9 @@
       <c r="AF65" s="3"/>
       <c r="AG65" s="3"/>
       <c r="AH65" s="3"/>
-      <c r="AI65" s="3"/>
+      <c r="AI65" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
       <c r="AL65" s="3"/>
@@ -6793,14 +6962,14 @@
       <c r="AR65" s="3"/>
       <c r="AS65" s="3"/>
     </row>
-    <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="201"/>
-      <c r="B66" s="327"/>
-      <c r="C66" s="329"/>
-      <c r="D66" s="263"/>
-      <c r="E66" s="264"/>
-      <c r="F66" s="264"/>
-      <c r="G66" s="264"/>
+    <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="326"/>
+      <c r="B66" s="198"/>
+      <c r="C66" s="200"/>
+      <c r="D66" s="300"/>
+      <c r="E66" s="301"/>
+      <c r="F66" s="301"/>
+      <c r="G66" s="301"/>
       <c r="H66" s="152">
         <f>SUM(H62:H65)</f>
         <v>0</v>
@@ -6861,18 +7030,18 @@
       <c r="AR66" s="2"/>
       <c r="AS66" s="2"/>
     </row>
-    <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="201"/>
-      <c r="B67" s="327"/>
-      <c r="C67" s="329"/>
-      <c r="D67" s="251" t="s">
+    <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="326"/>
+      <c r="B67" s="198"/>
+      <c r="C67" s="200"/>
+      <c r="D67" s="290" t="s">
         <v>49</v>
       </c>
       <c r="E67" s="134"/>
       <c r="F67" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="255">
+      <c r="G67" s="294">
         <v>384</v>
       </c>
       <c r="H67" s="128">
@@ -6884,7 +7053,7 @@
       <c r="L67" s="128"/>
       <c r="M67" s="128"/>
       <c r="N67" s="128"/>
-      <c r="O67" s="354">
+      <c r="O67" s="195">
         <f>SUM(P67:P72)</f>
         <v>384</v>
       </c>
@@ -6922,8 +7091,8 @@
         <f>AG67/O67</f>
         <v>1</v>
       </c>
-      <c r="AI67" s="356" t="s">
-        <v>112</v>
+      <c r="AI67" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
@@ -6936,16 +7105,16 @@
       <c r="AR67" s="3"/>
       <c r="AS67" s="3"/>
     </row>
-    <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="201"/>
-      <c r="B68" s="327"/>
-      <c r="C68" s="329"/>
-      <c r="D68" s="252"/>
+    <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="326"/>
+      <c r="B68" s="198"/>
+      <c r="C68" s="200"/>
+      <c r="D68" s="291"/>
       <c r="E68" s="133"/>
       <c r="F68" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="256"/>
+      <c r="G68" s="295"/>
       <c r="H68" s="130"/>
       <c r="I68" s="130">
         <v>72</v>
@@ -6955,7 +7124,7 @@
       <c r="L68" s="130"/>
       <c r="M68" s="130"/>
       <c r="N68" s="130"/>
-      <c r="O68" s="355"/>
+      <c r="O68" s="196"/>
       <c r="P68" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -6978,7 +7147,9 @@
       <c r="AF68" s="3"/>
       <c r="AG68" s="3"/>
       <c r="AH68" s="3"/>
-      <c r="AI68" s="3"/>
+      <c r="AI68" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
       <c r="AL68" s="3"/>
@@ -6990,16 +7161,16 @@
       <c r="AR68" s="3"/>
       <c r="AS68" s="3"/>
     </row>
-    <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="201"/>
-      <c r="B69" s="327"/>
-      <c r="C69" s="329"/>
-      <c r="D69" s="252"/>
+    <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="326"/>
+      <c r="B69" s="198"/>
+      <c r="C69" s="200"/>
+      <c r="D69" s="291"/>
       <c r="E69" s="133"/>
       <c r="F69" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="256"/>
+      <c r="G69" s="295"/>
       <c r="H69" s="130"/>
       <c r="I69" s="130"/>
       <c r="J69" s="130">
@@ -7009,7 +7180,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="130"/>
       <c r="N69" s="130"/>
-      <c r="O69" s="355"/>
+      <c r="O69" s="196"/>
       <c r="P69" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7032,7 +7203,9 @@
       <c r="AF69" s="3"/>
       <c r="AG69" s="3"/>
       <c r="AH69" s="3"/>
-      <c r="AI69" s="3"/>
+      <c r="AI69" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
       <c r="AL69" s="3"/>
@@ -7044,16 +7217,16 @@
       <c r="AR69" s="3"/>
       <c r="AS69" s="3"/>
     </row>
-    <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="201"/>
-      <c r="B70" s="327"/>
-      <c r="C70" s="329"/>
-      <c r="D70" s="252"/>
+    <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="326"/>
+      <c r="B70" s="198"/>
+      <c r="C70" s="200"/>
+      <c r="D70" s="291"/>
       <c r="E70" s="133"/>
       <c r="F70" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="256"/>
+      <c r="G70" s="295"/>
       <c r="H70" s="130"/>
       <c r="I70" s="130"/>
       <c r="J70" s="130"/>
@@ -7063,7 +7236,7 @@
       <c r="L70" s="130"/>
       <c r="M70" s="130"/>
       <c r="N70" s="130"/>
-      <c r="O70" s="355"/>
+      <c r="O70" s="196"/>
       <c r="P70" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7086,7 +7259,9 @@
       <c r="AF70" s="3"/>
       <c r="AG70" s="3"/>
       <c r="AH70" s="3"/>
-      <c r="AI70" s="3"/>
+      <c r="AI70" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ70" s="3"/>
       <c r="AK70" s="3"/>
       <c r="AL70" s="3"/>
@@ -7098,16 +7273,16 @@
       <c r="AR70" s="3"/>
       <c r="AS70" s="3"/>
     </row>
-    <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="201"/>
-      <c r="B71" s="327"/>
-      <c r="C71" s="329"/>
-      <c r="D71" s="252"/>
+    <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="326"/>
+      <c r="B71" s="198"/>
+      <c r="C71" s="200"/>
+      <c r="D71" s="291"/>
       <c r="E71" s="133"/>
       <c r="F71" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="256"/>
+      <c r="G71" s="295"/>
       <c r="H71" s="130"/>
       <c r="I71" s="130"/>
       <c r="J71" s="130"/>
@@ -7117,7 +7292,7 @@
       </c>
       <c r="M71" s="130"/>
       <c r="N71" s="130"/>
-      <c r="O71" s="355"/>
+      <c r="O71" s="196"/>
       <c r="P71" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7140,7 +7315,9 @@
       <c r="AF71" s="3"/>
       <c r="AG71" s="3"/>
       <c r="AH71" s="3"/>
-      <c r="AI71" s="3"/>
+      <c r="AI71" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
       <c r="AL71" s="3"/>
@@ -7152,16 +7329,16 @@
       <c r="AR71" s="3"/>
       <c r="AS71" s="3"/>
     </row>
-    <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="201"/>
-      <c r="B72" s="327"/>
-      <c r="C72" s="329"/>
-      <c r="D72" s="252"/>
+    <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="326"/>
+      <c r="B72" s="198"/>
+      <c r="C72" s="200"/>
+      <c r="D72" s="291"/>
       <c r="E72" s="133"/>
       <c r="F72" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="256"/>
+      <c r="G72" s="295"/>
       <c r="H72" s="130"/>
       <c r="I72" s="130"/>
       <c r="J72" s="130"/>
@@ -7171,7 +7348,7 @@
         <v>24</v>
       </c>
       <c r="N72" s="130"/>
-      <c r="O72" s="355"/>
+      <c r="O72" s="196"/>
       <c r="P72" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7194,7 +7371,9 @@
       <c r="AF72" s="3"/>
       <c r="AG72" s="3"/>
       <c r="AH72" s="3"/>
-      <c r="AI72" s="3"/>
+      <c r="AI72" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3"/>
       <c r="AL72" s="3"/>
@@ -7206,14 +7385,14 @@
       <c r="AR72" s="3"/>
       <c r="AS72" s="3"/>
     </row>
-    <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="201"/>
-      <c r="B73" s="327"/>
-      <c r="C73" s="329"/>
-      <c r="D73" s="305"/>
-      <c r="E73" s="306"/>
-      <c r="F73" s="306"/>
-      <c r="G73" s="306"/>
+    <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="326"/>
+      <c r="B73" s="198"/>
+      <c r="C73" s="200"/>
+      <c r="D73" s="220"/>
+      <c r="E73" s="221"/>
+      <c r="F73" s="221"/>
+      <c r="G73" s="221"/>
       <c r="H73" s="135">
         <f>SUM(H67:H72)</f>
         <v>72</v>
@@ -7274,18 +7453,18 @@
       <c r="AR73" s="2"/>
       <c r="AS73" s="2"/>
     </row>
-    <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="201"/>
-      <c r="B74" s="327"/>
-      <c r="C74" s="329"/>
-      <c r="D74" s="325" t="s">
+    <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="326"/>
+      <c r="B74" s="198"/>
+      <c r="C74" s="200"/>
+      <c r="D74" s="240" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="146"/>
       <c r="F74" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="315">
+      <c r="G74" s="230">
         <v>48</v>
       </c>
       <c r="H74" s="148"/>
@@ -7297,7 +7476,7 @@
       <c r="N74" s="148">
         <v>12</v>
       </c>
-      <c r="O74" s="346">
+      <c r="O74" s="187">
         <f>SUM(P74:P77)</f>
         <v>48</v>
       </c>
@@ -7335,8 +7514,8 @@
         <f>AG74/O74</f>
         <v>1</v>
       </c>
-      <c r="AI74" s="356" t="s">
-        <v>112</v>
+      <c r="AI74" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
@@ -7349,16 +7528,16 @@
       <c r="AR74" s="3"/>
       <c r="AS74" s="3"/>
     </row>
-    <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="201"/>
-      <c r="B75" s="327"/>
-      <c r="C75" s="329"/>
-      <c r="D75" s="258"/>
+    <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="326"/>
+      <c r="B75" s="198"/>
+      <c r="C75" s="200"/>
+      <c r="D75" s="241"/>
       <c r="E75" s="145"/>
       <c r="F75" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="315"/>
+      <c r="G75" s="230"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117"/>
       <c r="J75" s="117"/>
@@ -7368,7 +7547,7 @@
       <c r="N75" s="117">
         <v>12</v>
       </c>
-      <c r="O75" s="346"/>
+      <c r="O75" s="187"/>
       <c r="P75" s="9">
         <f t="shared" ref="P75:P77" si="81">SUM(H75:N75)</f>
         <v>12</v>
@@ -7391,7 +7570,9 @@
       <c r="AF75" s="3"/>
       <c r="AG75" s="3"/>
       <c r="AH75" s="3"/>
-      <c r="AI75" s="3"/>
+      <c r="AI75" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
       <c r="AL75" s="3"/>
@@ -7403,16 +7584,16 @@
       <c r="AR75" s="3"/>
       <c r="AS75" s="3"/>
     </row>
-    <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="201"/>
-      <c r="B76" s="327"/>
-      <c r="C76" s="329"/>
-      <c r="D76" s="258"/>
+    <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="326"/>
+      <c r="B76" s="198"/>
+      <c r="C76" s="200"/>
+      <c r="D76" s="241"/>
       <c r="E76" s="145"/>
       <c r="F76" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="315"/>
+      <c r="G76" s="230"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117"/>
       <c r="J76" s="117"/>
@@ -7422,7 +7603,7 @@
       <c r="N76" s="117">
         <v>12</v>
       </c>
-      <c r="O76" s="346"/>
+      <c r="O76" s="187"/>
       <c r="P76" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7445,7 +7626,9 @@
       <c r="AF76" s="3"/>
       <c r="AG76" s="3"/>
       <c r="AH76" s="3"/>
-      <c r="AI76" s="3"/>
+      <c r="AI76" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="AJ76" s="3"/>
       <c r="AK76" s="3"/>
       <c r="AL76" s="3"/>
@@ -7457,16 +7640,16 @@
       <c r="AR76" s="3"/>
       <c r="AS76" s="3"/>
     </row>
-    <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="201"/>
-      <c r="B77" s="327"/>
-      <c r="C77" s="329"/>
-      <c r="D77" s="261"/>
+    <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="326"/>
+      <c r="B77" s="198"/>
+      <c r="C77" s="200"/>
+      <c r="D77" s="242"/>
       <c r="E77" s="145"/>
       <c r="F77" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G77" s="316"/>
+      <c r="G77" s="231"/>
       <c r="H77" s="118"/>
       <c r="I77" s="118"/>
       <c r="J77" s="118"/>
@@ -7476,7 +7659,7 @@
       <c r="N77" s="118">
         <v>12</v>
       </c>
-      <c r="O77" s="347"/>
+      <c r="O77" s="188"/>
       <c r="P77" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7499,7 +7682,9 @@
       <c r="AF77" s="3"/>
       <c r="AG77" s="3"/>
       <c r="AH77" s="3"/>
-      <c r="AI77" s="3"/>
+      <c r="AI77" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="AJ77" s="3"/>
       <c r="AK77" s="3"/>
       <c r="AL77" s="3"/>
@@ -7511,14 +7696,14 @@
       <c r="AR77" s="3"/>
       <c r="AS77" s="3"/>
     </row>
-    <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="201"/>
-      <c r="B78" s="327"/>
-      <c r="C78" s="329"/>
-      <c r="D78" s="307"/>
-      <c r="E78" s="308"/>
-      <c r="F78" s="309"/>
-      <c r="G78" s="310"/>
+    <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="326"/>
+      <c r="B78" s="198"/>
+      <c r="C78" s="200"/>
+      <c r="D78" s="222"/>
+      <c r="E78" s="223"/>
+      <c r="F78" s="224"/>
+      <c r="G78" s="225"/>
       <c r="H78" s="112">
         <f>SUM(H74:H77)</f>
         <v>0</v>
@@ -7579,18 +7764,18 @@
       <c r="AR78" s="2"/>
       <c r="AS78" s="2"/>
     </row>
-    <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="201"/>
-      <c r="B79" s="327"/>
-      <c r="C79" s="329"/>
-      <c r="D79" s="323" t="s">
+    <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="326"/>
+      <c r="B79" s="198"/>
+      <c r="C79" s="200"/>
+      <c r="D79" s="238" t="s">
         <v>50</v>
       </c>
       <c r="E79" s="157"/>
       <c r="F79" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="G79" s="317">
+      <c r="G79" s="232">
         <v>48</v>
       </c>
       <c r="H79" s="159">
@@ -7602,7 +7787,7 @@
       <c r="L79" s="159"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
-      <c r="O79" s="350">
+      <c r="O79" s="191">
         <f>SUM(P79:P82)</f>
         <v>48</v>
       </c>
@@ -7634,8 +7819,8 @@
         <f>AG79/O79</f>
         <v>1</v>
       </c>
-      <c r="AI79" s="356" t="s">
-        <v>112</v>
+      <c r="AI79" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
@@ -7648,16 +7833,16 @@
       <c r="AR79" s="3"/>
       <c r="AS79" s="3"/>
     </row>
-    <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="201"/>
-      <c r="B80" s="327"/>
-      <c r="C80" s="329"/>
-      <c r="D80" s="324"/>
+    <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="326"/>
+      <c r="B80" s="198"/>
+      <c r="C80" s="200"/>
+      <c r="D80" s="239"/>
       <c r="E80" s="154"/>
       <c r="F80" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G80" s="318"/>
+      <c r="G80" s="233"/>
       <c r="H80" s="156">
         <v>12</v>
       </c>
@@ -7667,7 +7852,7 @@
       <c r="L80" s="156"/>
       <c r="M80" s="156"/>
       <c r="N80" s="156"/>
-      <c r="O80" s="351"/>
+      <c r="O80" s="192"/>
       <c r="P80" s="9">
         <f t="shared" ref="P80:P82" si="83">SUM(H80:N80)</f>
         <v>12</v>
@@ -7690,7 +7875,9 @@
       <c r="AF80" s="3"/>
       <c r="AG80" s="3"/>
       <c r="AH80" s="3"/>
-      <c r="AI80" s="3"/>
+      <c r="AI80" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
       <c r="AL80" s="3"/>
@@ -7702,16 +7889,16 @@
       <c r="AR80" s="3"/>
       <c r="AS80" s="3"/>
     </row>
-    <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="201"/>
-      <c r="B81" s="327"/>
-      <c r="C81" s="329"/>
-      <c r="D81" s="324"/>
+    <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="326"/>
+      <c r="B81" s="198"/>
+      <c r="C81" s="200"/>
+      <c r="D81" s="239"/>
       <c r="E81" s="154"/>
       <c r="F81" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G81" s="318"/>
+      <c r="G81" s="233"/>
       <c r="H81" s="156">
         <v>12</v>
       </c>
@@ -7721,7 +7908,7 @@
       <c r="L81" s="156"/>
       <c r="M81" s="156"/>
       <c r="N81" s="156"/>
-      <c r="O81" s="351"/>
+      <c r="O81" s="192"/>
       <c r="P81" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7744,7 +7931,9 @@
       <c r="AF81" s="3"/>
       <c r="AG81" s="3"/>
       <c r="AH81" s="3"/>
-      <c r="AI81" s="3"/>
+      <c r="AI81" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
       <c r="AL81" s="3"/>
@@ -7756,16 +7945,16 @@
       <c r="AR81" s="3"/>
       <c r="AS81" s="3"/>
     </row>
-    <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="201"/>
-      <c r="B82" s="327"/>
-      <c r="C82" s="329"/>
-      <c r="D82" s="324"/>
+    <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="326"/>
+      <c r="B82" s="198"/>
+      <c r="C82" s="200"/>
+      <c r="D82" s="239"/>
       <c r="E82" s="154"/>
       <c r="F82" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="G82" s="318"/>
+      <c r="G82" s="233"/>
       <c r="H82" s="156">
         <v>12</v>
       </c>
@@ -7775,7 +7964,7 @@
       <c r="L82" s="156"/>
       <c r="M82" s="156"/>
       <c r="N82" s="156"/>
-      <c r="O82" s="351"/>
+      <c r="O82" s="192"/>
       <c r="P82" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7798,7 +7987,9 @@
       <c r="AF82" s="3"/>
       <c r="AG82" s="3"/>
       <c r="AH82" s="3"/>
-      <c r="AI82" s="3"/>
+      <c r="AI82" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
       <c r="AL82" s="3"/>
@@ -7810,14 +8001,14 @@
       <c r="AR82" s="3"/>
       <c r="AS82" s="3"/>
     </row>
-    <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="201"/>
-      <c r="B83" s="327"/>
-      <c r="C83" s="329"/>
-      <c r="D83" s="311"/>
-      <c r="E83" s="312"/>
-      <c r="F83" s="312"/>
-      <c r="G83" s="312"/>
+    <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="326"/>
+      <c r="B83" s="198"/>
+      <c r="C83" s="200"/>
+      <c r="D83" s="226"/>
+      <c r="E83" s="227"/>
+      <c r="F83" s="227"/>
+      <c r="G83" s="227"/>
       <c r="H83" s="160">
         <f>SUM(H79:H82)</f>
         <v>48</v>
@@ -7878,18 +8069,18 @@
       <c r="AR83" s="2"/>
       <c r="AS83" s="2"/>
     </row>
-    <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="201"/>
-      <c r="B84" s="327"/>
-      <c r="C84" s="330"/>
-      <c r="D84" s="321" t="s">
+    <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="326"/>
+      <c r="B84" s="198"/>
+      <c r="C84" s="201"/>
+      <c r="D84" s="236" t="s">
         <v>51</v>
       </c>
       <c r="E84" s="125"/>
       <c r="F84" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="319">
+      <c r="G84" s="234">
         <v>48</v>
       </c>
       <c r="H84" s="126"/>
@@ -7901,7 +8092,7 @@
       <c r="L84" s="126"/>
       <c r="M84" s="126"/>
       <c r="N84" s="126"/>
-      <c r="O84" s="348">
+      <c r="O84" s="189">
         <f>SUM(P84:P87)</f>
         <v>48</v>
       </c>
@@ -7933,8 +8124,8 @@
         <f>AG84/O84</f>
         <v>1</v>
       </c>
-      <c r="AI84" s="356" t="s">
-        <v>112</v>
+      <c r="AI84" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="AJ84" s="3"/>
       <c r="AK84" s="3"/>
@@ -7947,16 +8138,16 @@
       <c r="AR84" s="3"/>
       <c r="AS84" s="3"/>
     </row>
-    <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="201"/>
-      <c r="B85" s="327"/>
-      <c r="C85" s="330"/>
-      <c r="D85" s="322"/>
+    <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="326"/>
+      <c r="B85" s="198"/>
+      <c r="C85" s="201"/>
+      <c r="D85" s="237"/>
       <c r="E85" s="123"/>
       <c r="F85" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="G85" s="320"/>
+      <c r="G85" s="235"/>
       <c r="H85" s="124"/>
       <c r="I85" s="124">
         <v>12</v>
@@ -7966,7 +8157,7 @@
       <c r="L85" s="124"/>
       <c r="M85" s="124"/>
       <c r="N85" s="124"/>
-      <c r="O85" s="349"/>
+      <c r="O85" s="190"/>
       <c r="P85" s="9">
         <f t="shared" ref="P85:P87" si="90">SUM(H85:N85)</f>
         <v>12</v>
@@ -7987,9 +8178,11 @@
       <c r="AD85" s="3"/>
       <c r="AE85" s="3"/>
       <c r="AF85" s="3"/>
-      <c r="AG85" s="358"/>
+      <c r="AG85" s="3"/>
       <c r="AH85" s="3"/>
-      <c r="AI85" s="3"/>
+      <c r="AI85" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="AJ85" s="3"/>
       <c r="AK85" s="3"/>
       <c r="AL85" s="3"/>
@@ -8001,16 +8194,16 @@
       <c r="AR85" s="3"/>
       <c r="AS85" s="3"/>
     </row>
-    <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="201"/>
-      <c r="B86" s="327"/>
-      <c r="C86" s="330"/>
-      <c r="D86" s="322"/>
+    <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="326"/>
+      <c r="B86" s="198"/>
+      <c r="C86" s="201"/>
+      <c r="D86" s="237"/>
       <c r="E86" s="123"/>
       <c r="F86" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="320"/>
+      <c r="G86" s="235"/>
       <c r="H86" s="124"/>
       <c r="I86" s="124">
         <v>12</v>
@@ -8020,7 +8213,7 @@
       <c r="L86" s="124"/>
       <c r="M86" s="124"/>
       <c r="N86" s="124"/>
-      <c r="O86" s="349"/>
+      <c r="O86" s="190"/>
       <c r="P86" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8043,7 +8236,9 @@
       <c r="AF86" s="3"/>
       <c r="AG86" s="3"/>
       <c r="AH86" s="3"/>
-      <c r="AI86" s="3"/>
+      <c r="AI86" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="AJ86" s="3"/>
       <c r="AK86" s="3"/>
       <c r="AL86" s="3"/>
@@ -8055,16 +8250,16 @@
       <c r="AR86" s="3"/>
       <c r="AS86" s="3"/>
     </row>
-    <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="202"/>
-      <c r="B87" s="327"/>
-      <c r="C87" s="330"/>
-      <c r="D87" s="322"/>
+    <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="327"/>
+      <c r="B87" s="198"/>
+      <c r="C87" s="201"/>
+      <c r="D87" s="237"/>
       <c r="E87" s="123"/>
       <c r="F87" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="320"/>
+      <c r="G87" s="235"/>
       <c r="H87" s="124"/>
       <c r="I87" s="124">
         <v>12</v>
@@ -8074,7 +8269,7 @@
       <c r="L87" s="124"/>
       <c r="M87" s="124"/>
       <c r="N87" s="124"/>
-      <c r="O87" s="349"/>
+      <c r="O87" s="190"/>
       <c r="P87" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8097,7 +8292,9 @@
       <c r="AF87" s="3"/>
       <c r="AG87" s="3"/>
       <c r="AH87" s="3"/>
-      <c r="AI87" s="3"/>
+      <c r="AI87" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="AJ87" s="3"/>
       <c r="AK87" s="3"/>
       <c r="AL87" s="3"/>
@@ -8109,14 +8306,14 @@
       <c r="AR87" s="3"/>
       <c r="AS87" s="3"/>
     </row>
-    <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
-      <c r="B88" s="327"/>
-      <c r="C88" s="330"/>
-      <c r="D88" s="313"/>
-      <c r="E88" s="314"/>
-      <c r="F88" s="314"/>
-      <c r="G88" s="314"/>
+      <c r="B88" s="198"/>
+      <c r="C88" s="201"/>
+      <c r="D88" s="228"/>
+      <c r="E88" s="229"/>
+      <c r="F88" s="229"/>
+      <c r="G88" s="229"/>
       <c r="H88" s="162">
         <f>SUM(H84:H87)</f>
         <v>0</v>
@@ -8177,10 +8374,10 @@
       <c r="AR88" s="2"/>
       <c r="AS88" s="2"/>
     </row>
-    <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
-      <c r="B89" s="327"/>
-      <c r="C89" s="330"/>
+      <c r="B89" s="198"/>
+      <c r="C89" s="201"/>
       <c r="D89" s="122" t="s">
         <v>17</v>
       </c>
@@ -8232,7 +8429,7 @@
         <f>AG89/O89</f>
         <v>1</v>
       </c>
-      <c r="AI89" s="356" t="s">
+      <c r="AI89" s="3" t="s">
         <v>112</v>
       </c>
       <c r="AJ89" s="3"/>
@@ -8246,14 +8443,14 @@
       <c r="AR89" s="3"/>
       <c r="AS89" s="3"/>
     </row>
-    <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
-      <c r="B90" s="327"/>
-      <c r="C90" s="330"/>
-      <c r="D90" s="196"/>
-      <c r="E90" s="304"/>
-      <c r="F90" s="304"/>
-      <c r="G90" s="304"/>
+      <c r="B90" s="198"/>
+      <c r="C90" s="201"/>
+      <c r="D90" s="218"/>
+      <c r="E90" s="219"/>
+      <c r="F90" s="219"/>
+      <c r="G90" s="219"/>
       <c r="H90" s="140">
         <f t="shared" ref="H90:N90" si="97">SUM(H89:H89)</f>
         <v>48</v>
@@ -8314,7 +8511,7 @@
       <c r="AR90" s="2"/>
       <c r="AS90" s="2"/>
     </row>
-    <row r="91" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H91" s="164">
         <f t="shared" ref="H91:N91" si="98">SUM(H6+H11+H16+H21+H26+H31+H36+H41+H46+H51+H56+H61+H66+H73+H78+H83+H88+H90)</f>
         <v>480</v>
@@ -8349,7 +8546,7 @@
       </c>
       <c r="Q91" s="121"/>
     </row>
-    <row r="93" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="H93" s="166">
         <f t="shared" ref="H93:N93" si="99">IF(H91=0,"SIN HORAS",432-H91)</f>
         <v>-48</v>
@@ -8378,93 +8575,33 @@
         <f t="shared" si="99"/>
         <v>-48</v>
       </c>
-      <c r="AI93" s="357"/>
-    </row>
-    <row r="97" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H97" s="303" t="s">
+    </row>
+    <row r="97" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="H97" s="202" t="s">
         <v>104</v>
       </c>
-      <c r="I97" s="303"/>
-      <c r="J97" s="303"/>
-    </row>
-    <row r="99" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="I99" s="303" t="s">
+      <c r="I97" s="202"/>
+      <c r="J97" s="202"/>
+    </row>
+    <row r="99" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="I99" s="202" t="s">
         <v>105</v>
       </c>
-      <c r="J99" s="303"/>
-      <c r="K99" s="303"/>
-      <c r="L99" s="303"/>
-    </row>
-    <row r="101" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="K101" s="303" t="s">
+      <c r="J99" s="202"/>
+      <c r="K99" s="202"/>
+      <c r="L99" s="202"/>
+    </row>
+    <row r="101" spans="8:14" x14ac:dyDescent="0.3">
+      <c r="K101" s="202" t="s">
         <v>106</v>
       </c>
-      <c r="L101" s="303"/>
-      <c r="M101" s="303"/>
-      <c r="N101" s="303"/>
+      <c r="L101" s="202"/>
+      <c r="M101" s="202"/>
+      <c r="N101" s="202"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS91" xr:uid="{44B9DB88-0080-4900-9B58-5C638DC6AAB3}"/>
   <mergeCells count="75">
-    <mergeCell ref="O74:O77"/>
-    <mergeCell ref="O84:O87"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="O67:O72"/>
-    <mergeCell ref="B2:B90"/>
-    <mergeCell ref="C2:C90"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="K101:N101"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="O32:O35"/>
-    <mergeCell ref="O37:O40"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O52:O55"/>
-    <mergeCell ref="O57:O60"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="G12:G15"/>
     <mergeCell ref="D17:D20"/>
@@ -8481,6 +8618,65 @@
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="G37:G40"/>
     <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O52:O55"/>
+    <mergeCell ref="O57:O60"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="O32:O35"/>
+    <mergeCell ref="O37:O40"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="B2:B90"/>
+    <mergeCell ref="C2:C90"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="O74:O77"/>
+    <mergeCell ref="O84:O87"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="O67:O72"/>
   </mergeCells>
   <conditionalFormatting sqref="H93:N93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Cambios en la licencia de EPPlus
</commit_message>
<xml_diff>
--- a/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
+++ b/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1234\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8EB1A3-61D5-4E01-8979-F67FC9E6B9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10042F2-5D60-4AB8-AEFA-AC9BAA4DD0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="178">
   <si>
     <t>DENOMINACION</t>
   </si>
@@ -376,50 +376,209 @@
     <t>INSTRUCTOR</t>
   </si>
   <si>
-    <t>LUIS F GARCIA</t>
-  </si>
-  <si>
-    <t>BEATRIZ ALFARO</t>
-  </si>
-  <si>
-    <t>ANEDIA GONZALEZ</t>
-  </si>
-  <si>
-    <t>DAVID ARRIETA</t>
-  </si>
-  <si>
-    <t>FERNANDO FLOREZ</t>
-  </si>
-  <si>
     <t>PILAR PRADA</t>
   </si>
   <si>
-    <t>LUIS PEREZ</t>
-  </si>
-  <si>
-    <t>YOVANNI URREGO</t>
-  </si>
-  <si>
-    <t>OSMEIDA RAMIREZ</t>
-  </si>
-  <si>
-    <t>ANDRES MARQUEZ</t>
-  </si>
-  <si>
-    <t>LUZ E CARRIAZO</t>
-  </si>
-  <si>
-    <t>JORGE VASQUEZ</t>
-  </si>
-  <si>
-    <t>ENADITH HERNANDEZ</t>
+    <t>MARRUGO LEYVA  WILLIAM</t>
+  </si>
+  <si>
+    <t>BOSSIO CASTRO EUGENIO LUCIO</t>
+  </si>
+  <si>
+    <t>GONZALEZ VELILLA RICHARD MANUEL</t>
+  </si>
+  <si>
+    <t>MARIMON MATURANA JASIR ALBERTO</t>
+  </si>
+  <si>
+    <t>PASTRANA MERCADO MANUEL DE JESUS</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ DOMINGUEZ JAIRO ENRIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMERO OSPINO MANUEL </t>
+  </si>
+  <si>
+    <t>GARCIA DIAZ LUIS FERNANDO</t>
+  </si>
+  <si>
+    <t>NIETO VARGAS JAIRO RAMÓN</t>
+  </si>
+  <si>
+    <t>OBANDO LOBO  HOLGER ENRIQUE</t>
+  </si>
+  <si>
+    <t>UPARELA OSPINO YONHYS</t>
+  </si>
+  <si>
+    <t>OVIEDO VILLERO JUAN FRANCISCO</t>
+  </si>
+  <si>
+    <t>MARTELO CHING RONALD</t>
+  </si>
+  <si>
+    <t>BENJUMEA ACUÑA NILSON</t>
+  </si>
+  <si>
+    <t>PADILLA RODRIGUEZ JULIO CÉSAR</t>
+  </si>
+  <si>
+    <t>HERNÁNDEZ FLÓREZ MARIO ALBERTO</t>
+  </si>
+  <si>
+    <t>SEVERICHE TORREGROZA JORGE ELIECER</t>
+  </si>
+  <si>
+    <t>LASTRE GOMEZ HEDIER HUMBERTO</t>
+  </si>
+  <si>
+    <t>VEGA LIZCANO JOSE LUIS</t>
+  </si>
+  <si>
+    <t>OSPINO OLIVEROS JAIRO</t>
+  </si>
+  <si>
+    <t>VASQUEZ RUEDA ALVARO JOSE</t>
+  </si>
+  <si>
+    <t>NUÑEZ CAMPO ENRIQUETA DEL SOCORRO</t>
+  </si>
+  <si>
+    <t>SOLAR ARREDONDO DORAIDA NAYARITH</t>
+  </si>
+  <si>
+    <t>CASTAÑO OSORIO BIBIANA</t>
+  </si>
+  <si>
+    <t>MANCILLA DIAZ TATIANA</t>
+  </si>
+  <si>
+    <t>MEZA TATIS NADIA ACELA</t>
+  </si>
+  <si>
+    <t>MANOTAS CUELLO MARTA DE JESUS</t>
+  </si>
+  <si>
+    <t>RAMIREZ BALLESTA OSMEIDA DEL CARMEN</t>
+  </si>
+  <si>
+    <t>PÉREZ CORREA MARISTELA</t>
+  </si>
+  <si>
+    <t>BENITEZ OROZCO KAREN PAOLA</t>
+  </si>
+  <si>
+    <t>CARRASCAL GONZALEZ DILIA BERTA</t>
+  </si>
+  <si>
+    <t>CABRALES GUARDO MARA SOFIA</t>
+  </si>
+  <si>
+    <t>ROMERO BUCIGO VANESSA JUDITH</t>
+  </si>
+  <si>
+    <t>HERNANDEZ SALGADO ATILIO MANUEL</t>
+  </si>
+  <si>
+    <t>BARROS CHAPARRO DAVID JESUS</t>
+  </si>
+  <si>
+    <t>VÉLEZ GENES MARCO ANTONIO</t>
+  </si>
+  <si>
+    <t>GOMEZ PEREZ WAGNER STEVEN</t>
+  </si>
+  <si>
+    <t>VILLALOBOS DE AVILA HILDEBERTO</t>
+  </si>
+  <si>
+    <t>DE POMBO BETTIN JOSE IGNACIO</t>
+  </si>
+  <si>
+    <t>JULIO DIAZ FREDY</t>
+  </si>
+  <si>
+    <t>HOYOS HOYOS  MARCELIANO JOSE</t>
+  </si>
+  <si>
+    <t>ACOSTA TREJOS ALFONSO MARIA</t>
+  </si>
+  <si>
+    <t>HERRERA ESPINOSA  IVAN</t>
+  </si>
+  <si>
+    <t>LICERO ARZUZA NICOLAS RAFAEL</t>
+  </si>
+  <si>
+    <t>VILLANUEVA VILLARREAL JORGE ALBERTO</t>
+  </si>
+  <si>
+    <t>CUESTA PEREZ  CARLOS</t>
+  </si>
+  <si>
+    <t>BELENO CALDERON JAIRO ERNESTO</t>
+  </si>
+  <si>
+    <t>RUIZ GARIZADO ARNULFO</t>
+  </si>
+  <si>
+    <t>VELEZ CANTILLO NELSON ENRIQUE</t>
+  </si>
+  <si>
+    <t>AGUILERA AURELA ARODIZ</t>
+  </si>
+  <si>
+    <t>MASTRASCUSA TOVAR MARCELO ANTONIO</t>
+  </si>
+  <si>
+    <t>TORRES AGUAS ALEXIS JOSE</t>
+  </si>
+  <si>
+    <t>TORRES SARA  GERLIN HERNANDO</t>
+  </si>
+  <si>
+    <t>SALGADO SIERRA  FELIPE MIGUEL</t>
+  </si>
+  <si>
+    <t>TORRES PALOMINO  FIDEL</t>
+  </si>
+  <si>
+    <t>URREGO PEÑA YOVANNI</t>
+  </si>
+  <si>
+    <t>DIAZ FORERO HERNANDO</t>
+  </si>
+  <si>
+    <t>SABALZA JIMENEZ CARLOS ENRIQUE</t>
+  </si>
+  <si>
+    <t>FLOREZ ARRIETA FERNANDO JAVIER</t>
+  </si>
+  <si>
+    <t>NUÑEZ GOMEZ JAN CARLOS</t>
+  </si>
+  <si>
+    <t>ARIAS CORONEL ERIK JOSÉ</t>
+  </si>
+  <si>
+    <t>MANOSALVA PORRAS LAURA JULIANA</t>
+  </si>
+  <si>
+    <t>ARRIETA ROJANO ANGEL DE JESUS</t>
+  </si>
+  <si>
+    <t>ROJAS GONZALEZ YEIMY CATALINA</t>
+  </si>
+  <si>
+    <t>MALLARINO MIRANDA CLARIBEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +660,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1243,7 +1409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="362">
+  <cellXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1801,54 +1967,415 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1894,81 +2421,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1987,120 +2439,6 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2122,208 +2460,42 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,11 +2845,11 @@
   <dimension ref="A1:AS101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="AG5" sqref="AG5"/>
+      <selection pane="bottomRight" activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2798,16 +2970,16 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="325" t="s">
+      <c r="A2" s="206" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="197">
+      <c r="B2" s="319">
         <v>228183</v>
       </c>
-      <c r="C2" s="199">
+      <c r="C2" s="321">
         <v>2</v>
       </c>
-      <c r="D2" s="328" t="s">
+      <c r="D2" s="209" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
@@ -2816,7 +2988,7 @@
       <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="331">
+      <c r="G2" s="212">
         <v>528</v>
       </c>
       <c r="H2" s="12"/>
@@ -2828,7 +3000,7 @@
       <c r="N2" s="12">
         <v>72</v>
       </c>
-      <c r="O2" s="275">
+      <c r="O2" s="272">
         <f>SUM(P2:P5)</f>
         <v>528</v>
       </c>
@@ -2895,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
@@ -2908,18 +3080,18 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
     </row>
-    <row r="3" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="326"/>
-      <c r="B3" s="198"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="329"/>
+    <row r="3" spans="1:45" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="207"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="210"/>
       <c r="E3" s="13">
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="332"/>
+      <c r="G3" s="213"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -2929,7 +3101,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="276"/>
+      <c r="O3" s="273"/>
       <c r="P3" s="9">
         <f>SUM(H3:N3)</f>
         <v>64</v>
@@ -2953,7 +3125,7 @@
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
@@ -2966,18 +3138,18 @@
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
     </row>
-    <row r="4" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="326"/>
-      <c r="B4" s="198"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="329"/>
+    <row r="4" spans="1:45" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="207"/>
+      <c r="B4" s="320"/>
+      <c r="C4" s="322"/>
+      <c r="D4" s="210"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="332"/>
+      <c r="G4" s="213"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -2987,7 +3159,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="276"/>
+      <c r="O4" s="273"/>
       <c r="P4" s="9">
         <f>SUM(H4:N4)</f>
         <v>80</v>
@@ -3011,7 +3183,7 @@
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
@@ -3025,17 +3197,17 @@
       <c r="AS4" s="2"/>
     </row>
     <row r="5" spans="1:45" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="326"/>
-      <c r="B5" s="198"/>
-      <c r="C5" s="200"/>
-      <c r="D5" s="330"/>
+      <c r="A5" s="207"/>
+      <c r="B5" s="320"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="211"/>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="333"/>
+      <c r="G5" s="214"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -3049,7 +3221,7 @@
       <c r="N5" s="18">
         <v>168</v>
       </c>
-      <c r="O5" s="277"/>
+      <c r="O5" s="274"/>
       <c r="P5" s="9">
         <f>SUM(H5:N5)</f>
         <v>312</v>
@@ -3073,7 +3245,7 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
@@ -3087,13 +3259,13 @@
       <c r="AS5" s="2"/>
     </row>
     <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="326"/>
-      <c r="B6" s="198"/>
-      <c r="C6" s="200"/>
-      <c r="D6" s="203"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="205"/>
+      <c r="A6" s="207"/>
+      <c r="B6" s="320"/>
+      <c r="C6" s="322"/>
+      <c r="D6" s="324"/>
+      <c r="E6" s="325"/>
+      <c r="F6" s="325"/>
+      <c r="G6" s="326"/>
       <c r="H6" s="56">
         <f>SUM(H2:H5)</f>
         <v>0</v>
@@ -3155,10 +3327,10 @@
       <c r="AS6" s="2"/>
     </row>
     <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="326"/>
-      <c r="B7" s="198"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="334" t="s">
+      <c r="A7" s="207"/>
+      <c r="B7" s="320"/>
+      <c r="C7" s="322"/>
+      <c r="D7" s="221" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="19">
@@ -3167,7 +3339,7 @@
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="337">
+      <c r="G7" s="224">
         <v>384</v>
       </c>
       <c r="H7" s="25"/>
@@ -3179,7 +3351,7 @@
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="278">
+      <c r="O7" s="275">
         <f>SUM(P7:P10)</f>
         <v>384</v>
       </c>
@@ -3246,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
@@ -3260,17 +3432,17 @@
       <c r="AS7" s="3"/>
     </row>
     <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="326"/>
-      <c r="B8" s="198"/>
-      <c r="C8" s="200"/>
-      <c r="D8" s="335"/>
+      <c r="A8" s="207"/>
+      <c r="B8" s="320"/>
+      <c r="C8" s="322"/>
+      <c r="D8" s="222"/>
       <c r="E8" s="21">
         <v>3</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="338"/>
+      <c r="G8" s="225"/>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
@@ -3280,7 +3452,7 @@
         <v>144</v>
       </c>
       <c r="N8" s="26"/>
-      <c r="O8" s="279"/>
+      <c r="O8" s="276"/>
       <c r="P8" s="9">
         <f t="shared" ref="P8:P10" si="1">SUM(H8:N8)</f>
         <v>144</v>
@@ -3304,7 +3476,7 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
@@ -3318,17 +3490,17 @@
       <c r="AS8" s="3"/>
     </row>
     <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="326"/>
-      <c r="B9" s="198"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="335"/>
+      <c r="A9" s="207"/>
+      <c r="B9" s="320"/>
+      <c r="C9" s="322"/>
+      <c r="D9" s="222"/>
       <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="338"/>
+      <c r="G9" s="225"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -3338,7 +3510,7 @@
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="279"/>
+      <c r="O9" s="276"/>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3362,7 +3534,7 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
@@ -3376,17 +3548,17 @@
       <c r="AS9" s="3"/>
     </row>
     <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="326"/>
-      <c r="B10" s="198"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="336"/>
+      <c r="A10" s="207"/>
+      <c r="B10" s="320"/>
+      <c r="C10" s="322"/>
+      <c r="D10" s="223"/>
       <c r="E10" s="23">
         <v>4</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="339"/>
+      <c r="G10" s="226"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -3396,7 +3568,7 @@
       <c r="N10" s="27">
         <v>96</v>
       </c>
-      <c r="O10" s="280"/>
+      <c r="O10" s="277"/>
       <c r="P10" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3420,7 +3592,7 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
@@ -3434,13 +3606,13 @@
       <c r="AS10" s="3"/>
     </row>
     <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="326"/>
-      <c r="B11" s="198"/>
-      <c r="C11" s="200"/>
-      <c r="D11" s="206"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="207"/>
-      <c r="G11" s="208"/>
+      <c r="A11" s="207"/>
+      <c r="B11" s="320"/>
+      <c r="C11" s="322"/>
+      <c r="D11" s="327"/>
+      <c r="E11" s="328"/>
+      <c r="F11" s="328"/>
+      <c r="G11" s="329"/>
       <c r="H11" s="61">
         <f>SUM(H7:H10)</f>
         <v>0</v>
@@ -3502,17 +3674,17 @@
       <c r="AS11" s="2"/>
     </row>
     <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="326"/>
-      <c r="B12" s="198"/>
-      <c r="C12" s="200"/>
-      <c r="D12" s="258" t="s">
+      <c r="A12" s="207"/>
+      <c r="B12" s="320"/>
+      <c r="C12" s="322"/>
+      <c r="D12" s="194" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="261">
+      <c r="G12" s="197">
         <v>48</v>
       </c>
       <c r="H12" s="34">
@@ -3524,7 +3696,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="255">
+      <c r="O12" s="278">
         <f t="shared" ref="O12" si="3">SUM(P12:P15)</f>
         <v>48</v>
       </c>
@@ -3573,33 +3745,33 @@
         <f>O12-AC12</f>
         <v>48</v>
       </c>
-      <c r="AE12" s="360">
+      <c r="AE12" s="192">
         <f>AD12/O12</f>
         <v>1</v>
       </c>
       <c r="AF12" s="179"/>
-      <c r="AG12" s="355">
+      <c r="AG12" s="187">
         <f>O12-AF12</f>
         <v>48</v>
       </c>
-      <c r="AH12" s="356">
+      <c r="AH12" s="188">
         <f>AG12/O12</f>
         <v>1</v>
       </c>
-      <c r="AI12" s="357" t="s">
-        <v>112</v>
+      <c r="AI12" s="189" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="326"/>
-      <c r="B13" s="198"/>
-      <c r="C13" s="200"/>
-      <c r="D13" s="259"/>
+      <c r="A13" s="207"/>
+      <c r="B13" s="320"/>
+      <c r="C13" s="322"/>
+      <c r="D13" s="195"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="262"/>
+      <c r="G13" s="198"/>
       <c r="H13" s="35">
         <v>12</v>
       </c>
@@ -3609,7 +3781,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="256"/>
+      <c r="O13" s="279"/>
       <c r="P13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3628,24 +3800,24 @@
       <c r="AB13" s="178"/>
       <c r="AC13" s="179"/>
       <c r="AD13" s="179"/>
-      <c r="AE13" s="361"/>
+      <c r="AE13" s="193"/>
       <c r="AF13" s="179"/>
       <c r="AG13" s="179"/>
       <c r="AH13" s="179"/>
-      <c r="AI13" s="357" t="s">
-        <v>112</v>
+      <c r="AI13" s="189" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="326"/>
-      <c r="B14" s="198"/>
-      <c r="C14" s="200"/>
-      <c r="D14" s="259"/>
+      <c r="A14" s="207"/>
+      <c r="B14" s="320"/>
+      <c r="C14" s="322"/>
+      <c r="D14" s="195"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="262"/>
+      <c r="G14" s="198"/>
       <c r="H14" s="35">
         <v>12</v>
       </c>
@@ -3655,7 +3827,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="256"/>
+      <c r="O14" s="279"/>
       <c r="P14" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3674,24 +3846,24 @@
       <c r="AB14" s="178"/>
       <c r="AC14" s="179"/>
       <c r="AD14" s="179"/>
-      <c r="AE14" s="361"/>
+      <c r="AE14" s="193"/>
       <c r="AF14" s="179"/>
       <c r="AG14" s="179"/>
       <c r="AH14" s="179"/>
-      <c r="AI14" s="357" t="s">
-        <v>112</v>
+      <c r="AI14" s="189" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="326"/>
-      <c r="B15" s="198"/>
-      <c r="C15" s="200"/>
-      <c r="D15" s="260"/>
+      <c r="A15" s="207"/>
+      <c r="B15" s="320"/>
+      <c r="C15" s="322"/>
+      <c r="D15" s="196"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="263"/>
+      <c r="G15" s="199"/>
       <c r="H15" s="36">
         <v>12</v>
       </c>
@@ -3701,7 +3873,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="257"/>
+      <c r="O15" s="280"/>
       <c r="P15" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3720,22 +3892,22 @@
       <c r="AB15" s="178"/>
       <c r="AC15" s="179"/>
       <c r="AD15" s="179"/>
-      <c r="AE15" s="361"/>
+      <c r="AE15" s="193"/>
       <c r="AF15" s="179"/>
       <c r="AG15" s="179"/>
       <c r="AH15" s="179"/>
-      <c r="AI15" s="357" t="s">
-        <v>112</v>
+      <c r="AI15" s="189" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="326"/>
-      <c r="B16" s="198"/>
-      <c r="C16" s="200"/>
-      <c r="D16" s="203"/>
-      <c r="E16" s="204"/>
-      <c r="F16" s="204"/>
-      <c r="G16" s="205"/>
+      <c r="A16" s="207"/>
+      <c r="B16" s="320"/>
+      <c r="C16" s="322"/>
+      <c r="D16" s="324"/>
+      <c r="E16" s="325"/>
+      <c r="F16" s="325"/>
+      <c r="G16" s="326"/>
       <c r="H16" s="56">
         <f>SUM(H12:H15)</f>
         <v>48</v>
@@ -3797,17 +3969,17 @@
       <c r="AS16" s="2"/>
     </row>
     <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="326"/>
-      <c r="B17" s="198"/>
-      <c r="C17" s="200"/>
-      <c r="D17" s="320" t="s">
+      <c r="A17" s="207"/>
+      <c r="B17" s="320"/>
+      <c r="C17" s="322"/>
+      <c r="D17" s="200" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="322">
+      <c r="G17" s="203">
         <v>48</v>
       </c>
       <c r="H17" s="44"/>
@@ -3882,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="AI17" s="3" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
@@ -3896,15 +4068,15 @@
       <c r="AS17" s="3"/>
     </row>
     <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="326"/>
-      <c r="B18" s="198"/>
-      <c r="C18" s="200"/>
-      <c r="D18" s="321"/>
+      <c r="A18" s="207"/>
+      <c r="B18" s="320"/>
+      <c r="C18" s="322"/>
+      <c r="D18" s="201"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="323"/>
+      <c r="G18" s="204"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45">
         <v>12</v>
@@ -3938,7 +4110,7 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
@@ -3952,15 +4124,15 @@
       <c r="AS18" s="3"/>
     </row>
     <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="326"/>
-      <c r="B19" s="198"/>
-      <c r="C19" s="200"/>
-      <c r="D19" s="321"/>
+      <c r="A19" s="207"/>
+      <c r="B19" s="320"/>
+      <c r="C19" s="322"/>
+      <c r="D19" s="201"/>
       <c r="E19" s="39"/>
       <c r="F19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="323"/>
+      <c r="G19" s="204"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45">
         <v>12</v>
@@ -3994,7 +4166,7 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
@@ -4008,15 +4180,15 @@
       <c r="AS19" s="3"/>
     </row>
     <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="326"/>
-      <c r="B20" s="198"/>
-      <c r="C20" s="200"/>
-      <c r="D20" s="218"/>
+      <c r="A20" s="207"/>
+      <c r="B20" s="320"/>
+      <c r="C20" s="322"/>
+      <c r="D20" s="202"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="324"/>
+      <c r="G20" s="205"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46">
         <v>12</v>
@@ -4050,7 +4222,7 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
@@ -4064,13 +4236,13 @@
       <c r="AS20" s="3"/>
     </row>
     <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="326"/>
-      <c r="B21" s="198"/>
-      <c r="C21" s="200"/>
-      <c r="D21" s="209"/>
-      <c r="E21" s="210"/>
-      <c r="F21" s="210"/>
-      <c r="G21" s="211"/>
+      <c r="A21" s="207"/>
+      <c r="B21" s="320"/>
+      <c r="C21" s="322"/>
+      <c r="D21" s="330"/>
+      <c r="E21" s="331"/>
+      <c r="F21" s="331"/>
+      <c r="G21" s="332"/>
       <c r="H21" s="62">
         <f>SUM(H17:H20)</f>
         <v>0</v>
@@ -4131,11 +4303,11 @@
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
     </row>
-    <row r="22" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="326"/>
-      <c r="B22" s="198"/>
-      <c r="C22" s="200"/>
-      <c r="D22" s="317" t="s">
+    <row r="22" spans="1:45" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="207"/>
+      <c r="B22" s="320"/>
+      <c r="C22" s="322"/>
+      <c r="D22" s="215" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="47">
@@ -4144,7 +4316,7 @@
       <c r="F22" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="305">
+      <c r="G22" s="218">
         <v>336</v>
       </c>
       <c r="H22" s="53"/>
@@ -4154,7 +4326,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="53"/>
       <c r="N22" s="53"/>
-      <c r="O22" s="270">
+      <c r="O22" s="267">
         <f t="shared" ref="O22" si="13">SUM(P22:P25)</f>
         <v>336</v>
       </c>
@@ -4227,7 +4399,7 @@
         <v>1</v>
       </c>
       <c r="AI22" s="3" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
@@ -4240,18 +4412,18 @@
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
     </row>
-    <row r="23" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="326"/>
-      <c r="B23" s="198"/>
-      <c r="C23" s="200"/>
-      <c r="D23" s="318"/>
+    <row r="23" spans="1:45" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="207"/>
+      <c r="B23" s="320"/>
+      <c r="C23" s="322"/>
+      <c r="D23" s="216"/>
       <c r="E23" s="49">
         <v>2</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="306"/>
+      <c r="G23" s="219"/>
       <c r="H23" s="54">
         <v>72</v>
       </c>
@@ -4261,7 +4433,7 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="271"/>
+      <c r="O23" s="268"/>
       <c r="P23" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4285,7 +4457,7 @@
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
       <c r="AI23" s="3" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
@@ -4298,18 +4470,18 @@
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
     </row>
-    <row r="24" spans="1:45" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="326"/>
-      <c r="B24" s="198"/>
-      <c r="C24" s="200"/>
-      <c r="D24" s="318"/>
+    <row r="24" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="207"/>
+      <c r="B24" s="320"/>
+      <c r="C24" s="322"/>
+      <c r="D24" s="216"/>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="306"/>
+      <c r="G24" s="219"/>
       <c r="H24" s="54">
         <v>72</v>
       </c>
@@ -4319,7 +4491,7 @@
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
-      <c r="O24" s="271"/>
+      <c r="O24" s="268"/>
       <c r="P24" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4343,7 +4515,7 @@
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="3" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
@@ -4356,18 +4528,18 @@
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
     </row>
-    <row r="25" spans="1:45" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="326"/>
-      <c r="B25" s="198"/>
-      <c r="C25" s="200"/>
-      <c r="D25" s="319"/>
+    <row r="25" spans="1:45" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="207"/>
+      <c r="B25" s="320"/>
+      <c r="C25" s="322"/>
+      <c r="D25" s="217"/>
       <c r="E25" s="51">
         <v>3</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="307"/>
+      <c r="G25" s="220"/>
       <c r="H25" s="55"/>
       <c r="I25" s="55">
         <v>72</v>
@@ -4379,7 +4551,7 @@
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
-      <c r="O25" s="272"/>
+      <c r="O25" s="269"/>
       <c r="P25" s="9">
         <f t="shared" si="4"/>
         <v>192</v>
@@ -4403,7 +4575,7 @@
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="3" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
@@ -4417,13 +4589,13 @@
       <c r="AS25" s="3"/>
     </row>
     <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="326"/>
-      <c r="B26" s="198"/>
-      <c r="C26" s="200"/>
-      <c r="D26" s="212"/>
-      <c r="E26" s="213"/>
-      <c r="F26" s="213"/>
-      <c r="G26" s="214"/>
+      <c r="A26" s="207"/>
+      <c r="B26" s="320"/>
+      <c r="C26" s="322"/>
+      <c r="D26" s="333"/>
+      <c r="E26" s="334"/>
+      <c r="F26" s="334"/>
+      <c r="G26" s="335"/>
       <c r="H26" s="64">
         <f>SUM(H22:H25)</f>
         <v>144</v>
@@ -4485,10 +4657,10 @@
       <c r="AS26" s="2"/>
     </row>
     <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="326"/>
-      <c r="B27" s="198"/>
-      <c r="C27" s="200"/>
-      <c r="D27" s="352" t="s">
+      <c r="A27" s="207"/>
+      <c r="B27" s="320"/>
+      <c r="C27" s="322"/>
+      <c r="D27" s="239" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="65">
@@ -4497,7 +4669,7 @@
       <c r="F27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="340">
+      <c r="G27" s="227">
         <v>576</v>
       </c>
       <c r="H27" s="73"/>
@@ -4581,8 +4753,8 @@
         <f>AG27/O27</f>
         <v>1</v>
       </c>
-      <c r="AI27" s="3" t="s">
-        <v>112</v>
+      <c r="AI27" s="189" t="s">
+        <v>132</v>
       </c>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
@@ -4596,17 +4768,17 @@
       <c r="AS27" s="3"/>
     </row>
     <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="326"/>
-      <c r="B28" s="198"/>
-      <c r="C28" s="200"/>
-      <c r="D28" s="353"/>
+      <c r="A28" s="207"/>
+      <c r="B28" s="320"/>
+      <c r="C28" s="322"/>
+      <c r="D28" s="240"/>
       <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="341"/>
+      <c r="G28" s="228"/>
       <c r="H28" s="74"/>
       <c r="I28" s="74">
         <v>72</v>
@@ -4639,8 +4811,8 @@
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
-      <c r="AI28" s="3" t="s">
-        <v>112</v>
+      <c r="AI28" s="189" t="s">
+        <v>133</v>
       </c>
       <c r="AJ28" s="3"/>
       <c r="AK28" s="3"/>
@@ -4654,17 +4826,17 @@
       <c r="AS28" s="3"/>
     </row>
     <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="326"/>
-      <c r="B29" s="198"/>
-      <c r="C29" s="200"/>
-      <c r="D29" s="353"/>
+      <c r="A29" s="207"/>
+      <c r="B29" s="320"/>
+      <c r="C29" s="322"/>
+      <c r="D29" s="240"/>
       <c r="E29" s="67">
         <v>1</v>
       </c>
       <c r="F29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="341"/>
+      <c r="G29" s="228"/>
       <c r="H29" s="74">
         <v>72</v>
       </c>
@@ -4697,8 +4869,8 @@
       <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
-      <c r="AI29" s="3" t="s">
-        <v>112</v>
+      <c r="AI29" s="189" t="s">
+        <v>134</v>
       </c>
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
@@ -4712,17 +4884,17 @@
       <c r="AS29" s="3"/>
     </row>
     <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="326"/>
-      <c r="B30" s="198"/>
-      <c r="C30" s="200"/>
-      <c r="D30" s="354"/>
+      <c r="A30" s="207"/>
+      <c r="B30" s="320"/>
+      <c r="C30" s="322"/>
+      <c r="D30" s="241"/>
       <c r="E30" s="69">
         <v>3</v>
       </c>
       <c r="F30" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="342"/>
+      <c r="G30" s="229"/>
       <c r="H30" s="75"/>
       <c r="I30" s="75">
         <v>72</v>
@@ -4761,10 +4933,10 @@
       <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
-      <c r="AI30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ30" s="3"/>
+      <c r="AI30" s="189" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ30" s="362"/>
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
       <c r="AM30" s="3"/>
@@ -4776,13 +4948,13 @@
       <c r="AS30" s="3"/>
     </row>
     <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="326"/>
-      <c r="B31" s="198"/>
-      <c r="C31" s="200"/>
-      <c r="D31" s="215"/>
-      <c r="E31" s="216"/>
-      <c r="F31" s="216"/>
-      <c r="G31" s="217"/>
+      <c r="A31" s="207"/>
+      <c r="B31" s="320"/>
+      <c r="C31" s="322"/>
+      <c r="D31" s="336"/>
+      <c r="E31" s="337"/>
+      <c r="F31" s="337"/>
+      <c r="G31" s="338"/>
       <c r="H31" s="71">
         <f>SUM(H27:H30)</f>
         <v>72</v>
@@ -4831,7 +5003,7 @@
       <c r="AF31" s="120"/>
       <c r="AG31" s="120"/>
       <c r="AH31" s="120"/>
-      <c r="AI31" s="120"/>
+      <c r="AI31" s="189"/>
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="2"/>
@@ -4844,17 +5016,17 @@
       <c r="AS31" s="2"/>
     </row>
     <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="326"/>
-      <c r="B32" s="198"/>
-      <c r="C32" s="200"/>
-      <c r="D32" s="264" t="s">
+      <c r="A32" s="207"/>
+      <c r="B32" s="320"/>
+      <c r="C32" s="322"/>
+      <c r="D32" s="293" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="343">
+      <c r="G32" s="230">
         <v>48</v>
       </c>
       <c r="H32" s="82"/>
@@ -4866,7 +5038,7 @@
         <v>12</v>
       </c>
       <c r="N32" s="82"/>
-      <c r="O32" s="249">
+      <c r="O32" s="287">
         <f t="shared" ref="O32" si="27">SUM(P32:P35)</f>
         <v>48</v>
       </c>
@@ -4915,33 +5087,33 @@
         <f>O32-AC32</f>
         <v>48</v>
       </c>
-      <c r="AE32" s="360">
+      <c r="AE32" s="192">
         <f>AD32/O32</f>
         <v>1</v>
       </c>
       <c r="AF32" s="179"/>
-      <c r="AG32" s="355">
+      <c r="AG32" s="187">
         <f>O32-AF32</f>
         <v>48</v>
       </c>
-      <c r="AH32" s="356">
+      <c r="AH32" s="188">
         <f>AG32/O32</f>
         <v>1</v>
       </c>
-      <c r="AI32" s="357" t="s">
-        <v>119</v>
+      <c r="AI32" s="189" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="326"/>
-      <c r="B33" s="198"/>
-      <c r="C33" s="200"/>
-      <c r="D33" s="265"/>
+      <c r="A33" s="207"/>
+      <c r="B33" s="320"/>
+      <c r="C33" s="322"/>
+      <c r="D33" s="294"/>
       <c r="E33" s="78"/>
       <c r="F33" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="344"/>
+      <c r="G33" s="231"/>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -4951,7 +5123,7 @@
         <v>12</v>
       </c>
       <c r="N33" s="83"/>
-      <c r="O33" s="250"/>
+      <c r="O33" s="288"/>
       <c r="P33" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4970,24 +5142,24 @@
       <c r="AB33" s="178"/>
       <c r="AC33" s="179"/>
       <c r="AD33" s="179"/>
-      <c r="AE33" s="361"/>
+      <c r="AE33" s="193"/>
       <c r="AF33" s="179"/>
       <c r="AG33" s="179"/>
       <c r="AH33" s="179"/>
-      <c r="AI33" s="357" t="s">
-        <v>119</v>
+      <c r="AI33" s="189" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="326"/>
-      <c r="B34" s="198"/>
-      <c r="C34" s="200"/>
-      <c r="D34" s="265"/>
+      <c r="A34" s="207"/>
+      <c r="B34" s="320"/>
+      <c r="C34" s="322"/>
+      <c r="D34" s="294"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="344"/>
+      <c r="G34" s="231"/>
       <c r="H34" s="83"/>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -4997,7 +5169,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="83"/>
-      <c r="O34" s="250"/>
+      <c r="O34" s="288"/>
       <c r="P34" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5016,24 +5188,24 @@
       <c r="AB34" s="178"/>
       <c r="AC34" s="179"/>
       <c r="AD34" s="179"/>
-      <c r="AE34" s="361"/>
+      <c r="AE34" s="193"/>
       <c r="AF34" s="179"/>
       <c r="AG34" s="179"/>
       <c r="AH34" s="179"/>
-      <c r="AI34" s="357" t="s">
-        <v>119</v>
+      <c r="AI34" s="189" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="326"/>
-      <c r="B35" s="198"/>
-      <c r="C35" s="200"/>
-      <c r="D35" s="266"/>
+      <c r="A35" s="207"/>
+      <c r="B35" s="320"/>
+      <c r="C35" s="322"/>
+      <c r="D35" s="295"/>
       <c r="E35" s="80"/>
       <c r="F35" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="345"/>
+      <c r="G35" s="232"/>
       <c r="H35" s="84"/>
       <c r="I35" s="84"/>
       <c r="J35" s="84"/>
@@ -5043,7 +5215,7 @@
         <v>12</v>
       </c>
       <c r="N35" s="84"/>
-      <c r="O35" s="251"/>
+      <c r="O35" s="289"/>
       <c r="P35" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5062,22 +5234,22 @@
       <c r="AB35" s="178"/>
       <c r="AC35" s="179"/>
       <c r="AD35" s="179"/>
-      <c r="AE35" s="361"/>
+      <c r="AE35" s="193"/>
       <c r="AF35" s="179"/>
       <c r="AG35" s="179"/>
       <c r="AH35" s="179"/>
-      <c r="AI35" s="357" t="s">
-        <v>119</v>
+      <c r="AI35" s="189" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="326"/>
-      <c r="B36" s="198"/>
-      <c r="C36" s="200"/>
-      <c r="D36" s="243"/>
-      <c r="E36" s="244"/>
-      <c r="F36" s="244"/>
-      <c r="G36" s="245"/>
+      <c r="A36" s="207"/>
+      <c r="B36" s="320"/>
+      <c r="C36" s="322"/>
+      <c r="D36" s="339"/>
+      <c r="E36" s="340"/>
+      <c r="F36" s="340"/>
+      <c r="G36" s="341"/>
       <c r="H36" s="86">
         <f>SUM(H32:H35)</f>
         <v>0</v>
@@ -5126,7 +5298,7 @@
       <c r="AF36" s="168"/>
       <c r="AG36" s="168"/>
       <c r="AH36" s="168"/>
-      <c r="AI36" s="168"/>
+      <c r="AI36" s="189"/>
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
       <c r="AL36" s="2"/>
@@ -5139,17 +5311,17 @@
       <c r="AS36" s="2"/>
     </row>
     <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="326"/>
-      <c r="B37" s="198"/>
-      <c r="C37" s="200"/>
-      <c r="D37" s="346" t="s">
+      <c r="A37" s="207"/>
+      <c r="B37" s="320"/>
+      <c r="C37" s="322"/>
+      <c r="D37" s="233" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="349">
+      <c r="G37" s="236">
         <v>48</v>
       </c>
       <c r="H37" s="95"/>
@@ -5161,7 +5333,7 @@
       <c r="N37" s="95">
         <v>12</v>
       </c>
-      <c r="O37" s="252">
+      <c r="O37" s="290">
         <f t="shared" ref="O37" si="34">SUM(P37:P40)</f>
         <v>48</v>
       </c>
@@ -5199,8 +5371,8 @@
         <f>AG37/O37</f>
         <v>1</v>
       </c>
-      <c r="AI37" s="3" t="s">
-        <v>114</v>
+      <c r="AI37" s="189" t="s">
+        <v>140</v>
       </c>
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
@@ -5214,15 +5386,15 @@
       <c r="AS37" s="3"/>
     </row>
     <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="326"/>
-      <c r="B38" s="198"/>
-      <c r="C38" s="200"/>
-      <c r="D38" s="347"/>
+      <c r="A38" s="207"/>
+      <c r="B38" s="320"/>
+      <c r="C38" s="322"/>
+      <c r="D38" s="234"/>
       <c r="E38" s="89"/>
       <c r="F38" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="350"/>
+      <c r="G38" s="237"/>
       <c r="H38" s="96"/>
       <c r="I38" s="96"/>
       <c r="J38" s="96"/>
@@ -5232,7 +5404,7 @@
       <c r="N38" s="96">
         <v>12</v>
       </c>
-      <c r="O38" s="253"/>
+      <c r="O38" s="291"/>
       <c r="P38" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5255,8 +5427,8 @@
       <c r="AF38" s="3"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
-      <c r="AI38" s="3" t="s">
-        <v>114</v>
+      <c r="AI38" s="189" t="s">
+        <v>141</v>
       </c>
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
@@ -5270,15 +5442,15 @@
       <c r="AS38" s="3"/>
     </row>
     <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="326"/>
-      <c r="B39" s="198"/>
-      <c r="C39" s="200"/>
-      <c r="D39" s="347"/>
+      <c r="A39" s="207"/>
+      <c r="B39" s="320"/>
+      <c r="C39" s="322"/>
+      <c r="D39" s="234"/>
       <c r="E39" s="89"/>
       <c r="F39" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="350"/>
+      <c r="G39" s="237"/>
       <c r="H39" s="96"/>
       <c r="I39" s="96"/>
       <c r="J39" s="96"/>
@@ -5288,7 +5460,7 @@
       <c r="N39" s="96">
         <v>12</v>
       </c>
-      <c r="O39" s="253"/>
+      <c r="O39" s="291"/>
       <c r="P39" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5311,8 +5483,8 @@
       <c r="AF39" s="3"/>
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
-      <c r="AI39" s="3" t="s">
-        <v>114</v>
+      <c r="AI39" s="189" t="s">
+        <v>142</v>
       </c>
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
@@ -5326,15 +5498,15 @@
       <c r="AS39" s="3"/>
     </row>
     <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="326"/>
-      <c r="B40" s="198"/>
-      <c r="C40" s="200"/>
-      <c r="D40" s="348"/>
+      <c r="A40" s="207"/>
+      <c r="B40" s="320"/>
+      <c r="C40" s="322"/>
+      <c r="D40" s="235"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="351"/>
+      <c r="G40" s="238"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
       <c r="J40" s="97"/>
@@ -5344,7 +5516,7 @@
       <c r="N40" s="97">
         <v>12</v>
       </c>
-      <c r="O40" s="254"/>
+      <c r="O40" s="292"/>
       <c r="P40" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5367,8 +5539,8 @@
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
-      <c r="AI40" s="3" t="s">
-        <v>114</v>
+      <c r="AI40" s="189" t="s">
+        <v>143</v>
       </c>
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
@@ -5382,13 +5554,13 @@
       <c r="AS40" s="3"/>
     </row>
     <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="326"/>
-      <c r="B41" s="198"/>
-      <c r="C41" s="200"/>
-      <c r="D41" s="246"/>
-      <c r="E41" s="247"/>
-      <c r="F41" s="247"/>
-      <c r="G41" s="248"/>
+      <c r="A41" s="207"/>
+      <c r="B41" s="320"/>
+      <c r="C41" s="322"/>
+      <c r="D41" s="342"/>
+      <c r="E41" s="343"/>
+      <c r="F41" s="343"/>
+      <c r="G41" s="344"/>
       <c r="H41" s="93">
         <f>SUM(H37:H40)</f>
         <v>0</v>
@@ -5437,7 +5609,7 @@
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
-      <c r="AI41" s="2"/>
+      <c r="AI41" s="189"/>
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
@@ -5450,17 +5622,17 @@
       <c r="AS41" s="2"/>
     </row>
     <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="326"/>
-      <c r="B42" s="198"/>
-      <c r="C42" s="200"/>
-      <c r="D42" s="258" t="s">
+      <c r="A42" s="207"/>
+      <c r="B42" s="320"/>
+      <c r="C42" s="322"/>
+      <c r="D42" s="194" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="261">
+      <c r="G42" s="197">
         <v>48</v>
       </c>
       <c r="H42" s="34">
@@ -5472,7 +5644,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
-      <c r="O42" s="255">
+      <c r="O42" s="278">
         <f t="shared" ref="O42" si="41">SUM(P42:P45)</f>
         <v>48</v>
       </c>
@@ -5510,8 +5682,8 @@
         <f>AG42/O42</f>
         <v>1</v>
       </c>
-      <c r="AI42" s="3" t="s">
-        <v>120</v>
+      <c r="AI42" s="189" t="s">
+        <v>144</v>
       </c>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -5525,15 +5697,15 @@
       <c r="AS42" s="3"/>
     </row>
     <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="326"/>
-      <c r="B43" s="198"/>
-      <c r="C43" s="200"/>
-      <c r="D43" s="259"/>
+      <c r="A43" s="207"/>
+      <c r="B43" s="320"/>
+      <c r="C43" s="322"/>
+      <c r="D43" s="195"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="262"/>
+      <c r="G43" s="198"/>
       <c r="H43" s="35">
         <v>12</v>
       </c>
@@ -5543,7 +5715,7 @@
       <c r="L43" s="35"/>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="256"/>
+      <c r="O43" s="279"/>
       <c r="P43" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5566,8 +5738,8 @@
       <c r="AF43" s="3"/>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
-      <c r="AI43" s="3" t="s">
-        <v>120</v>
+      <c r="AI43" s="189" t="s">
+        <v>145</v>
       </c>
       <c r="AJ43" s="3"/>
       <c r="AK43" s="3"/>
@@ -5581,15 +5753,15 @@
       <c r="AS43" s="3"/>
     </row>
     <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="326"/>
-      <c r="B44" s="198"/>
-      <c r="C44" s="200"/>
-      <c r="D44" s="259"/>
+      <c r="A44" s="207"/>
+      <c r="B44" s="320"/>
+      <c r="C44" s="322"/>
+      <c r="D44" s="195"/>
       <c r="E44" s="30"/>
       <c r="F44" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="262"/>
+      <c r="G44" s="198"/>
       <c r="H44" s="35">
         <v>12</v>
       </c>
@@ -5599,7 +5771,7 @@
       <c r="L44" s="35"/>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
-      <c r="O44" s="256"/>
+      <c r="O44" s="279"/>
       <c r="P44" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5622,8 +5794,8 @@
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
-      <c r="AI44" s="3" t="s">
-        <v>120</v>
+      <c r="AI44" s="189" t="s">
+        <v>146</v>
       </c>
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
@@ -5637,15 +5809,15 @@
       <c r="AS44" s="3"/>
     </row>
     <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="326"/>
-      <c r="B45" s="198"/>
-      <c r="C45" s="200"/>
-      <c r="D45" s="260"/>
+      <c r="A45" s="207"/>
+      <c r="B45" s="320"/>
+      <c r="C45" s="322"/>
+      <c r="D45" s="196"/>
       <c r="E45" s="32"/>
       <c r="F45" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="263"/>
+      <c r="G45" s="199"/>
       <c r="H45" s="36">
         <v>12</v>
       </c>
@@ -5655,7 +5827,7 @@
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
-      <c r="O45" s="257"/>
+      <c r="O45" s="280"/>
       <c r="P45" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5678,8 +5850,8 @@
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
-      <c r="AI45" s="3" t="s">
-        <v>120</v>
+      <c r="AI45" s="189" t="s">
+        <v>147</v>
       </c>
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
@@ -5693,13 +5865,13 @@
       <c r="AS45" s="3"/>
     </row>
     <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="326"/>
-      <c r="B46" s="198"/>
-      <c r="C46" s="200"/>
-      <c r="D46" s="308"/>
-      <c r="E46" s="309"/>
-      <c r="F46" s="309"/>
-      <c r="G46" s="310"/>
+      <c r="A46" s="207"/>
+      <c r="B46" s="320"/>
+      <c r="C46" s="322"/>
+      <c r="D46" s="245"/>
+      <c r="E46" s="246"/>
+      <c r="F46" s="246"/>
+      <c r="G46" s="247"/>
       <c r="H46" s="98">
         <f>SUM(H42:H45)</f>
         <v>48</v>
@@ -5748,7 +5920,7 @@
       <c r="AF46" s="120"/>
       <c r="AG46" s="120"/>
       <c r="AH46" s="120"/>
-      <c r="AI46" s="120"/>
+      <c r="AI46" s="189"/>
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
       <c r="AL46" s="2"/>
@@ -5761,17 +5933,17 @@
       <c r="AS46" s="2"/>
     </row>
     <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="326"/>
-      <c r="B47" s="198"/>
-      <c r="C47" s="200"/>
-      <c r="D47" s="314" t="s">
+      <c r="A47" s="207"/>
+      <c r="B47" s="320"/>
+      <c r="C47" s="322"/>
+      <c r="D47" s="251" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="99"/>
       <c r="F47" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="302">
+      <c r="G47" s="242">
         <v>48</v>
       </c>
       <c r="H47" s="107"/>
@@ -5783,7 +5955,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
-      <c r="O47" s="267">
+      <c r="O47" s="264">
         <f t="shared" ref="O47" si="48">SUM(P47:P50)</f>
         <v>48</v>
       </c>
@@ -5813,28 +5985,28 @@
       <c r="AD47" s="179"/>
       <c r="AE47" s="179"/>
       <c r="AF47" s="179"/>
-      <c r="AG47" s="355">
+      <c r="AG47" s="187">
         <f>O47-AF47</f>
         <v>48</v>
       </c>
-      <c r="AH47" s="356">
+      <c r="AH47" s="188">
         <f>AG47/O47</f>
         <v>1</v>
       </c>
-      <c r="AI47" s="357" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:45" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="326"/>
-      <c r="B48" s="198"/>
-      <c r="C48" s="200"/>
-      <c r="D48" s="315"/>
+      <c r="AI47" s="189" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:45" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="207"/>
+      <c r="B48" s="320"/>
+      <c r="C48" s="322"/>
+      <c r="D48" s="252"/>
       <c r="E48" s="101"/>
       <c r="F48" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="303"/>
+      <c r="G48" s="243"/>
       <c r="H48" s="108"/>
       <c r="I48" s="108">
         <v>12</v>
@@ -5844,7 +6016,7 @@
       <c r="L48" s="108"/>
       <c r="M48" s="108"/>
       <c r="N48" s="108"/>
-      <c r="O48" s="268"/>
+      <c r="O48" s="265"/>
       <c r="P48" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5867,20 +6039,20 @@
       <c r="AF48" s="179"/>
       <c r="AG48" s="179"/>
       <c r="AH48" s="179"/>
-      <c r="AI48" s="357" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="326"/>
-      <c r="B49" s="198"/>
-      <c r="C49" s="200"/>
-      <c r="D49" s="315"/>
+      <c r="AI48" s="189" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:45" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="207"/>
+      <c r="B49" s="320"/>
+      <c r="C49" s="322"/>
+      <c r="D49" s="252"/>
       <c r="E49" s="101"/>
       <c r="F49" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="303"/>
+      <c r="G49" s="243"/>
       <c r="H49" s="108"/>
       <c r="I49" s="108">
         <v>12</v>
@@ -5890,7 +6062,7 @@
       <c r="L49" s="108"/>
       <c r="M49" s="108"/>
       <c r="N49" s="108"/>
-      <c r="O49" s="268"/>
+      <c r="O49" s="265"/>
       <c r="P49" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5913,20 +6085,20 @@
       <c r="AF49" s="179"/>
       <c r="AG49" s="179"/>
       <c r="AH49" s="179"/>
-      <c r="AI49" s="357" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:45" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="326"/>
-      <c r="B50" s="198"/>
-      <c r="C50" s="200"/>
-      <c r="D50" s="316"/>
+      <c r="AI49" s="189" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="207"/>
+      <c r="B50" s="320"/>
+      <c r="C50" s="322"/>
+      <c r="D50" s="253"/>
       <c r="E50" s="103"/>
       <c r="F50" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="G50" s="304"/>
+      <c r="G50" s="244"/>
       <c r="H50" s="109"/>
       <c r="I50" s="109">
         <v>12</v>
@@ -5936,7 +6108,7 @@
       <c r="L50" s="109"/>
       <c r="M50" s="109"/>
       <c r="N50" s="109"/>
-      <c r="O50" s="269"/>
+      <c r="O50" s="266"/>
       <c r="P50" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5959,18 +6131,18 @@
       <c r="AF50" s="179"/>
       <c r="AG50" s="179"/>
       <c r="AH50" s="179"/>
-      <c r="AI50" s="357" t="s">
-        <v>121</v>
+      <c r="AI50" s="189" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="326"/>
-      <c r="B51" s="198"/>
-      <c r="C51" s="200"/>
-      <c r="D51" s="311"/>
-      <c r="E51" s="312"/>
-      <c r="F51" s="312"/>
-      <c r="G51" s="313"/>
+      <c r="A51" s="207"/>
+      <c r="B51" s="320"/>
+      <c r="C51" s="322"/>
+      <c r="D51" s="248"/>
+      <c r="E51" s="249"/>
+      <c r="F51" s="249"/>
+      <c r="G51" s="250"/>
       <c r="H51" s="106">
         <f>SUM(H47:H50)</f>
         <v>0</v>
@@ -6032,17 +6204,17 @@
       <c r="AS51" s="2"/>
     </row>
     <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="326"/>
-      <c r="B52" s="198"/>
-      <c r="C52" s="200"/>
-      <c r="D52" s="317" t="s">
+      <c r="A52" s="207"/>
+      <c r="B52" s="320"/>
+      <c r="C52" s="322"/>
+      <c r="D52" s="215" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="47"/>
       <c r="F52" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G52" s="305">
+      <c r="G52" s="218">
         <v>48</v>
       </c>
       <c r="H52" s="53"/>
@@ -6054,7 +6226,7 @@
       <c r="N52" s="53">
         <v>12</v>
       </c>
-      <c r="O52" s="270">
+      <c r="O52" s="267">
         <f t="shared" ref="O52" si="55">SUM(P52:P55)</f>
         <v>48</v>
       </c>
@@ -6092,8 +6264,8 @@
         <f>AG52/O52</f>
         <v>1</v>
       </c>
-      <c r="AI52" s="3" t="s">
-        <v>115</v>
+      <c r="AI52" s="189" t="s">
+        <v>152</v>
       </c>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3"/>
@@ -6107,15 +6279,15 @@
       <c r="AS52" s="3"/>
     </row>
     <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="326"/>
-      <c r="B53" s="198"/>
-      <c r="C53" s="200"/>
-      <c r="D53" s="318"/>
+      <c r="A53" s="207"/>
+      <c r="B53" s="320"/>
+      <c r="C53" s="322"/>
+      <c r="D53" s="216"/>
       <c r="E53" s="49"/>
       <c r="F53" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G53" s="306"/>
+      <c r="G53" s="219"/>
       <c r="H53" s="54"/>
       <c r="I53" s="54"/>
       <c r="J53" s="54"/>
@@ -6125,7 +6297,7 @@
       <c r="N53" s="54">
         <v>12</v>
       </c>
-      <c r="O53" s="271"/>
+      <c r="O53" s="268"/>
       <c r="P53" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6148,8 +6320,8 @@
       <c r="AF53" s="3"/>
       <c r="AG53" s="3"/>
       <c r="AH53" s="3"/>
-      <c r="AI53" s="3" t="s">
-        <v>115</v>
+      <c r="AI53" s="189" t="s">
+        <v>153</v>
       </c>
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
@@ -6162,16 +6334,16 @@
       <c r="AR53" s="3"/>
       <c r="AS53" s="3"/>
     </row>
-    <row r="54" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="326"/>
-      <c r="B54" s="198"/>
-      <c r="C54" s="200"/>
-      <c r="D54" s="318"/>
+    <row r="54" spans="1:45" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="207"/>
+      <c r="B54" s="320"/>
+      <c r="C54" s="322"/>
+      <c r="D54" s="216"/>
       <c r="E54" s="49"/>
       <c r="F54" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="306"/>
+      <c r="G54" s="219"/>
       <c r="H54" s="54"/>
       <c r="I54" s="54"/>
       <c r="J54" s="54"/>
@@ -6181,7 +6353,7 @@
       <c r="N54" s="54">
         <v>12</v>
       </c>
-      <c r="O54" s="271"/>
+      <c r="O54" s="268"/>
       <c r="P54" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6204,8 +6376,8 @@
       <c r="AF54" s="3"/>
       <c r="AG54" s="3"/>
       <c r="AH54" s="3"/>
-      <c r="AI54" s="3" t="s">
-        <v>115</v>
+      <c r="AI54" s="189" t="s">
+        <v>154</v>
       </c>
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
@@ -6219,15 +6391,15 @@
       <c r="AS54" s="3"/>
     </row>
     <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="326"/>
-      <c r="B55" s="198"/>
-      <c r="C55" s="200"/>
-      <c r="D55" s="319"/>
+      <c r="A55" s="207"/>
+      <c r="B55" s="320"/>
+      <c r="C55" s="322"/>
+      <c r="D55" s="217"/>
       <c r="E55" s="51"/>
       <c r="F55" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="307"/>
+      <c r="G55" s="220"/>
       <c r="H55" s="55"/>
       <c r="I55" s="55"/>
       <c r="J55" s="55"/>
@@ -6237,7 +6409,7 @@
       <c r="N55" s="55">
         <v>12</v>
       </c>
-      <c r="O55" s="272"/>
+      <c r="O55" s="269"/>
       <c r="P55" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6260,8 +6432,8 @@
       <c r="AF55" s="3"/>
       <c r="AG55" s="3"/>
       <c r="AH55" s="3"/>
-      <c r="AI55" s="3" t="s">
-        <v>115</v>
+      <c r="AI55" s="189" t="s">
+        <v>155</v>
       </c>
       <c r="AJ55" s="3"/>
       <c r="AK55" s="3"/>
@@ -6275,13 +6447,13 @@
       <c r="AS55" s="3"/>
     </row>
     <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="326"/>
-      <c r="B56" s="198"/>
-      <c r="C56" s="200"/>
-      <c r="D56" s="287"/>
-      <c r="E56" s="288"/>
-      <c r="F56" s="288"/>
-      <c r="G56" s="289"/>
+      <c r="A56" s="207"/>
+      <c r="B56" s="320"/>
+      <c r="C56" s="322"/>
+      <c r="D56" s="345"/>
+      <c r="E56" s="346"/>
+      <c r="F56" s="346"/>
+      <c r="G56" s="347"/>
       <c r="H56" s="64">
         <f>SUM(H52:H55)</f>
         <v>0</v>
@@ -6330,7 +6502,7 @@
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
-      <c r="AI56" s="2"/>
+      <c r="AI56" s="168"/>
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
       <c r="AL56" s="2"/>
@@ -6342,11 +6514,11 @@
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
     </row>
-    <row r="57" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="326"/>
-      <c r="B57" s="198"/>
-      <c r="C57" s="200"/>
-      <c r="D57" s="296" t="s">
+    <row r="57" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="207"/>
+      <c r="B57" s="320"/>
+      <c r="C57" s="322"/>
+      <c r="D57" s="256" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="149">
@@ -6355,7 +6527,7 @@
       <c r="F57" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="297">
+      <c r="G57" s="258">
         <v>96</v>
       </c>
       <c r="H57" s="114"/>
@@ -6367,7 +6539,7 @@
       <c r="L57" s="114"/>
       <c r="M57" s="114"/>
       <c r="N57" s="114"/>
-      <c r="O57" s="273">
+      <c r="O57" s="270">
         <f t="shared" ref="O57" si="62">SUM(P57:P60)</f>
         <v>96</v>
       </c>
@@ -6422,16 +6594,16 @@
         <v>0.3125</v>
       </c>
       <c r="AF57" s="176"/>
-      <c r="AG57" s="358">
+      <c r="AG57" s="190">
         <f>O57-AF57</f>
         <v>96</v>
       </c>
-      <c r="AH57" s="359">
+      <c r="AH57" s="191">
         <f>AG57/O57</f>
         <v>1</v>
       </c>
-      <c r="AI57" s="176" t="s">
-        <v>118</v>
+      <c r="AI57" s="189" t="s">
+        <v>156</v>
       </c>
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
@@ -6444,18 +6616,18 @@
       <c r="AR57" s="3"/>
       <c r="AS57" s="3"/>
     </row>
-    <row r="58" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="326"/>
-      <c r="B58" s="198"/>
-      <c r="C58" s="200"/>
-      <c r="D58" s="241"/>
+    <row r="58" spans="1:45" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="207"/>
+      <c r="B58" s="320"/>
+      <c r="C58" s="322"/>
+      <c r="D58" s="257"/>
       <c r="E58" s="145">
         <v>2</v>
       </c>
       <c r="F58" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="G58" s="298"/>
+      <c r="G58" s="259"/>
       <c r="H58" s="115"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115">
@@ -6465,7 +6637,7 @@
       <c r="L58" s="115"/>
       <c r="M58" s="115"/>
       <c r="N58" s="115"/>
-      <c r="O58" s="274"/>
+      <c r="O58" s="271"/>
       <c r="P58" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6488,8 +6660,8 @@
       <c r="AF58" s="177"/>
       <c r="AG58" s="177"/>
       <c r="AH58" s="177"/>
-      <c r="AI58" s="176" t="s">
-        <v>118</v>
+      <c r="AI58" s="189" t="s">
+        <v>157</v>
       </c>
       <c r="AJ58" s="7"/>
       <c r="AK58" s="7"/>
@@ -6502,18 +6674,18 @@
       <c r="AR58" s="7"/>
       <c r="AS58" s="7"/>
     </row>
-    <row r="59" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="326"/>
-      <c r="B59" s="198"/>
-      <c r="C59" s="200"/>
-      <c r="D59" s="241"/>
+    <row r="59" spans="1:45" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="207"/>
+      <c r="B59" s="320"/>
+      <c r="C59" s="322"/>
+      <c r="D59" s="257"/>
       <c r="E59" s="145">
         <v>4</v>
       </c>
       <c r="F59" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="298"/>
+      <c r="G59" s="259"/>
       <c r="H59" s="115"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115">
@@ -6523,7 +6695,7 @@
       <c r="L59" s="115"/>
       <c r="M59" s="115"/>
       <c r="N59" s="115"/>
-      <c r="O59" s="274"/>
+      <c r="O59" s="271"/>
       <c r="P59" s="9">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -6546,8 +6718,8 @@
       <c r="AF59" s="177"/>
       <c r="AG59" s="177"/>
       <c r="AH59" s="177"/>
-      <c r="AI59" s="176" t="s">
-        <v>118</v>
+      <c r="AI59" s="189" t="s">
+        <v>158</v>
       </c>
       <c r="AJ59" s="7"/>
       <c r="AK59" s="7"/>
@@ -6561,17 +6733,17 @@
       <c r="AS59" s="7"/>
     </row>
     <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="326"/>
-      <c r="B60" s="198"/>
-      <c r="C60" s="200"/>
-      <c r="D60" s="241"/>
+      <c r="A60" s="207"/>
+      <c r="B60" s="320"/>
+      <c r="C60" s="322"/>
+      <c r="D60" s="257"/>
       <c r="E60" s="145">
         <v>1</v>
       </c>
       <c r="F60" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="298"/>
+      <c r="G60" s="259"/>
       <c r="H60" s="115"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115">
@@ -6581,7 +6753,7 @@
       <c r="L60" s="115"/>
       <c r="M60" s="115"/>
       <c r="N60" s="115"/>
-      <c r="O60" s="274"/>
+      <c r="O60" s="271"/>
       <c r="P60" s="9">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -6604,8 +6776,8 @@
       <c r="AF60" s="177"/>
       <c r="AG60" s="177"/>
       <c r="AH60" s="177"/>
-      <c r="AI60" s="176" t="s">
-        <v>118</v>
+      <c r="AI60" s="189" t="s">
+        <v>159</v>
       </c>
       <c r="AJ60" s="7"/>
       <c r="AK60" s="7"/>
@@ -6619,13 +6791,13 @@
       <c r="AS60" s="7"/>
     </row>
     <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="326"/>
-      <c r="B61" s="198"/>
-      <c r="C61" s="200"/>
-      <c r="D61" s="242"/>
-      <c r="E61" s="299"/>
-      <c r="F61" s="299"/>
-      <c r="G61" s="299"/>
+      <c r="A61" s="207"/>
+      <c r="B61" s="320"/>
+      <c r="C61" s="322"/>
+      <c r="D61" s="260"/>
+      <c r="E61" s="261"/>
+      <c r="F61" s="261"/>
+      <c r="G61" s="261"/>
       <c r="H61" s="150">
         <f>SUM(H57:H60)</f>
         <v>0</v>
@@ -6674,7 +6846,7 @@
       <c r="AF61" s="168"/>
       <c r="AG61" s="168"/>
       <c r="AH61" s="168"/>
-      <c r="AI61" s="168"/>
+      <c r="AI61" s="189"/>
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
       <c r="AL61" s="2"/>
@@ -6687,10 +6859,10 @@
       <c r="AS61" s="2"/>
     </row>
     <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="326"/>
-      <c r="B62" s="198"/>
-      <c r="C62" s="200"/>
-      <c r="D62" s="292" t="s">
+      <c r="A62" s="207"/>
+      <c r="B62" s="320"/>
+      <c r="C62" s="322"/>
+      <c r="D62" s="350" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="142">
@@ -6699,7 +6871,7 @@
       <c r="F62" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="G62" s="293">
+      <c r="G62" s="351">
         <v>288</v>
       </c>
       <c r="H62" s="132"/>
@@ -6711,7 +6883,7 @@
         <v>72</v>
       </c>
       <c r="N62" s="132"/>
-      <c r="O62" s="193">
+      <c r="O62" s="358">
         <f t="shared" ref="O62" si="69">SUM(P62:P65)</f>
         <v>288</v>
       </c>
@@ -6772,8 +6944,8 @@
         <f>AG62/O62</f>
         <v>1</v>
       </c>
-      <c r="AI62" s="3" t="s">
-        <v>113</v>
+      <c r="AI62" s="189" t="s">
+        <v>160</v>
       </c>
       <c r="AJ62" s="3"/>
       <c r="AK62" s="3"/>
@@ -6787,17 +6959,17 @@
       <c r="AS62" s="3"/>
     </row>
     <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="326"/>
-      <c r="B63" s="198"/>
-      <c r="C63" s="200"/>
-      <c r="D63" s="259"/>
+      <c r="A63" s="207"/>
+      <c r="B63" s="320"/>
+      <c r="C63" s="322"/>
+      <c r="D63" s="195"/>
       <c r="E63" s="116">
         <v>1</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="262"/>
+      <c r="G63" s="198"/>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
@@ -6807,7 +6979,7 @@
       <c r="L63" s="35"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
-      <c r="O63" s="194"/>
+      <c r="O63" s="359"/>
       <c r="P63" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6830,8 +7002,8 @@
       <c r="AF63" s="3"/>
       <c r="AG63" s="3"/>
       <c r="AH63" s="3"/>
-      <c r="AI63" s="3" t="s">
-        <v>113</v>
+      <c r="AI63" s="189" t="s">
+        <v>161</v>
       </c>
       <c r="AJ63" s="3"/>
       <c r="AK63" s="3"/>
@@ -6845,17 +7017,17 @@
       <c r="AS63" s="3"/>
     </row>
     <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="326"/>
-      <c r="B64" s="198"/>
-      <c r="C64" s="200"/>
-      <c r="D64" s="259"/>
+      <c r="A64" s="207"/>
+      <c r="B64" s="320"/>
+      <c r="C64" s="322"/>
+      <c r="D64" s="195"/>
       <c r="E64" s="116">
         <v>2</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="262"/>
+      <c r="G64" s="198"/>
       <c r="H64" s="35"/>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
@@ -6865,7 +7037,7 @@
       <c r="L64" s="35"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
-      <c r="O64" s="194"/>
+      <c r="O64" s="359"/>
       <c r="P64" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6888,8 +7060,8 @@
       <c r="AF64" s="3"/>
       <c r="AG64" s="3"/>
       <c r="AH64" s="3"/>
-      <c r="AI64" s="3" t="s">
-        <v>113</v>
+      <c r="AI64" s="189" t="s">
+        <v>162</v>
       </c>
       <c r="AJ64" s="3"/>
       <c r="AK64" s="3"/>
@@ -6903,17 +7075,17 @@
       <c r="AS64" s="3"/>
     </row>
     <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="326"/>
-      <c r="B65" s="198"/>
-      <c r="C65" s="200"/>
-      <c r="D65" s="259"/>
+      <c r="A65" s="207"/>
+      <c r="B65" s="320"/>
+      <c r="C65" s="322"/>
+      <c r="D65" s="195"/>
       <c r="E65" s="116">
         <v>3</v>
       </c>
       <c r="F65" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G65" s="262"/>
+      <c r="G65" s="198"/>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
       <c r="J65" s="35"/>
@@ -6925,7 +7097,7 @@
       </c>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
-      <c r="O65" s="194"/>
+      <c r="O65" s="359"/>
       <c r="P65" s="9">
         <f t="shared" si="4"/>
         <v>168</v>
@@ -6948,8 +7120,8 @@
       <c r="AF65" s="3"/>
       <c r="AG65" s="3"/>
       <c r="AH65" s="3"/>
-      <c r="AI65" s="3" t="s">
-        <v>113</v>
+      <c r="AI65" s="189" t="s">
+        <v>163</v>
       </c>
       <c r="AJ65" s="3"/>
       <c r="AK65" s="3"/>
@@ -6963,13 +7135,13 @@
       <c r="AS65" s="3"/>
     </row>
     <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="326"/>
-      <c r="B66" s="198"/>
-      <c r="C66" s="200"/>
-      <c r="D66" s="300"/>
-      <c r="E66" s="301"/>
-      <c r="F66" s="301"/>
-      <c r="G66" s="301"/>
+      <c r="A66" s="207"/>
+      <c r="B66" s="320"/>
+      <c r="C66" s="322"/>
+      <c r="D66" s="262"/>
+      <c r="E66" s="263"/>
+      <c r="F66" s="263"/>
+      <c r="G66" s="263"/>
       <c r="H66" s="152">
         <f>SUM(H62:H65)</f>
         <v>0</v>
@@ -7018,7 +7190,7 @@
       <c r="AF66" s="2"/>
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
-      <c r="AI66" s="2"/>
+      <c r="AI66" s="189"/>
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
       <c r="AL66" s="2"/>
@@ -7031,17 +7203,17 @@
       <c r="AS66" s="2"/>
     </row>
     <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="326"/>
-      <c r="B67" s="198"/>
-      <c r="C67" s="200"/>
-      <c r="D67" s="290" t="s">
+      <c r="A67" s="207"/>
+      <c r="B67" s="320"/>
+      <c r="C67" s="322"/>
+      <c r="D67" s="348" t="s">
         <v>49</v>
       </c>
       <c r="E67" s="134"/>
       <c r="F67" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="294">
+      <c r="G67" s="254">
         <v>384</v>
       </c>
       <c r="H67" s="128">
@@ -7053,7 +7225,7 @@
       <c r="L67" s="128"/>
       <c r="M67" s="128"/>
       <c r="N67" s="128"/>
-      <c r="O67" s="195">
+      <c r="O67" s="360">
         <f>SUM(P67:P72)</f>
         <v>384</v>
       </c>
@@ -7091,8 +7263,8 @@
         <f>AG67/O67</f>
         <v>1</v>
       </c>
-      <c r="AI67" s="3" t="s">
-        <v>122</v>
+      <c r="AI67" s="189" t="s">
+        <v>164</v>
       </c>
       <c r="AJ67" s="3"/>
       <c r="AK67" s="3"/>
@@ -7106,15 +7278,15 @@
       <c r="AS67" s="3"/>
     </row>
     <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="326"/>
-      <c r="B68" s="198"/>
-      <c r="C68" s="200"/>
-      <c r="D68" s="291"/>
+      <c r="A68" s="207"/>
+      <c r="B68" s="320"/>
+      <c r="C68" s="322"/>
+      <c r="D68" s="349"/>
       <c r="E68" s="133"/>
       <c r="F68" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="295"/>
+      <c r="G68" s="255"/>
       <c r="H68" s="130"/>
       <c r="I68" s="130">
         <v>72</v>
@@ -7124,7 +7296,7 @@
       <c r="L68" s="130"/>
       <c r="M68" s="130"/>
       <c r="N68" s="130"/>
-      <c r="O68" s="196"/>
+      <c r="O68" s="361"/>
       <c r="P68" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7147,8 +7319,8 @@
       <c r="AF68" s="3"/>
       <c r="AG68" s="3"/>
       <c r="AH68" s="3"/>
-      <c r="AI68" s="3" t="s">
-        <v>122</v>
+      <c r="AI68" s="189" t="s">
+        <v>165</v>
       </c>
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
@@ -7162,15 +7334,15 @@
       <c r="AS68" s="3"/>
     </row>
     <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="326"/>
-      <c r="B69" s="198"/>
-      <c r="C69" s="200"/>
-      <c r="D69" s="291"/>
+      <c r="A69" s="207"/>
+      <c r="B69" s="320"/>
+      <c r="C69" s="322"/>
+      <c r="D69" s="349"/>
       <c r="E69" s="133"/>
       <c r="F69" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="295"/>
+      <c r="G69" s="255"/>
       <c r="H69" s="130"/>
       <c r="I69" s="130"/>
       <c r="J69" s="130">
@@ -7180,7 +7352,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="130"/>
       <c r="N69" s="130"/>
-      <c r="O69" s="196"/>
+      <c r="O69" s="361"/>
       <c r="P69" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7203,8 +7375,8 @@
       <c r="AF69" s="3"/>
       <c r="AG69" s="3"/>
       <c r="AH69" s="3"/>
-      <c r="AI69" s="3" t="s">
-        <v>122</v>
+      <c r="AI69" s="189" t="s">
+        <v>166</v>
       </c>
       <c r="AJ69" s="3"/>
       <c r="AK69" s="3"/>
@@ -7218,15 +7390,15 @@
       <c r="AS69" s="3"/>
     </row>
     <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="326"/>
-      <c r="B70" s="198"/>
-      <c r="C70" s="200"/>
-      <c r="D70" s="291"/>
+      <c r="A70" s="207"/>
+      <c r="B70" s="320"/>
+      <c r="C70" s="322"/>
+      <c r="D70" s="349"/>
       <c r="E70" s="133"/>
       <c r="F70" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="295"/>
+      <c r="G70" s="255"/>
       <c r="H70" s="130"/>
       <c r="I70" s="130"/>
       <c r="J70" s="130"/>
@@ -7236,7 +7408,7 @@
       <c r="L70" s="130"/>
       <c r="M70" s="130"/>
       <c r="N70" s="130"/>
-      <c r="O70" s="196"/>
+      <c r="O70" s="361"/>
       <c r="P70" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7259,8 +7431,8 @@
       <c r="AF70" s="3"/>
       <c r="AG70" s="3"/>
       <c r="AH70" s="3"/>
-      <c r="AI70" s="3" t="s">
-        <v>122</v>
+      <c r="AI70" s="189" t="s">
+        <v>167</v>
       </c>
       <c r="AJ70" s="3"/>
       <c r="AK70" s="3"/>
@@ -7274,15 +7446,15 @@
       <c r="AS70" s="3"/>
     </row>
     <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="326"/>
-      <c r="B71" s="198"/>
-      <c r="C71" s="200"/>
-      <c r="D71" s="291"/>
+      <c r="A71" s="207"/>
+      <c r="B71" s="320"/>
+      <c r="C71" s="322"/>
+      <c r="D71" s="349"/>
       <c r="E71" s="133"/>
       <c r="F71" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="295"/>
+      <c r="G71" s="255"/>
       <c r="H71" s="130"/>
       <c r="I71" s="130"/>
       <c r="J71" s="130"/>
@@ -7292,7 +7464,7 @@
       </c>
       <c r="M71" s="130"/>
       <c r="N71" s="130"/>
-      <c r="O71" s="196"/>
+      <c r="O71" s="361"/>
       <c r="P71" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7315,8 +7487,8 @@
       <c r="AF71" s="3"/>
       <c r="AG71" s="3"/>
       <c r="AH71" s="3"/>
-      <c r="AI71" s="3" t="s">
-        <v>122</v>
+      <c r="AI71" s="189" t="s">
+        <v>168</v>
       </c>
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
@@ -7330,15 +7502,15 @@
       <c r="AS71" s="3"/>
     </row>
     <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="326"/>
-      <c r="B72" s="198"/>
-      <c r="C72" s="200"/>
-      <c r="D72" s="291"/>
+      <c r="A72" s="207"/>
+      <c r="B72" s="320"/>
+      <c r="C72" s="322"/>
+      <c r="D72" s="349"/>
       <c r="E72" s="133"/>
       <c r="F72" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="295"/>
+      <c r="G72" s="255"/>
       <c r="H72" s="130"/>
       <c r="I72" s="130"/>
       <c r="J72" s="130"/>
@@ -7348,7 +7520,7 @@
         <v>24</v>
       </c>
       <c r="N72" s="130"/>
-      <c r="O72" s="196"/>
+      <c r="O72" s="361"/>
       <c r="P72" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7371,8 +7543,8 @@
       <c r="AF72" s="3"/>
       <c r="AG72" s="3"/>
       <c r="AH72" s="3"/>
-      <c r="AI72" s="3" t="s">
-        <v>122</v>
+      <c r="AI72" s="189" t="s">
+        <v>169</v>
       </c>
       <c r="AJ72" s="3"/>
       <c r="AK72" s="3"/>
@@ -7386,13 +7558,13 @@
       <c r="AS72" s="3"/>
     </row>
     <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="326"/>
-      <c r="B73" s="198"/>
-      <c r="C73" s="200"/>
-      <c r="D73" s="220"/>
-      <c r="E73" s="221"/>
-      <c r="F73" s="221"/>
-      <c r="G73" s="221"/>
+      <c r="A73" s="207"/>
+      <c r="B73" s="320"/>
+      <c r="C73" s="322"/>
+      <c r="D73" s="298"/>
+      <c r="E73" s="299"/>
+      <c r="F73" s="299"/>
+      <c r="G73" s="299"/>
       <c r="H73" s="135">
         <f>SUM(H67:H72)</f>
         <v>72</v>
@@ -7441,7 +7613,7 @@
       <c r="AF73" s="2"/>
       <c r="AG73" s="2"/>
       <c r="AH73" s="2"/>
-      <c r="AI73" s="2"/>
+      <c r="AI73" s="189"/>
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
       <c r="AL73" s="2"/>
@@ -7453,18 +7625,18 @@
       <c r="AR73" s="2"/>
       <c r="AS73" s="2"/>
     </row>
-    <row r="74" spans="1:45" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="326"/>
-      <c r="B74" s="198"/>
-      <c r="C74" s="200"/>
-      <c r="D74" s="240" t="s">
+    <row r="74" spans="1:45" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="207"/>
+      <c r="B74" s="320"/>
+      <c r="C74" s="322"/>
+      <c r="D74" s="318" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="146"/>
       <c r="F74" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="230">
+      <c r="G74" s="308">
         <v>48</v>
       </c>
       <c r="H74" s="148"/>
@@ -7476,7 +7648,7 @@
       <c r="N74" s="148">
         <v>12</v>
       </c>
-      <c r="O74" s="187">
+      <c r="O74" s="352">
         <f>SUM(P74:P77)</f>
         <v>48</v>
       </c>
@@ -7514,8 +7686,8 @@
         <f>AG74/O74</f>
         <v>1</v>
       </c>
-      <c r="AI74" s="3" t="s">
-        <v>116</v>
+      <c r="AI74" s="189" t="s">
+        <v>170</v>
       </c>
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
@@ -7528,16 +7700,16 @@
       <c r="AR74" s="3"/>
       <c r="AS74" s="3"/>
     </row>
-    <row r="75" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="326"/>
-      <c r="B75" s="198"/>
-      <c r="C75" s="200"/>
-      <c r="D75" s="241"/>
+    <row r="75" spans="1:45" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="207"/>
+      <c r="B75" s="320"/>
+      <c r="C75" s="322"/>
+      <c r="D75" s="257"/>
       <c r="E75" s="145"/>
       <c r="F75" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="230"/>
+      <c r="G75" s="308"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117"/>
       <c r="J75" s="117"/>
@@ -7547,7 +7719,7 @@
       <c r="N75" s="117">
         <v>12</v>
       </c>
-      <c r="O75" s="187"/>
+      <c r="O75" s="352"/>
       <c r="P75" s="9">
         <f t="shared" ref="P75:P77" si="81">SUM(H75:N75)</f>
         <v>12</v>
@@ -7570,8 +7742,8 @@
       <c r="AF75" s="3"/>
       <c r="AG75" s="3"/>
       <c r="AH75" s="3"/>
-      <c r="AI75" s="3" t="s">
-        <v>116</v>
+      <c r="AI75" s="189" t="s">
+        <v>171</v>
       </c>
       <c r="AJ75" s="3"/>
       <c r="AK75" s="3"/>
@@ -7584,16 +7756,16 @@
       <c r="AR75" s="3"/>
       <c r="AS75" s="3"/>
     </row>
-    <row r="76" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="326"/>
-      <c r="B76" s="198"/>
-      <c r="C76" s="200"/>
-      <c r="D76" s="241"/>
+    <row r="76" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="207"/>
+      <c r="B76" s="320"/>
+      <c r="C76" s="322"/>
+      <c r="D76" s="257"/>
       <c r="E76" s="145"/>
       <c r="F76" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="230"/>
+      <c r="G76" s="308"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117"/>
       <c r="J76" s="117"/>
@@ -7603,7 +7775,7 @@
       <c r="N76" s="117">
         <v>12</v>
       </c>
-      <c r="O76" s="187"/>
+      <c r="O76" s="352"/>
       <c r="P76" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7626,8 +7798,8 @@
       <c r="AF76" s="3"/>
       <c r="AG76" s="3"/>
       <c r="AH76" s="3"/>
-      <c r="AI76" s="3" t="s">
-        <v>116</v>
+      <c r="AI76" s="189" t="s">
+        <v>172</v>
       </c>
       <c r="AJ76" s="3"/>
       <c r="AK76" s="3"/>
@@ -7640,16 +7812,16 @@
       <c r="AR76" s="3"/>
       <c r="AS76" s="3"/>
     </row>
-    <row r="77" spans="1:45" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="326"/>
-      <c r="B77" s="198"/>
-      <c r="C77" s="200"/>
-      <c r="D77" s="242"/>
+    <row r="77" spans="1:45" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="207"/>
+      <c r="B77" s="320"/>
+      <c r="C77" s="322"/>
+      <c r="D77" s="260"/>
       <c r="E77" s="145"/>
       <c r="F77" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G77" s="231"/>
+      <c r="G77" s="309"/>
       <c r="H77" s="118"/>
       <c r="I77" s="118"/>
       <c r="J77" s="118"/>
@@ -7659,7 +7831,7 @@
       <c r="N77" s="118">
         <v>12</v>
       </c>
-      <c r="O77" s="188"/>
+      <c r="O77" s="353"/>
       <c r="P77" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7682,8 +7854,8 @@
       <c r="AF77" s="3"/>
       <c r="AG77" s="3"/>
       <c r="AH77" s="3"/>
-      <c r="AI77" s="3" t="s">
-        <v>116</v>
+      <c r="AI77" s="189" t="s">
+        <v>173</v>
       </c>
       <c r="AJ77" s="3"/>
       <c r="AK77" s="3"/>
@@ -7697,13 +7869,13 @@
       <c r="AS77" s="3"/>
     </row>
     <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="326"/>
-      <c r="B78" s="198"/>
-      <c r="C78" s="200"/>
-      <c r="D78" s="222"/>
-      <c r="E78" s="223"/>
-      <c r="F78" s="224"/>
-      <c r="G78" s="225"/>
+      <c r="A78" s="207"/>
+      <c r="B78" s="320"/>
+      <c r="C78" s="322"/>
+      <c r="D78" s="300"/>
+      <c r="E78" s="301"/>
+      <c r="F78" s="302"/>
+      <c r="G78" s="303"/>
       <c r="H78" s="112">
         <f>SUM(H74:H77)</f>
         <v>0</v>
@@ -7752,7 +7924,7 @@
       <c r="AF78" s="2"/>
       <c r="AG78" s="2"/>
       <c r="AH78" s="2"/>
-      <c r="AI78" s="2"/>
+      <c r="AI78" s="189"/>
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
       <c r="AL78" s="2"/>
@@ -7765,17 +7937,17 @@
       <c r="AS78" s="2"/>
     </row>
     <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="326"/>
-      <c r="B79" s="198"/>
-      <c r="C79" s="200"/>
-      <c r="D79" s="238" t="s">
+      <c r="A79" s="207"/>
+      <c r="B79" s="320"/>
+      <c r="C79" s="322"/>
+      <c r="D79" s="316" t="s">
         <v>50</v>
       </c>
       <c r="E79" s="157"/>
       <c r="F79" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="G79" s="232">
+      <c r="G79" s="310">
         <v>48</v>
       </c>
       <c r="H79" s="159">
@@ -7787,7 +7959,7 @@
       <c r="L79" s="159"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
-      <c r="O79" s="191">
+      <c r="O79" s="356">
         <f>SUM(P79:P82)</f>
         <v>48</v>
       </c>
@@ -7819,8 +7991,8 @@
         <f>AG79/O79</f>
         <v>1</v>
       </c>
-      <c r="AI79" s="3" t="s">
-        <v>123</v>
+      <c r="AI79" s="189" t="s">
+        <v>174</v>
       </c>
       <c r="AJ79" s="3"/>
       <c r="AK79" s="3"/>
@@ -7833,16 +8005,16 @@
       <c r="AR79" s="3"/>
       <c r="AS79" s="3"/>
     </row>
-    <row r="80" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="326"/>
-      <c r="B80" s="198"/>
-      <c r="C80" s="200"/>
-      <c r="D80" s="239"/>
+    <row r="80" spans="1:45" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="207"/>
+      <c r="B80" s="320"/>
+      <c r="C80" s="322"/>
+      <c r="D80" s="317"/>
       <c r="E80" s="154"/>
       <c r="F80" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G80" s="233"/>
+      <c r="G80" s="311"/>
       <c r="H80" s="156">
         <v>12</v>
       </c>
@@ -7852,7 +8024,7 @@
       <c r="L80" s="156"/>
       <c r="M80" s="156"/>
       <c r="N80" s="156"/>
-      <c r="O80" s="192"/>
+      <c r="O80" s="357"/>
       <c r="P80" s="9">
         <f t="shared" ref="P80:P82" si="83">SUM(H80:N80)</f>
         <v>12</v>
@@ -7875,8 +8047,8 @@
       <c r="AF80" s="3"/>
       <c r="AG80" s="3"/>
       <c r="AH80" s="3"/>
-      <c r="AI80" s="3" t="s">
-        <v>123</v>
+      <c r="AI80" s="189" t="s">
+        <v>175</v>
       </c>
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
@@ -7890,15 +8062,15 @@
       <c r="AS80" s="3"/>
     </row>
     <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="326"/>
-      <c r="B81" s="198"/>
-      <c r="C81" s="200"/>
-      <c r="D81" s="239"/>
+      <c r="A81" s="207"/>
+      <c r="B81" s="320"/>
+      <c r="C81" s="322"/>
+      <c r="D81" s="317"/>
       <c r="E81" s="154"/>
       <c r="F81" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G81" s="233"/>
+      <c r="G81" s="311"/>
       <c r="H81" s="156">
         <v>12</v>
       </c>
@@ -7908,7 +8080,7 @@
       <c r="L81" s="156"/>
       <c r="M81" s="156"/>
       <c r="N81" s="156"/>
-      <c r="O81" s="192"/>
+      <c r="O81" s="357"/>
       <c r="P81" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7931,8 +8103,8 @@
       <c r="AF81" s="3"/>
       <c r="AG81" s="3"/>
       <c r="AH81" s="3"/>
-      <c r="AI81" s="3" t="s">
-        <v>123</v>
+      <c r="AI81" s="189" t="s">
+        <v>176</v>
       </c>
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
@@ -7946,15 +8118,15 @@
       <c r="AS81" s="3"/>
     </row>
     <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="326"/>
-      <c r="B82" s="198"/>
-      <c r="C82" s="200"/>
-      <c r="D82" s="239"/>
+      <c r="A82" s="207"/>
+      <c r="B82" s="320"/>
+      <c r="C82" s="322"/>
+      <c r="D82" s="317"/>
       <c r="E82" s="154"/>
       <c r="F82" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="G82" s="233"/>
+      <c r="G82" s="311"/>
       <c r="H82" s="156">
         <v>12</v>
       </c>
@@ -7964,7 +8136,7 @@
       <c r="L82" s="156"/>
       <c r="M82" s="156"/>
       <c r="N82" s="156"/>
-      <c r="O82" s="192"/>
+      <c r="O82" s="357"/>
       <c r="P82" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -7987,8 +8159,8 @@
       <c r="AF82" s="3"/>
       <c r="AG82" s="3"/>
       <c r="AH82" s="3"/>
-      <c r="AI82" s="3" t="s">
-        <v>123</v>
+      <c r="AI82" s="189" t="s">
+        <v>177</v>
       </c>
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
@@ -8002,13 +8174,13 @@
       <c r="AS82" s="3"/>
     </row>
     <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="326"/>
-      <c r="B83" s="198"/>
-      <c r="C83" s="200"/>
-      <c r="D83" s="226"/>
-      <c r="E83" s="227"/>
-      <c r="F83" s="227"/>
-      <c r="G83" s="227"/>
+      <c r="A83" s="207"/>
+      <c r="B83" s="320"/>
+      <c r="C83" s="322"/>
+      <c r="D83" s="304"/>
+      <c r="E83" s="305"/>
+      <c r="F83" s="305"/>
+      <c r="G83" s="305"/>
       <c r="H83" s="160">
         <f>SUM(H79:H82)</f>
         <v>48</v>
@@ -8057,7 +8229,7 @@
       <c r="AF83" s="2"/>
       <c r="AG83" s="2"/>
       <c r="AH83" s="2"/>
-      <c r="AI83" s="2"/>
+      <c r="AI83" s="189"/>
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
       <c r="AL83" s="2"/>
@@ -8069,18 +8241,18 @@
       <c r="AR83" s="2"/>
       <c r="AS83" s="2"/>
     </row>
-    <row r="84" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="326"/>
-      <c r="B84" s="198"/>
-      <c r="C84" s="201"/>
-      <c r="D84" s="236" t="s">
+    <row r="84" spans="1:45" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="207"/>
+      <c r="B84" s="320"/>
+      <c r="C84" s="323"/>
+      <c r="D84" s="314" t="s">
         <v>51</v>
       </c>
       <c r="E84" s="125"/>
       <c r="F84" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="234">
+      <c r="G84" s="312">
         <v>48</v>
       </c>
       <c r="H84" s="126"/>
@@ -8092,7 +8264,7 @@
       <c r="L84" s="126"/>
       <c r="M84" s="126"/>
       <c r="N84" s="126"/>
-      <c r="O84" s="189">
+      <c r="O84" s="354">
         <f>SUM(P84:P87)</f>
         <v>48</v>
       </c>
@@ -8124,8 +8296,8 @@
         <f>AG84/O84</f>
         <v>1</v>
       </c>
-      <c r="AI84" s="3" t="s">
-        <v>124</v>
+      <c r="AI84" s="189" t="s">
+        <v>159</v>
       </c>
       <c r="AJ84" s="3"/>
       <c r="AK84" s="3"/>
@@ -8138,16 +8310,16 @@
       <c r="AR84" s="3"/>
       <c r="AS84" s="3"/>
     </row>
-    <row r="85" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="326"/>
-      <c r="B85" s="198"/>
-      <c r="C85" s="201"/>
-      <c r="D85" s="237"/>
+    <row r="85" spans="1:45" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="207"/>
+      <c r="B85" s="320"/>
+      <c r="C85" s="323"/>
+      <c r="D85" s="315"/>
       <c r="E85" s="123"/>
       <c r="F85" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="G85" s="235"/>
+      <c r="G85" s="313"/>
       <c r="H85" s="124"/>
       <c r="I85" s="124">
         <v>12</v>
@@ -8157,7 +8329,7 @@
       <c r="L85" s="124"/>
       <c r="M85" s="124"/>
       <c r="N85" s="124"/>
-      <c r="O85" s="190"/>
+      <c r="O85" s="355"/>
       <c r="P85" s="9">
         <f t="shared" ref="P85:P87" si="90">SUM(H85:N85)</f>
         <v>12</v>
@@ -8180,8 +8352,8 @@
       <c r="AF85" s="3"/>
       <c r="AG85" s="3"/>
       <c r="AH85" s="3"/>
-      <c r="AI85" s="3" t="s">
-        <v>124</v>
+      <c r="AI85" s="189" t="s">
+        <v>160</v>
       </c>
       <c r="AJ85" s="3"/>
       <c r="AK85" s="3"/>
@@ -8194,16 +8366,16 @@
       <c r="AR85" s="3"/>
       <c r="AS85" s="3"/>
     </row>
-    <row r="86" spans="1:45" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="326"/>
-      <c r="B86" s="198"/>
-      <c r="C86" s="201"/>
-      <c r="D86" s="237"/>
+    <row r="86" spans="1:45" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="207"/>
+      <c r="B86" s="320"/>
+      <c r="C86" s="323"/>
+      <c r="D86" s="315"/>
       <c r="E86" s="123"/>
       <c r="F86" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="235"/>
+      <c r="G86" s="313"/>
       <c r="H86" s="124"/>
       <c r="I86" s="124">
         <v>12</v>
@@ -8213,7 +8385,7 @@
       <c r="L86" s="124"/>
       <c r="M86" s="124"/>
       <c r="N86" s="124"/>
-      <c r="O86" s="190"/>
+      <c r="O86" s="355"/>
       <c r="P86" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8236,8 +8408,8 @@
       <c r="AF86" s="3"/>
       <c r="AG86" s="3"/>
       <c r="AH86" s="3"/>
-      <c r="AI86" s="3" t="s">
-        <v>124</v>
+      <c r="AI86" s="189" t="s">
+        <v>161</v>
       </c>
       <c r="AJ86" s="3"/>
       <c r="AK86" s="3"/>
@@ -8251,15 +8423,15 @@
       <c r="AS86" s="3"/>
     </row>
     <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="327"/>
-      <c r="B87" s="198"/>
-      <c r="C87" s="201"/>
-      <c r="D87" s="237"/>
+      <c r="A87" s="208"/>
+      <c r="B87" s="320"/>
+      <c r="C87" s="323"/>
+      <c r="D87" s="315"/>
       <c r="E87" s="123"/>
       <c r="F87" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="235"/>
+      <c r="G87" s="313"/>
       <c r="H87" s="124"/>
       <c r="I87" s="124">
         <v>12</v>
@@ -8269,7 +8441,7 @@
       <c r="L87" s="124"/>
       <c r="M87" s="124"/>
       <c r="N87" s="124"/>
-      <c r="O87" s="190"/>
+      <c r="O87" s="355"/>
       <c r="P87" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8292,8 +8464,8 @@
       <c r="AF87" s="3"/>
       <c r="AG87" s="3"/>
       <c r="AH87" s="3"/>
-      <c r="AI87" s="3" t="s">
-        <v>124</v>
+      <c r="AI87" s="189" t="s">
+        <v>162</v>
       </c>
       <c r="AJ87" s="3"/>
       <c r="AK87" s="3"/>
@@ -8308,12 +8480,12 @@
     </row>
     <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
-      <c r="B88" s="198"/>
-      <c r="C88" s="201"/>
-      <c r="D88" s="228"/>
-      <c r="E88" s="229"/>
-      <c r="F88" s="229"/>
-      <c r="G88" s="229"/>
+      <c r="B88" s="320"/>
+      <c r="C88" s="323"/>
+      <c r="D88" s="306"/>
+      <c r="E88" s="307"/>
+      <c r="F88" s="307"/>
+      <c r="G88" s="307"/>
       <c r="H88" s="162">
         <f>SUM(H84:H87)</f>
         <v>0</v>
@@ -8362,7 +8534,7 @@
       <c r="AF88" s="2"/>
       <c r="AG88" s="2"/>
       <c r="AH88" s="2"/>
-      <c r="AI88" s="2"/>
+      <c r="AI88" s="189"/>
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
       <c r="AL88" s="2"/>
@@ -8376,8 +8548,8 @@
     </row>
     <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
-      <c r="B89" s="198"/>
-      <c r="C89" s="201"/>
+      <c r="B89" s="320"/>
+      <c r="C89" s="323"/>
       <c r="D89" s="122" t="s">
         <v>17</v>
       </c>
@@ -8429,8 +8601,8 @@
         <f>AG89/O89</f>
         <v>1</v>
       </c>
-      <c r="AI89" s="3" t="s">
-        <v>112</v>
+      <c r="AI89" s="363" t="s">
+        <v>163</v>
       </c>
       <c r="AJ89" s="3"/>
       <c r="AK89" s="3"/>
@@ -8445,12 +8617,12 @@
     </row>
     <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
-      <c r="B90" s="198"/>
-      <c r="C90" s="201"/>
-      <c r="D90" s="218"/>
-      <c r="E90" s="219"/>
-      <c r="F90" s="219"/>
-      <c r="G90" s="219"/>
+      <c r="B90" s="320"/>
+      <c r="C90" s="323"/>
+      <c r="D90" s="202"/>
+      <c r="E90" s="297"/>
+      <c r="F90" s="297"/>
+      <c r="G90" s="297"/>
       <c r="H90" s="140">
         <f t="shared" ref="H90:N90" si="97">SUM(H89:H89)</f>
         <v>48</v>
@@ -8577,31 +8749,90 @@
       </c>
     </row>
     <row r="97" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H97" s="202" t="s">
+      <c r="H97" s="296" t="s">
         <v>104</v>
       </c>
-      <c r="I97" s="202"/>
-      <c r="J97" s="202"/>
+      <c r="I97" s="296"/>
+      <c r="J97" s="296"/>
     </row>
     <row r="99" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="I99" s="202" t="s">
+      <c r="I99" s="296" t="s">
         <v>105</v>
       </c>
-      <c r="J99" s="202"/>
-      <c r="K99" s="202"/>
-      <c r="L99" s="202"/>
+      <c r="J99" s="296"/>
+      <c r="K99" s="296"/>
+      <c r="L99" s="296"/>
     </row>
     <row r="101" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="K101" s="202" t="s">
+      <c r="K101" s="296" t="s">
         <v>106</v>
       </c>
-      <c r="L101" s="202"/>
-      <c r="M101" s="202"/>
-      <c r="N101" s="202"/>
+      <c r="L101" s="296"/>
+      <c r="M101" s="296"/>
+      <c r="N101" s="296"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS91" xr:uid="{44B9DB88-0080-4900-9B58-5C638DC6AAB3}"/>
   <mergeCells count="75">
+    <mergeCell ref="O74:O77"/>
+    <mergeCell ref="O84:O87"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="O67:O72"/>
+    <mergeCell ref="B2:B90"/>
+    <mergeCell ref="C2:C90"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O52:O55"/>
+    <mergeCell ref="O57:O60"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="O32:O35"/>
+    <mergeCell ref="O37:O40"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="G12:G15"/>
     <mergeCell ref="D17:D20"/>
@@ -8618,65 +8849,6 @@
     <mergeCell ref="D37:D40"/>
     <mergeCell ref="G37:G40"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O52:O55"/>
-    <mergeCell ref="O57:O60"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="O32:O35"/>
-    <mergeCell ref="O37:O40"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="K101:N101"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="B2:B90"/>
-    <mergeCell ref="C2:C90"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="O74:O77"/>
-    <mergeCell ref="O84:O87"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="O67:O72"/>
   </mergeCells>
   <conditionalFormatting sqref="H93:N93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Nuevas Funciones para los cambios actuales
</commit_message>
<xml_diff>
--- a/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
+++ b/EjemploHorarios/Uploads/COMPETENCIAS GESTION REDES DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1234\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954DEF5B-471A-43E1-AE9E-CF714CCB191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59202FAA-919C-400B-A735-7B3603D4D67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE872B91-7A5E-45D1-BE70-0BA4C3B6BDED}"/>
   </bookViews>
@@ -1992,309 +1992,147 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2361,139 +2199,301 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2845,11 +2845,11 @@
   <dimension ref="A1:AS101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F38" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2993,16 +2993,16 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="322" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="321">
+      <c r="B2" s="208">
         <v>228183</v>
       </c>
-      <c r="C2" s="323">
+      <c r="C2" s="210">
         <v>2</v>
       </c>
-      <c r="D2" s="199" t="s">
+      <c r="D2" s="325" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
@@ -3011,7 +3011,7 @@
       <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="202">
+      <c r="G2" s="328">
         <v>528</v>
       </c>
       <c r="H2" s="12"/>
@@ -3023,7 +3023,7 @@
       <c r="N2" s="12">
         <v>72</v>
       </c>
-      <c r="O2" s="272">
+      <c r="O2" s="287">
         <f>SUM(P2:P5)</f>
         <v>528</v>
       </c>
@@ -3104,17 +3104,17 @@
       <c r="AS2" s="2"/>
     </row>
     <row r="3" spans="1:45" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="197"/>
-      <c r="B3" s="322"/>
-      <c r="C3" s="324"/>
-      <c r="D3" s="200"/>
+      <c r="A3" s="323"/>
+      <c r="B3" s="209"/>
+      <c r="C3" s="211"/>
+      <c r="D3" s="326"/>
       <c r="E3" s="13">
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="203"/>
+      <c r="G3" s="329"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -3124,7 +3124,7 @@
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="273"/>
+      <c r="O3" s="288"/>
       <c r="P3" s="9">
         <f>SUM(H3:N3)</f>
         <v>64</v>
@@ -3162,17 +3162,17 @@
       <c r="AS3" s="2"/>
     </row>
     <row r="4" spans="1:45" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="197"/>
-      <c r="B4" s="322"/>
-      <c r="C4" s="324"/>
-      <c r="D4" s="200"/>
+      <c r="A4" s="323"/>
+      <c r="B4" s="209"/>
+      <c r="C4" s="211"/>
+      <c r="D4" s="326"/>
       <c r="E4" s="13">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="203"/>
+      <c r="G4" s="329"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -3182,7 +3182,7 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="273"/>
+      <c r="O4" s="288"/>
       <c r="P4" s="9">
         <f>SUM(H4:N4)</f>
         <v>80</v>
@@ -3220,17 +3220,17 @@
       <c r="AS4" s="2"/>
     </row>
     <row r="5" spans="1:45" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="197"/>
-      <c r="B5" s="322"/>
-      <c r="C5" s="324"/>
-      <c r="D5" s="201"/>
+      <c r="A5" s="323"/>
+      <c r="B5" s="209"/>
+      <c r="C5" s="211"/>
+      <c r="D5" s="327"/>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="204"/>
+      <c r="G5" s="330"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -3244,7 +3244,7 @@
       <c r="N5" s="18">
         <v>168</v>
       </c>
-      <c r="O5" s="274"/>
+      <c r="O5" s="289"/>
       <c r="P5" s="9">
         <f>SUM(H5:N5)</f>
         <v>312</v>
@@ -3282,13 +3282,13 @@
       <c r="AS5" s="2"/>
     </row>
     <row r="6" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="197"/>
-      <c r="B6" s="322"/>
-      <c r="C6" s="324"/>
-      <c r="D6" s="326"/>
-      <c r="E6" s="327"/>
-      <c r="F6" s="327"/>
-      <c r="G6" s="328"/>
+      <c r="A6" s="323"/>
+      <c r="B6" s="209"/>
+      <c r="C6" s="211"/>
+      <c r="D6" s="214"/>
+      <c r="E6" s="215"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="216"/>
       <c r="H6" s="56">
         <f>SUM(H2:H5)</f>
         <v>0</v>
@@ -3350,10 +3350,10 @@
       <c r="AS6" s="2"/>
     </row>
     <row r="7" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="197"/>
-      <c r="B7" s="322"/>
-      <c r="C7" s="324"/>
-      <c r="D7" s="211" t="s">
+      <c r="A7" s="323"/>
+      <c r="B7" s="209"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="334" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="19">
@@ -3362,7 +3362,7 @@
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="214">
+      <c r="G7" s="337">
         <v>384</v>
       </c>
       <c r="H7" s="25"/>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="25"/>
-      <c r="O7" s="275">
+      <c r="O7" s="290">
         <f>SUM(P7:P10)</f>
         <v>384</v>
       </c>
@@ -3455,17 +3455,17 @@
       <c r="AS7" s="3"/>
     </row>
     <row r="8" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="197"/>
-      <c r="B8" s="322"/>
-      <c r="C8" s="324"/>
-      <c r="D8" s="212"/>
+      <c r="A8" s="323"/>
+      <c r="B8" s="209"/>
+      <c r="C8" s="211"/>
+      <c r="D8" s="335"/>
       <c r="E8" s="21">
         <v>3</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="215"/>
+      <c r="G8" s="338"/>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26"/>
@@ -3475,7 +3475,7 @@
         <v>144</v>
       </c>
       <c r="N8" s="26"/>
-      <c r="O8" s="276"/>
+      <c r="O8" s="291"/>
       <c r="P8" s="9">
         <f t="shared" ref="P8:P10" si="1">SUM(H8:N8)</f>
         <v>144</v>
@@ -3513,17 +3513,17 @@
       <c r="AS8" s="3"/>
     </row>
     <row r="9" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="197"/>
-      <c r="B9" s="322"/>
-      <c r="C9" s="324"/>
-      <c r="D9" s="212"/>
+      <c r="A9" s="323"/>
+      <c r="B9" s="209"/>
+      <c r="C9" s="211"/>
+      <c r="D9" s="335"/>
       <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="215"/>
+      <c r="G9" s="338"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="276"/>
+      <c r="O9" s="291"/>
       <c r="P9" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3571,17 +3571,17 @@
       <c r="AS9" s="3"/>
     </row>
     <row r="10" spans="1:45" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="197"/>
-      <c r="B10" s="322"/>
-      <c r="C10" s="324"/>
-      <c r="D10" s="213"/>
+      <c r="A10" s="323"/>
+      <c r="B10" s="209"/>
+      <c r="C10" s="211"/>
+      <c r="D10" s="336"/>
       <c r="E10" s="23">
         <v>4</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="216"/>
+      <c r="G10" s="339"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -3591,7 +3591,7 @@
       <c r="N10" s="27">
         <v>96</v>
       </c>
-      <c r="O10" s="277"/>
+      <c r="O10" s="292"/>
       <c r="P10" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3629,13 +3629,13 @@
       <c r="AS10" s="3"/>
     </row>
     <row r="11" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="197"/>
-      <c r="B11" s="322"/>
-      <c r="C11" s="324"/>
-      <c r="D11" s="329"/>
-      <c r="E11" s="330"/>
-      <c r="F11" s="330"/>
-      <c r="G11" s="331"/>
+      <c r="A11" s="323"/>
+      <c r="B11" s="209"/>
+      <c r="C11" s="211"/>
+      <c r="D11" s="217"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="219"/>
       <c r="H11" s="61">
         <f>SUM(H7:H10)</f>
         <v>0</v>
@@ -3697,17 +3697,17 @@
       <c r="AS11" s="2"/>
     </row>
     <row r="12" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="197"/>
-      <c r="B12" s="322"/>
-      <c r="C12" s="324"/>
-      <c r="D12" s="241" t="s">
+      <c r="A12" s="323"/>
+      <c r="B12" s="209"/>
+      <c r="C12" s="211"/>
+      <c r="D12" s="279" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="244">
+      <c r="G12" s="281">
         <v>48</v>
       </c>
       <c r="H12" s="34">
@@ -3719,7 +3719,7 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="278">
+      <c r="O12" s="276">
         <f t="shared" ref="O12" si="3">SUM(P12:P15)</f>
         <v>48</v>
       </c>
@@ -3786,15 +3786,15 @@
       </c>
     </row>
     <row r="13" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="197"/>
-      <c r="B13" s="322"/>
-      <c r="C13" s="324"/>
-      <c r="D13" s="242"/>
+      <c r="A13" s="323"/>
+      <c r="B13" s="209"/>
+      <c r="C13" s="211"/>
+      <c r="D13" s="241"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="245"/>
+      <c r="G13" s="282"/>
       <c r="H13" s="35">
         <v>12</v>
       </c>
@@ -3804,7 +3804,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="279"/>
+      <c r="O13" s="277"/>
       <c r="P13" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3832,15 +3832,15 @@
       </c>
     </row>
     <row r="14" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="197"/>
-      <c r="B14" s="322"/>
-      <c r="C14" s="324"/>
-      <c r="D14" s="242"/>
+      <c r="A14" s="323"/>
+      <c r="B14" s="209"/>
+      <c r="C14" s="211"/>
+      <c r="D14" s="241"/>
       <c r="E14" s="30"/>
       <c r="F14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="245"/>
+      <c r="G14" s="282"/>
       <c r="H14" s="35">
         <v>12</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="279"/>
+      <c r="O14" s="277"/>
       <c r="P14" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3878,15 +3878,15 @@
       </c>
     </row>
     <row r="15" spans="1:45" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="197"/>
-      <c r="B15" s="322"/>
-      <c r="C15" s="324"/>
-      <c r="D15" s="243"/>
+      <c r="A15" s="323"/>
+      <c r="B15" s="209"/>
+      <c r="C15" s="211"/>
+      <c r="D15" s="280"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="246"/>
+      <c r="G15" s="283"/>
       <c r="H15" s="36">
         <v>12</v>
       </c>
@@ -3896,7 +3896,7 @@
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
-      <c r="O15" s="280"/>
+      <c r="O15" s="278"/>
       <c r="P15" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -3924,13 +3924,13 @@
       </c>
     </row>
     <row r="16" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="197"/>
-      <c r="B16" s="322"/>
-      <c r="C16" s="324"/>
-      <c r="D16" s="326"/>
-      <c r="E16" s="327"/>
-      <c r="F16" s="327"/>
-      <c r="G16" s="328"/>
+      <c r="A16" s="323"/>
+      <c r="B16" s="209"/>
+      <c r="C16" s="211"/>
+      <c r="D16" s="214"/>
+      <c r="E16" s="215"/>
+      <c r="F16" s="215"/>
+      <c r="G16" s="216"/>
       <c r="H16" s="56">
         <f>SUM(H12:H15)</f>
         <v>48</v>
@@ -3992,17 +3992,17 @@
       <c r="AS16" s="2"/>
     </row>
     <row r="17" spans="1:45" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="197"/>
-      <c r="B17" s="322"/>
-      <c r="C17" s="324"/>
-      <c r="D17" s="247" t="s">
+      <c r="A17" s="323"/>
+      <c r="B17" s="209"/>
+      <c r="C17" s="211"/>
+      <c r="D17" s="314" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="250">
+      <c r="G17" s="316">
         <v>48</v>
       </c>
       <c r="H17" s="44"/>
@@ -4014,7 +4014,7 @@
       <c r="L17" s="44"/>
       <c r="M17" s="44"/>
       <c r="N17" s="44"/>
-      <c r="O17" s="281">
+      <c r="O17" s="293">
         <f t="shared" ref="O17" si="6">SUM(P17:P20)</f>
         <v>48</v>
       </c>
@@ -4091,15 +4091,15 @@
       <c r="AS17" s="3"/>
     </row>
     <row r="18" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="197"/>
-      <c r="B18" s="322"/>
-      <c r="C18" s="324"/>
-      <c r="D18" s="248"/>
+      <c r="A18" s="323"/>
+      <c r="B18" s="209"/>
+      <c r="C18" s="211"/>
+      <c r="D18" s="315"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="251"/>
+      <c r="G18" s="317"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45">
         <v>12</v>
@@ -4109,7 +4109,7 @@
       <c r="L18" s="45"/>
       <c r="M18" s="45"/>
       <c r="N18" s="45"/>
-      <c r="O18" s="282"/>
+      <c r="O18" s="294"/>
       <c r="P18" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4147,15 +4147,15 @@
       <c r="AS18" s="3"/>
     </row>
     <row r="19" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="197"/>
-      <c r="B19" s="322"/>
-      <c r="C19" s="324"/>
-      <c r="D19" s="248"/>
+      <c r="A19" s="323"/>
+      <c r="B19" s="209"/>
+      <c r="C19" s="211"/>
+      <c r="D19" s="315"/>
       <c r="E19" s="39"/>
       <c r="F19" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="251"/>
+      <c r="G19" s="317"/>
       <c r="H19" s="45"/>
       <c r="I19" s="45">
         <v>12</v>
@@ -4165,7 +4165,7 @@
       <c r="L19" s="45"/>
       <c r="M19" s="45"/>
       <c r="N19" s="45"/>
-      <c r="O19" s="282"/>
+      <c r="O19" s="294"/>
       <c r="P19" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4203,15 +4203,15 @@
       <c r="AS19" s="3"/>
     </row>
     <row r="20" spans="1:45" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="197"/>
-      <c r="B20" s="322"/>
-      <c r="C20" s="324"/>
-      <c r="D20" s="249"/>
+      <c r="A20" s="323"/>
+      <c r="B20" s="209"/>
+      <c r="C20" s="211"/>
+      <c r="D20" s="242"/>
       <c r="E20" s="41"/>
       <c r="F20" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="252"/>
+      <c r="G20" s="318"/>
       <c r="H20" s="46"/>
       <c r="I20" s="46">
         <v>12</v>
@@ -4221,7 +4221,7 @@
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
       <c r="N20" s="46"/>
-      <c r="O20" s="283"/>
+      <c r="O20" s="295"/>
       <c r="P20" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -4259,13 +4259,13 @@
       <c r="AS20" s="3"/>
     </row>
     <row r="21" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="197"/>
-      <c r="B21" s="322"/>
-      <c r="C21" s="324"/>
-      <c r="D21" s="332"/>
-      <c r="E21" s="333"/>
-      <c r="F21" s="333"/>
-      <c r="G21" s="334"/>
+      <c r="A21" s="323"/>
+      <c r="B21" s="209"/>
+      <c r="C21" s="211"/>
+      <c r="D21" s="220"/>
+      <c r="E21" s="221"/>
+      <c r="F21" s="221"/>
+      <c r="G21" s="222"/>
       <c r="H21" s="62">
         <f>SUM(H17:H20)</f>
         <v>0</v>
@@ -4327,10 +4327,10 @@
       <c r="AS21" s="2"/>
     </row>
     <row r="22" spans="1:45" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="197"/>
-      <c r="B22" s="322"/>
-      <c r="C22" s="324"/>
-      <c r="D22" s="205" t="s">
+      <c r="A22" s="323"/>
+      <c r="B22" s="209"/>
+      <c r="C22" s="211"/>
+      <c r="D22" s="331" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="47">
@@ -4339,7 +4339,7 @@
       <c r="F22" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="208">
+      <c r="G22" s="305">
         <v>336</v>
       </c>
       <c r="H22" s="53"/>
@@ -4349,7 +4349,7 @@
       <c r="L22" s="53"/>
       <c r="M22" s="53"/>
       <c r="N22" s="53"/>
-      <c r="O22" s="267">
+      <c r="O22" s="296">
         <f t="shared" ref="O22" si="13">SUM(P22:P25)</f>
         <v>336</v>
       </c>
@@ -4436,17 +4436,17 @@
       <c r="AS22" s="3"/>
     </row>
     <row r="23" spans="1:45" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="197"/>
-      <c r="B23" s="322"/>
-      <c r="C23" s="324"/>
-      <c r="D23" s="206"/>
+      <c r="A23" s="323"/>
+      <c r="B23" s="209"/>
+      <c r="C23" s="211"/>
+      <c r="D23" s="332"/>
       <c r="E23" s="49">
         <v>2</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="209"/>
+      <c r="G23" s="306"/>
       <c r="H23" s="54">
         <v>72</v>
       </c>
@@ -4456,7 +4456,7 @@
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
-      <c r="O23" s="268"/>
+      <c r="O23" s="297"/>
       <c r="P23" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4494,17 +4494,17 @@
       <c r="AS23" s="3"/>
     </row>
     <row r="24" spans="1:45" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="197"/>
-      <c r="B24" s="322"/>
-      <c r="C24" s="324"/>
-      <c r="D24" s="206"/>
+      <c r="A24" s="323"/>
+      <c r="B24" s="209"/>
+      <c r="C24" s="211"/>
+      <c r="D24" s="332"/>
       <c r="E24" s="49">
         <v>1</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="209"/>
+      <c r="G24" s="306"/>
       <c r="H24" s="54">
         <v>72</v>
       </c>
@@ -4514,7 +4514,7 @@
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
-      <c r="O24" s="268"/>
+      <c r="O24" s="297"/>
       <c r="P24" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4552,17 +4552,17 @@
       <c r="AS24" s="3"/>
     </row>
     <row r="25" spans="1:45" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="197"/>
-      <c r="B25" s="322"/>
-      <c r="C25" s="324"/>
-      <c r="D25" s="207"/>
+      <c r="A25" s="323"/>
+      <c r="B25" s="209"/>
+      <c r="C25" s="211"/>
+      <c r="D25" s="333"/>
       <c r="E25" s="51">
         <v>3</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="210"/>
+      <c r="G25" s="307"/>
       <c r="H25" s="55"/>
       <c r="I25" s="55">
         <v>72</v>
@@ -4574,7 +4574,7 @@
       <c r="L25" s="55"/>
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
-      <c r="O25" s="269"/>
+      <c r="O25" s="298"/>
       <c r="P25" s="9">
         <f t="shared" si="4"/>
         <v>192</v>
@@ -4612,13 +4612,13 @@
       <c r="AS25" s="3"/>
     </row>
     <row r="26" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="197"/>
-      <c r="B26" s="322"/>
-      <c r="C26" s="324"/>
-      <c r="D26" s="335"/>
-      <c r="E26" s="336"/>
-      <c r="F26" s="336"/>
-      <c r="G26" s="337"/>
+      <c r="A26" s="323"/>
+      <c r="B26" s="209"/>
+      <c r="C26" s="211"/>
+      <c r="D26" s="223"/>
+      <c r="E26" s="224"/>
+      <c r="F26" s="224"/>
+      <c r="G26" s="225"/>
       <c r="H26" s="64">
         <f>SUM(H22:H25)</f>
         <v>144</v>
@@ -4680,10 +4680,10 @@
       <c r="AS26" s="2"/>
     </row>
     <row r="27" spans="1:45" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="197"/>
-      <c r="B27" s="322"/>
-      <c r="C27" s="324"/>
-      <c r="D27" s="229" t="s">
+      <c r="A27" s="323"/>
+      <c r="B27" s="209"/>
+      <c r="C27" s="211"/>
+      <c r="D27" s="352" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="65">
@@ -4692,7 +4692,7 @@
       <c r="F27" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="G27" s="217">
+      <c r="G27" s="340">
         <v>576</v>
       </c>
       <c r="H27" s="73"/>
@@ -4704,7 +4704,7 @@
         <v>72</v>
       </c>
       <c r="N27" s="73"/>
-      <c r="O27" s="284">
+      <c r="O27" s="267">
         <f t="shared" ref="O27" si="20">SUM(P27:P30)</f>
         <v>576</v>
       </c>
@@ -4791,17 +4791,17 @@
       <c r="AS27" s="3"/>
     </row>
     <row r="28" spans="1:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="197"/>
-      <c r="B28" s="322"/>
-      <c r="C28" s="324"/>
-      <c r="D28" s="230"/>
+      <c r="A28" s="323"/>
+      <c r="B28" s="209"/>
+      <c r="C28" s="211"/>
+      <c r="D28" s="353"/>
       <c r="E28" s="67">
         <v>2</v>
       </c>
       <c r="F28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="218"/>
+      <c r="G28" s="341"/>
       <c r="H28" s="74"/>
       <c r="I28" s="74">
         <v>72</v>
@@ -4811,7 +4811,7 @@
       <c r="L28" s="74"/>
       <c r="M28" s="74"/>
       <c r="N28" s="74"/>
-      <c r="O28" s="285"/>
+      <c r="O28" s="268"/>
       <c r="P28" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4849,17 +4849,17 @@
       <c r="AS28" s="3"/>
     </row>
     <row r="29" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="197"/>
-      <c r="B29" s="322"/>
-      <c r="C29" s="324"/>
-      <c r="D29" s="230"/>
+      <c r="A29" s="323"/>
+      <c r="B29" s="209"/>
+      <c r="C29" s="211"/>
+      <c r="D29" s="353"/>
       <c r="E29" s="67">
         <v>1</v>
       </c>
       <c r="F29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="218"/>
+      <c r="G29" s="341"/>
       <c r="H29" s="74">
         <v>72</v>
       </c>
@@ -4869,7 +4869,7 @@
       <c r="L29" s="74"/>
       <c r="M29" s="74"/>
       <c r="N29" s="74"/>
-      <c r="O29" s="285"/>
+      <c r="O29" s="268"/>
       <c r="P29" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -4907,17 +4907,17 @@
       <c r="AS29" s="3"/>
     </row>
     <row r="30" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="197"/>
-      <c r="B30" s="322"/>
-      <c r="C30" s="324"/>
-      <c r="D30" s="231"/>
+      <c r="A30" s="323"/>
+      <c r="B30" s="209"/>
+      <c r="C30" s="211"/>
+      <c r="D30" s="354"/>
       <c r="E30" s="69">
         <v>3</v>
       </c>
       <c r="F30" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="219"/>
+      <c r="G30" s="342"/>
       <c r="H30" s="75"/>
       <c r="I30" s="75">
         <v>72</v>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="M30" s="75"/>
       <c r="N30" s="75"/>
-      <c r="O30" s="286"/>
+      <c r="O30" s="269"/>
       <c r="P30" s="9">
         <f t="shared" si="4"/>
         <v>360</v>
@@ -4971,13 +4971,13 @@
       <c r="AS30" s="3"/>
     </row>
     <row r="31" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="197"/>
-      <c r="B31" s="322"/>
-      <c r="C31" s="324"/>
-      <c r="D31" s="338"/>
-      <c r="E31" s="339"/>
-      <c r="F31" s="339"/>
-      <c r="G31" s="340"/>
+      <c r="A31" s="323"/>
+      <c r="B31" s="209"/>
+      <c r="C31" s="211"/>
+      <c r="D31" s="226"/>
+      <c r="E31" s="227"/>
+      <c r="F31" s="227"/>
+      <c r="G31" s="228"/>
       <c r="H31" s="71">
         <f>SUM(H27:H30)</f>
         <v>72</v>
@@ -5039,17 +5039,17 @@
       <c r="AS31" s="2"/>
     </row>
     <row r="32" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="197"/>
-      <c r="B32" s="322"/>
-      <c r="C32" s="324"/>
-      <c r="D32" s="293" t="s">
+      <c r="A32" s="323"/>
+      <c r="B32" s="209"/>
+      <c r="C32" s="211"/>
+      <c r="D32" s="284" t="s">
         <v>44</v>
       </c>
       <c r="E32" s="76"/>
       <c r="F32" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="220">
+      <c r="G32" s="343">
         <v>48</v>
       </c>
       <c r="H32" s="82"/>
@@ -5061,7 +5061,7 @@
         <v>12</v>
       </c>
       <c r="N32" s="82"/>
-      <c r="O32" s="287">
+      <c r="O32" s="270">
         <f t="shared" ref="O32" si="27">SUM(P32:P35)</f>
         <v>48</v>
       </c>
@@ -5128,15 +5128,15 @@
       </c>
     </row>
     <row r="33" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="197"/>
-      <c r="B33" s="322"/>
-      <c r="C33" s="324"/>
-      <c r="D33" s="294"/>
+      <c r="A33" s="323"/>
+      <c r="B33" s="209"/>
+      <c r="C33" s="211"/>
+      <c r="D33" s="285"/>
       <c r="E33" s="78"/>
       <c r="F33" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="221"/>
+      <c r="G33" s="344"/>
       <c r="H33" s="83"/>
       <c r="I33" s="83"/>
       <c r="J33" s="83"/>
@@ -5146,7 +5146,7 @@
         <v>12</v>
       </c>
       <c r="N33" s="83"/>
-      <c r="O33" s="288"/>
+      <c r="O33" s="271"/>
       <c r="P33" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5174,15 +5174,15 @@
       </c>
     </row>
     <row r="34" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="197"/>
-      <c r="B34" s="322"/>
-      <c r="C34" s="324"/>
-      <c r="D34" s="294"/>
+      <c r="A34" s="323"/>
+      <c r="B34" s="209"/>
+      <c r="C34" s="211"/>
+      <c r="D34" s="285"/>
       <c r="E34" s="78"/>
       <c r="F34" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="221"/>
+      <c r="G34" s="344"/>
       <c r="H34" s="83"/>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -5192,7 +5192,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="83"/>
-      <c r="O34" s="288"/>
+      <c r="O34" s="271"/>
       <c r="P34" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5220,15 +5220,15 @@
       </c>
     </row>
     <row r="35" spans="1:45" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="197"/>
-      <c r="B35" s="322"/>
-      <c r="C35" s="324"/>
-      <c r="D35" s="295"/>
+      <c r="A35" s="323"/>
+      <c r="B35" s="209"/>
+      <c r="C35" s="211"/>
+      <c r="D35" s="286"/>
       <c r="E35" s="80"/>
       <c r="F35" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="222"/>
+      <c r="G35" s="345"/>
       <c r="H35" s="84"/>
       <c r="I35" s="84"/>
       <c r="J35" s="84"/>
@@ -5238,7 +5238,7 @@
         <v>12</v>
       </c>
       <c r="N35" s="84"/>
-      <c r="O35" s="289"/>
+      <c r="O35" s="272"/>
       <c r="P35" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5266,13 +5266,13 @@
       </c>
     </row>
     <row r="36" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="197"/>
-      <c r="B36" s="322"/>
-      <c r="C36" s="324"/>
-      <c r="D36" s="341"/>
-      <c r="E36" s="342"/>
-      <c r="F36" s="342"/>
-      <c r="G36" s="343"/>
+      <c r="A36" s="323"/>
+      <c r="B36" s="209"/>
+      <c r="C36" s="211"/>
+      <c r="D36" s="229"/>
+      <c r="E36" s="230"/>
+      <c r="F36" s="230"/>
+      <c r="G36" s="231"/>
       <c r="H36" s="86">
         <f>SUM(H32:H35)</f>
         <v>0</v>
@@ -5334,17 +5334,17 @@
       <c r="AS36" s="2"/>
     </row>
     <row r="37" spans="1:45" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="197"/>
-      <c r="B37" s="322"/>
-      <c r="C37" s="324"/>
-      <c r="D37" s="223" t="s">
+      <c r="A37" s="323"/>
+      <c r="B37" s="209"/>
+      <c r="C37" s="211"/>
+      <c r="D37" s="346" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="87"/>
       <c r="F37" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="226">
+      <c r="G37" s="349">
         <v>48</v>
       </c>
       <c r="H37" s="95"/>
@@ -5356,7 +5356,7 @@
       <c r="N37" s="95">
         <v>12</v>
       </c>
-      <c r="O37" s="290">
+      <c r="O37" s="273">
         <f t="shared" ref="O37" si="34">SUM(P37:P40)</f>
         <v>48</v>
       </c>
@@ -5409,15 +5409,15 @@
       <c r="AS37" s="3"/>
     </row>
     <row r="38" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="197"/>
-      <c r="B38" s="322"/>
-      <c r="C38" s="324"/>
-      <c r="D38" s="224"/>
+      <c r="A38" s="323"/>
+      <c r="B38" s="209"/>
+      <c r="C38" s="211"/>
+      <c r="D38" s="347"/>
       <c r="E38" s="89"/>
       <c r="F38" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="227"/>
+      <c r="G38" s="350"/>
       <c r="H38" s="96"/>
       <c r="I38" s="96"/>
       <c r="J38" s="96"/>
@@ -5427,7 +5427,7 @@
       <c r="N38" s="96">
         <v>12</v>
       </c>
-      <c r="O38" s="291"/>
+      <c r="O38" s="274"/>
       <c r="P38" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5465,15 +5465,15 @@
       <c r="AS38" s="3"/>
     </row>
     <row r="39" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="197"/>
-      <c r="B39" s="322"/>
-      <c r="C39" s="324"/>
-      <c r="D39" s="224"/>
+      <c r="A39" s="323"/>
+      <c r="B39" s="209"/>
+      <c r="C39" s="211"/>
+      <c r="D39" s="347"/>
       <c r="E39" s="89"/>
       <c r="F39" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="227"/>
+      <c r="G39" s="350"/>
       <c r="H39" s="96"/>
       <c r="I39" s="96"/>
       <c r="J39" s="96"/>
@@ -5483,7 +5483,7 @@
       <c r="N39" s="96">
         <v>12</v>
       </c>
-      <c r="O39" s="291"/>
+      <c r="O39" s="274"/>
       <c r="P39" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5521,15 +5521,15 @@
       <c r="AS39" s="3"/>
     </row>
     <row r="40" spans="1:45" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="197"/>
-      <c r="B40" s="322"/>
-      <c r="C40" s="324"/>
-      <c r="D40" s="225"/>
+      <c r="A40" s="323"/>
+      <c r="B40" s="209"/>
+      <c r="C40" s="211"/>
+      <c r="D40" s="348"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="228"/>
+      <c r="G40" s="351"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
       <c r="J40" s="97"/>
@@ -5539,7 +5539,7 @@
       <c r="N40" s="97">
         <v>12</v>
       </c>
-      <c r="O40" s="292"/>
+      <c r="O40" s="275"/>
       <c r="P40" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5577,13 +5577,13 @@
       <c r="AS40" s="3"/>
     </row>
     <row r="41" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="197"/>
-      <c r="B41" s="322"/>
-      <c r="C41" s="324"/>
-      <c r="D41" s="344"/>
-      <c r="E41" s="345"/>
-      <c r="F41" s="345"/>
-      <c r="G41" s="346"/>
+      <c r="A41" s="323"/>
+      <c r="B41" s="209"/>
+      <c r="C41" s="211"/>
+      <c r="D41" s="232"/>
+      <c r="E41" s="233"/>
+      <c r="F41" s="233"/>
+      <c r="G41" s="234"/>
       <c r="H41" s="93">
         <f>SUM(H37:H40)</f>
         <v>0</v>
@@ -5645,17 +5645,17 @@
       <c r="AS41" s="2"/>
     </row>
     <row r="42" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="197"/>
-      <c r="B42" s="322"/>
-      <c r="C42" s="324"/>
-      <c r="D42" s="241" t="s">
+      <c r="A42" s="323"/>
+      <c r="B42" s="209"/>
+      <c r="C42" s="211"/>
+      <c r="D42" s="279" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="244">
+      <c r="G42" s="281">
         <v>48</v>
       </c>
       <c r="H42" s="34">
@@ -5667,7 +5667,7 @@
       <c r="L42" s="34"/>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
-      <c r="O42" s="278">
+      <c r="O42" s="276">
         <f t="shared" ref="O42" si="41">SUM(P42:P45)</f>
         <v>48</v>
       </c>
@@ -5720,15 +5720,15 @@
       <c r="AS42" s="3"/>
     </row>
     <row r="43" spans="1:45" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="197"/>
-      <c r="B43" s="322"/>
-      <c r="C43" s="324"/>
-      <c r="D43" s="242"/>
+      <c r="A43" s="323"/>
+      <c r="B43" s="209"/>
+      <c r="C43" s="211"/>
+      <c r="D43" s="241"/>
       <c r="E43" s="30"/>
       <c r="F43" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="245"/>
+      <c r="G43" s="282"/>
       <c r="H43" s="35">
         <v>12</v>
       </c>
@@ -5738,7 +5738,7 @@
       <c r="L43" s="35"/>
       <c r="M43" s="35"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="279"/>
+      <c r="O43" s="277"/>
       <c r="P43" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5776,15 +5776,15 @@
       <c r="AS43" s="3"/>
     </row>
     <row r="44" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="197"/>
-      <c r="B44" s="322"/>
-      <c r="C44" s="324"/>
-      <c r="D44" s="242"/>
+      <c r="A44" s="323"/>
+      <c r="B44" s="209"/>
+      <c r="C44" s="211"/>
+      <c r="D44" s="241"/>
       <c r="E44" s="30"/>
       <c r="F44" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="245"/>
+      <c r="G44" s="282"/>
       <c r="H44" s="35">
         <v>12</v>
       </c>
@@ -5794,7 +5794,7 @@
       <c r="L44" s="35"/>
       <c r="M44" s="35"/>
       <c r="N44" s="35"/>
-      <c r="O44" s="279"/>
+      <c r="O44" s="277"/>
       <c r="P44" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5832,15 +5832,15 @@
       <c r="AS44" s="3"/>
     </row>
     <row r="45" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="197"/>
-      <c r="B45" s="322"/>
-      <c r="C45" s="324"/>
-      <c r="D45" s="243"/>
+      <c r="A45" s="323"/>
+      <c r="B45" s="209"/>
+      <c r="C45" s="211"/>
+      <c r="D45" s="280"/>
       <c r="E45" s="32"/>
       <c r="F45" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="246"/>
+      <c r="G45" s="283"/>
       <c r="H45" s="36">
         <v>12</v>
       </c>
@@ -5850,7 +5850,7 @@
       <c r="L45" s="36"/>
       <c r="M45" s="36"/>
       <c r="N45" s="36"/>
-      <c r="O45" s="280"/>
+      <c r="O45" s="278"/>
       <c r="P45" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -5888,13 +5888,13 @@
       <c r="AS45" s="3"/>
     </row>
     <row r="46" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="197"/>
-      <c r="B46" s="322"/>
-      <c r="C46" s="324"/>
-      <c r="D46" s="232"/>
-      <c r="E46" s="233"/>
-      <c r="F46" s="233"/>
-      <c r="G46" s="234"/>
+      <c r="A46" s="323"/>
+      <c r="B46" s="209"/>
+      <c r="C46" s="211"/>
+      <c r="D46" s="355"/>
+      <c r="E46" s="356"/>
+      <c r="F46" s="356"/>
+      <c r="G46" s="357"/>
       <c r="H46" s="98">
         <f>SUM(H42:H45)</f>
         <v>48</v>
@@ -5956,17 +5956,17 @@
       <c r="AS46" s="2"/>
     </row>
     <row r="47" spans="1:45" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="197"/>
-      <c r="B47" s="322"/>
-      <c r="C47" s="324"/>
-      <c r="D47" s="238" t="s">
+      <c r="A47" s="323"/>
+      <c r="B47" s="209"/>
+      <c r="C47" s="211"/>
+      <c r="D47" s="361" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="99"/>
       <c r="F47" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="261">
+      <c r="G47" s="302">
         <v>48</v>
       </c>
       <c r="H47" s="107"/>
@@ -5978,7 +5978,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="107"/>
       <c r="N47" s="107"/>
-      <c r="O47" s="264">
+      <c r="O47" s="308">
         <f t="shared" ref="O47" si="48">SUM(P47:P50)</f>
         <v>48</v>
       </c>
@@ -6021,15 +6021,15 @@
       </c>
     </row>
     <row r="48" spans="1:45" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="197"/>
-      <c r="B48" s="322"/>
-      <c r="C48" s="324"/>
-      <c r="D48" s="239"/>
+      <c r="A48" s="323"/>
+      <c r="B48" s="209"/>
+      <c r="C48" s="211"/>
+      <c r="D48" s="362"/>
       <c r="E48" s="101"/>
       <c r="F48" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="262"/>
+      <c r="G48" s="303"/>
       <c r="H48" s="108"/>
       <c r="I48" s="108">
         <v>12</v>
@@ -6039,7 +6039,7 @@
       <c r="L48" s="108"/>
       <c r="M48" s="108"/>
       <c r="N48" s="108"/>
-      <c r="O48" s="265"/>
+      <c r="O48" s="309"/>
       <c r="P48" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6067,15 +6067,15 @@
       </c>
     </row>
     <row r="49" spans="1:45" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="197"/>
-      <c r="B49" s="322"/>
-      <c r="C49" s="324"/>
-      <c r="D49" s="239"/>
+      <c r="A49" s="323"/>
+      <c r="B49" s="209"/>
+      <c r="C49" s="211"/>
+      <c r="D49" s="362"/>
       <c r="E49" s="101"/>
       <c r="F49" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="262"/>
+      <c r="G49" s="303"/>
       <c r="H49" s="108"/>
       <c r="I49" s="108">
         <v>12</v>
@@ -6085,7 +6085,7 @@
       <c r="L49" s="108"/>
       <c r="M49" s="108"/>
       <c r="N49" s="108"/>
-      <c r="O49" s="265"/>
+      <c r="O49" s="309"/>
       <c r="P49" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6113,15 +6113,15 @@
       </c>
     </row>
     <row r="50" spans="1:45" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="197"/>
-      <c r="B50" s="322"/>
-      <c r="C50" s="324"/>
-      <c r="D50" s="240"/>
+      <c r="A50" s="323"/>
+      <c r="B50" s="209"/>
+      <c r="C50" s="211"/>
+      <c r="D50" s="363"/>
       <c r="E50" s="103"/>
       <c r="F50" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="G50" s="263"/>
+      <c r="G50" s="304"/>
       <c r="H50" s="109"/>
       <c r="I50" s="109">
         <v>12</v>
@@ -6131,7 +6131,7 @@
       <c r="L50" s="109"/>
       <c r="M50" s="109"/>
       <c r="N50" s="109"/>
-      <c r="O50" s="266"/>
+      <c r="O50" s="310"/>
       <c r="P50" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6159,13 +6159,13 @@
       </c>
     </row>
     <row r="51" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="197"/>
-      <c r="B51" s="322"/>
-      <c r="C51" s="324"/>
-      <c r="D51" s="235"/>
-      <c r="E51" s="236"/>
-      <c r="F51" s="236"/>
-      <c r="G51" s="237"/>
+      <c r="A51" s="323"/>
+      <c r="B51" s="209"/>
+      <c r="C51" s="211"/>
+      <c r="D51" s="358"/>
+      <c r="E51" s="359"/>
+      <c r="F51" s="359"/>
+      <c r="G51" s="360"/>
       <c r="H51" s="106">
         <f>SUM(H47:H50)</f>
         <v>0</v>
@@ -6227,17 +6227,17 @@
       <c r="AS51" s="2"/>
     </row>
     <row r="52" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="197"/>
-      <c r="B52" s="322"/>
-      <c r="C52" s="324"/>
-      <c r="D52" s="205" t="s">
+      <c r="A52" s="323"/>
+      <c r="B52" s="209"/>
+      <c r="C52" s="211"/>
+      <c r="D52" s="331" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="47"/>
       <c r="F52" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G52" s="208">
+      <c r="G52" s="305">
         <v>48</v>
       </c>
       <c r="H52" s="53"/>
@@ -6249,7 +6249,7 @@
       <c r="N52" s="53">
         <v>12</v>
       </c>
-      <c r="O52" s="267">
+      <c r="O52" s="296">
         <f t="shared" ref="O52" si="55">SUM(P52:P55)</f>
         <v>48</v>
       </c>
@@ -6302,15 +6302,15 @@
       <c r="AS52" s="3"/>
     </row>
     <row r="53" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="197"/>
-      <c r="B53" s="322"/>
-      <c r="C53" s="324"/>
-      <c r="D53" s="206"/>
+      <c r="A53" s="323"/>
+      <c r="B53" s="209"/>
+      <c r="C53" s="211"/>
+      <c r="D53" s="332"/>
       <c r="E53" s="49"/>
       <c r="F53" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G53" s="209"/>
+      <c r="G53" s="306"/>
       <c r="H53" s="54"/>
       <c r="I53" s="54"/>
       <c r="J53" s="54"/>
@@ -6320,7 +6320,7 @@
       <c r="N53" s="54">
         <v>12</v>
       </c>
-      <c r="O53" s="268"/>
+      <c r="O53" s="297"/>
       <c r="P53" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6358,15 +6358,15 @@
       <c r="AS53" s="3"/>
     </row>
     <row r="54" spans="1:45" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="197"/>
-      <c r="B54" s="322"/>
-      <c r="C54" s="324"/>
-      <c r="D54" s="206"/>
+      <c r="A54" s="323"/>
+      <c r="B54" s="209"/>
+      <c r="C54" s="211"/>
+      <c r="D54" s="332"/>
       <c r="E54" s="49"/>
       <c r="F54" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G54" s="209"/>
+      <c r="G54" s="306"/>
       <c r="H54" s="54"/>
       <c r="I54" s="54"/>
       <c r="J54" s="54"/>
@@ -6376,7 +6376,7 @@
       <c r="N54" s="54">
         <v>12</v>
       </c>
-      <c r="O54" s="268"/>
+      <c r="O54" s="297"/>
       <c r="P54" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6414,15 +6414,15 @@
       <c r="AS54" s="3"/>
     </row>
     <row r="55" spans="1:45" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="197"/>
-      <c r="B55" s="322"/>
-      <c r="C55" s="324"/>
-      <c r="D55" s="207"/>
+      <c r="A55" s="323"/>
+      <c r="B55" s="209"/>
+      <c r="C55" s="211"/>
+      <c r="D55" s="333"/>
       <c r="E55" s="51"/>
       <c r="F55" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="210"/>
+      <c r="G55" s="307"/>
       <c r="H55" s="55"/>
       <c r="I55" s="55"/>
       <c r="J55" s="55"/>
@@ -6432,7 +6432,7 @@
       <c r="N55" s="55">
         <v>12</v>
       </c>
-      <c r="O55" s="269"/>
+      <c r="O55" s="298"/>
       <c r="P55" s="9">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -6470,13 +6470,13 @@
       <c r="AS55" s="3"/>
     </row>
     <row r="56" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="197"/>
-      <c r="B56" s="322"/>
-      <c r="C56" s="324"/>
-      <c r="D56" s="347"/>
-      <c r="E56" s="348"/>
-      <c r="F56" s="348"/>
-      <c r="G56" s="349"/>
+      <c r="A56" s="323"/>
+      <c r="B56" s="209"/>
+      <c r="C56" s="211"/>
+      <c r="D56" s="235"/>
+      <c r="E56" s="236"/>
+      <c r="F56" s="236"/>
+      <c r="G56" s="237"/>
       <c r="H56" s="64">
         <f>SUM(H52:H55)</f>
         <v>0</v>
@@ -6538,10 +6538,10 @@
       <c r="AS56" s="2"/>
     </row>
     <row r="57" spans="1:45" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="197"/>
-      <c r="B57" s="322"/>
-      <c r="C57" s="324"/>
-      <c r="D57" s="253" t="s">
+      <c r="A57" s="323"/>
+      <c r="B57" s="209"/>
+      <c r="C57" s="211"/>
+      <c r="D57" s="319" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="149">
@@ -6550,7 +6550,7 @@
       <c r="F57" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="255">
+      <c r="G57" s="320">
         <v>96</v>
       </c>
       <c r="H57" s="114"/>
@@ -6562,7 +6562,7 @@
       <c r="L57" s="114"/>
       <c r="M57" s="114"/>
       <c r="N57" s="114"/>
-      <c r="O57" s="270">
+      <c r="O57" s="311">
         <f t="shared" ref="O57" si="62">SUM(P57:P60)</f>
         <v>96</v>
       </c>
@@ -6640,17 +6640,17 @@
       <c r="AS57" s="3"/>
     </row>
     <row r="58" spans="1:45" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="197"/>
-      <c r="B58" s="322"/>
-      <c r="C58" s="324"/>
-      <c r="D58" s="254"/>
+      <c r="A58" s="323"/>
+      <c r="B58" s="209"/>
+      <c r="C58" s="211"/>
+      <c r="D58" s="265"/>
       <c r="E58" s="145">
         <v>2</v>
       </c>
       <c r="F58" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="G58" s="256"/>
+      <c r="G58" s="321"/>
       <c r="H58" s="115"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115">
@@ -6660,7 +6660,7 @@
       <c r="L58" s="115"/>
       <c r="M58" s="115"/>
       <c r="N58" s="115"/>
-      <c r="O58" s="271"/>
+      <c r="O58" s="312"/>
       <c r="P58" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -6698,17 +6698,17 @@
       <c r="AS58" s="7"/>
     </row>
     <row r="59" spans="1:45" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="197"/>
-      <c r="B59" s="322"/>
-      <c r="C59" s="324"/>
-      <c r="D59" s="254"/>
+      <c r="A59" s="323"/>
+      <c r="B59" s="209"/>
+      <c r="C59" s="211"/>
+      <c r="D59" s="265"/>
       <c r="E59" s="145">
         <v>4</v>
       </c>
       <c r="F59" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="G59" s="256"/>
+      <c r="G59" s="321"/>
       <c r="H59" s="115"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115">
@@ -6718,7 +6718,7 @@
       <c r="L59" s="115"/>
       <c r="M59" s="115"/>
       <c r="N59" s="115"/>
-      <c r="O59" s="271"/>
+      <c r="O59" s="312"/>
       <c r="P59" s="9">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -6756,17 +6756,17 @@
       <c r="AS59" s="7"/>
     </row>
     <row r="60" spans="1:45" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="197"/>
-      <c r="B60" s="322"/>
-      <c r="C60" s="324"/>
-      <c r="D60" s="254"/>
+      <c r="A60" s="323"/>
+      <c r="B60" s="209"/>
+      <c r="C60" s="211"/>
+      <c r="D60" s="265"/>
       <c r="E60" s="145">
         <v>1</v>
       </c>
       <c r="F60" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="G60" s="256"/>
+      <c r="G60" s="321"/>
       <c r="H60" s="115"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115">
@@ -6776,7 +6776,7 @@
       <c r="L60" s="115"/>
       <c r="M60" s="115"/>
       <c r="N60" s="115"/>
-      <c r="O60" s="271"/>
+      <c r="O60" s="312"/>
       <c r="P60" s="9">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -6814,13 +6814,13 @@
       <c r="AS60" s="7"/>
     </row>
     <row r="61" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="197"/>
-      <c r="B61" s="322"/>
-      <c r="C61" s="324"/>
-      <c r="D61" s="257"/>
-      <c r="E61" s="258"/>
-      <c r="F61" s="258"/>
-      <c r="G61" s="258"/>
+      <c r="A61" s="323"/>
+      <c r="B61" s="209"/>
+      <c r="C61" s="211"/>
+      <c r="D61" s="266"/>
+      <c r="E61" s="299"/>
+      <c r="F61" s="299"/>
+      <c r="G61" s="299"/>
       <c r="H61" s="150">
         <f>SUM(H57:H60)</f>
         <v>0</v>
@@ -6882,10 +6882,10 @@
       <c r="AS61" s="2"/>
     </row>
     <row r="62" spans="1:45" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="197"/>
-      <c r="B62" s="322"/>
-      <c r="C62" s="324"/>
-      <c r="D62" s="352" t="s">
+      <c r="A62" s="323"/>
+      <c r="B62" s="209"/>
+      <c r="C62" s="211"/>
+      <c r="D62" s="240" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="142">
@@ -6894,7 +6894,7 @@
       <c r="F62" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="G62" s="353">
+      <c r="G62" s="313">
         <v>288</v>
       </c>
       <c r="H62" s="132"/>
@@ -6906,7 +6906,7 @@
         <v>72</v>
       </c>
       <c r="N62" s="132"/>
-      <c r="O62" s="360">
+      <c r="O62" s="202">
         <f t="shared" ref="O62" si="69">SUM(P62:P65)</f>
         <v>288</v>
       </c>
@@ -6982,17 +6982,17 @@
       <c r="AS62" s="3"/>
     </row>
     <row r="63" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="197"/>
-      <c r="B63" s="322"/>
-      <c r="C63" s="324"/>
-      <c r="D63" s="242"/>
+      <c r="A63" s="323"/>
+      <c r="B63" s="209"/>
+      <c r="C63" s="211"/>
+      <c r="D63" s="241"/>
       <c r="E63" s="116">
         <v>1</v>
       </c>
       <c r="F63" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="245"/>
+      <c r="G63" s="282"/>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
@@ -7002,7 +7002,7 @@
       <c r="L63" s="35"/>
       <c r="M63" s="35"/>
       <c r="N63" s="35"/>
-      <c r="O63" s="361"/>
+      <c r="O63" s="203"/>
       <c r="P63" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7040,17 +7040,17 @@
       <c r="AS63" s="3"/>
     </row>
     <row r="64" spans="1:45" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="197"/>
-      <c r="B64" s="322"/>
-      <c r="C64" s="324"/>
-      <c r="D64" s="242"/>
+      <c r="A64" s="323"/>
+      <c r="B64" s="209"/>
+      <c r="C64" s="211"/>
+      <c r="D64" s="241"/>
       <c r="E64" s="116">
         <v>2</v>
       </c>
       <c r="F64" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="245"/>
+      <c r="G64" s="282"/>
       <c r="H64" s="35"/>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
@@ -7060,7 +7060,7 @@
       <c r="L64" s="35"/>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
-      <c r="O64" s="361"/>
+      <c r="O64" s="203"/>
       <c r="P64" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7098,17 +7098,17 @@
       <c r="AS64" s="3"/>
     </row>
     <row r="65" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="197"/>
-      <c r="B65" s="322"/>
-      <c r="C65" s="324"/>
-      <c r="D65" s="242"/>
+      <c r="A65" s="323"/>
+      <c r="B65" s="209"/>
+      <c r="C65" s="211"/>
+      <c r="D65" s="241"/>
       <c r="E65" s="116">
         <v>3</v>
       </c>
       <c r="F65" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G65" s="245"/>
+      <c r="G65" s="282"/>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
       <c r="J65" s="35"/>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="M65" s="35"/>
       <c r="N65" s="35"/>
-      <c r="O65" s="361"/>
+      <c r="O65" s="203"/>
       <c r="P65" s="9">
         <f t="shared" si="4"/>
         <v>168</v>
@@ -7158,13 +7158,13 @@
       <c r="AS65" s="3"/>
     </row>
     <row r="66" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="197"/>
-      <c r="B66" s="322"/>
-      <c r="C66" s="324"/>
-      <c r="D66" s="259"/>
-      <c r="E66" s="260"/>
-      <c r="F66" s="260"/>
-      <c r="G66" s="260"/>
+      <c r="A66" s="323"/>
+      <c r="B66" s="209"/>
+      <c r="C66" s="211"/>
+      <c r="D66" s="300"/>
+      <c r="E66" s="301"/>
+      <c r="F66" s="301"/>
+      <c r="G66" s="301"/>
       <c r="H66" s="152">
         <f>SUM(H62:H65)</f>
         <v>0</v>
@@ -7226,17 +7226,17 @@
       <c r="AS66" s="2"/>
     </row>
     <row r="67" spans="1:45" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="197"/>
-      <c r="B67" s="322"/>
-      <c r="C67" s="324"/>
-      <c r="D67" s="350" t="s">
+      <c r="A67" s="323"/>
+      <c r="B67" s="209"/>
+      <c r="C67" s="211"/>
+      <c r="D67" s="238" t="s">
         <v>49</v>
       </c>
       <c r="E67" s="134"/>
       <c r="F67" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="G67" s="319">
+      <c r="G67" s="206">
         <v>384</v>
       </c>
       <c r="H67" s="128">
@@ -7248,7 +7248,7 @@
       <c r="L67" s="128"/>
       <c r="M67" s="128"/>
       <c r="N67" s="128"/>
-      <c r="O67" s="362">
+      <c r="O67" s="204">
         <f>SUM(P67:P72)</f>
         <v>384</v>
       </c>
@@ -7301,15 +7301,15 @@
       <c r="AS67" s="3"/>
     </row>
     <row r="68" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="197"/>
-      <c r="B68" s="322"/>
-      <c r="C68" s="324"/>
-      <c r="D68" s="351"/>
+      <c r="A68" s="323"/>
+      <c r="B68" s="209"/>
+      <c r="C68" s="211"/>
+      <c r="D68" s="239"/>
       <c r="E68" s="133"/>
       <c r="F68" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="G68" s="320"/>
+      <c r="G68" s="207"/>
       <c r="H68" s="130"/>
       <c r="I68" s="130">
         <v>72</v>
@@ -7319,7 +7319,7 @@
       <c r="L68" s="130"/>
       <c r="M68" s="130"/>
       <c r="N68" s="130"/>
-      <c r="O68" s="363"/>
+      <c r="O68" s="205"/>
       <c r="P68" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7357,15 +7357,15 @@
       <c r="AS68" s="3"/>
     </row>
     <row r="69" spans="1:45" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="197"/>
-      <c r="B69" s="322"/>
-      <c r="C69" s="324"/>
-      <c r="D69" s="351"/>
+      <c r="A69" s="323"/>
+      <c r="B69" s="209"/>
+      <c r="C69" s="211"/>
+      <c r="D69" s="239"/>
       <c r="E69" s="133"/>
       <c r="F69" s="129" t="s">
         <v>86</v>
       </c>
-      <c r="G69" s="320"/>
+      <c r="G69" s="207"/>
       <c r="H69" s="130"/>
       <c r="I69" s="130"/>
       <c r="J69" s="130">
@@ -7375,7 +7375,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="130"/>
       <c r="N69" s="130"/>
-      <c r="O69" s="363"/>
+      <c r="O69" s="205"/>
       <c r="P69" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7413,15 +7413,15 @@
       <c r="AS69" s="3"/>
     </row>
     <row r="70" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="197"/>
-      <c r="B70" s="322"/>
-      <c r="C70" s="324"/>
-      <c r="D70" s="351"/>
+      <c r="A70" s="323"/>
+      <c r="B70" s="209"/>
+      <c r="C70" s="211"/>
+      <c r="D70" s="239"/>
       <c r="E70" s="133"/>
       <c r="F70" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="G70" s="320"/>
+      <c r="G70" s="207"/>
       <c r="H70" s="130"/>
       <c r="I70" s="130"/>
       <c r="J70" s="130"/>
@@ -7431,7 +7431,7 @@
       <c r="L70" s="130"/>
       <c r="M70" s="130"/>
       <c r="N70" s="130"/>
-      <c r="O70" s="363"/>
+      <c r="O70" s="205"/>
       <c r="P70" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7469,15 +7469,15 @@
       <c r="AS70" s="3"/>
     </row>
     <row r="71" spans="1:45" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="197"/>
-      <c r="B71" s="322"/>
-      <c r="C71" s="324"/>
-      <c r="D71" s="351"/>
+      <c r="A71" s="323"/>
+      <c r="B71" s="209"/>
+      <c r="C71" s="211"/>
+      <c r="D71" s="239"/>
       <c r="E71" s="133"/>
       <c r="F71" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="G71" s="320"/>
+      <c r="G71" s="207"/>
       <c r="H71" s="130"/>
       <c r="I71" s="130"/>
       <c r="J71" s="130"/>
@@ -7487,7 +7487,7 @@
       </c>
       <c r="M71" s="130"/>
       <c r="N71" s="130"/>
-      <c r="O71" s="363"/>
+      <c r="O71" s="205"/>
       <c r="P71" s="9">
         <f t="shared" si="4"/>
         <v>72</v>
@@ -7525,15 +7525,15 @@
       <c r="AS71" s="3"/>
     </row>
     <row r="72" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="197"/>
-      <c r="B72" s="322"/>
-      <c r="C72" s="324"/>
-      <c r="D72" s="351"/>
+      <c r="A72" s="323"/>
+      <c r="B72" s="209"/>
+      <c r="C72" s="211"/>
+      <c r="D72" s="239"/>
       <c r="E72" s="133"/>
       <c r="F72" s="129" t="s">
         <v>89</v>
       </c>
-      <c r="G72" s="320"/>
+      <c r="G72" s="207"/>
       <c r="H72" s="130"/>
       <c r="I72" s="130"/>
       <c r="J72" s="130"/>
@@ -7543,7 +7543,7 @@
         <v>24</v>
       </c>
       <c r="N72" s="130"/>
-      <c r="O72" s="363"/>
+      <c r="O72" s="205"/>
       <c r="P72" s="9">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -7581,13 +7581,13 @@
       <c r="AS72" s="3"/>
     </row>
     <row r="73" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="197"/>
-      <c r="B73" s="322"/>
-      <c r="C73" s="324"/>
-      <c r="D73" s="298"/>
-      <c r="E73" s="299"/>
-      <c r="F73" s="299"/>
-      <c r="G73" s="299"/>
+      <c r="A73" s="323"/>
+      <c r="B73" s="209"/>
+      <c r="C73" s="211"/>
+      <c r="D73" s="244"/>
+      <c r="E73" s="245"/>
+      <c r="F73" s="245"/>
+      <c r="G73" s="245"/>
       <c r="H73" s="135">
         <f>SUM(H67:H72)</f>
         <v>72</v>
@@ -7649,17 +7649,17 @@
       <c r="AS73" s="2"/>
     </row>
     <row r="74" spans="1:45" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="197"/>
-      <c r="B74" s="322"/>
-      <c r="C74" s="324"/>
-      <c r="D74" s="318" t="s">
+      <c r="A74" s="323"/>
+      <c r="B74" s="209"/>
+      <c r="C74" s="211"/>
+      <c r="D74" s="264" t="s">
         <v>16</v>
       </c>
       <c r="E74" s="146"/>
       <c r="F74" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="308">
+      <c r="G74" s="254">
         <v>48</v>
       </c>
       <c r="H74" s="148"/>
@@ -7671,7 +7671,7 @@
       <c r="N74" s="148">
         <v>12</v>
       </c>
-      <c r="O74" s="354">
+      <c r="O74" s="196">
         <f>SUM(P74:P77)</f>
         <v>48</v>
       </c>
@@ -7724,15 +7724,15 @@
       <c r="AS74" s="3"/>
     </row>
     <row r="75" spans="1:45" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="197"/>
-      <c r="B75" s="322"/>
-      <c r="C75" s="324"/>
-      <c r="D75" s="254"/>
+      <c r="A75" s="323"/>
+      <c r="B75" s="209"/>
+      <c r="C75" s="211"/>
+      <c r="D75" s="265"/>
       <c r="E75" s="145"/>
       <c r="F75" s="143" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="308"/>
+      <c r="G75" s="254"/>
       <c r="H75" s="117"/>
       <c r="I75" s="117"/>
       <c r="J75" s="117"/>
@@ -7742,7 +7742,7 @@
       <c r="N75" s="117">
         <v>12</v>
       </c>
-      <c r="O75" s="354"/>
+      <c r="O75" s="196"/>
       <c r="P75" s="9">
         <f t="shared" ref="P75:P77" si="81">SUM(H75:N75)</f>
         <v>12</v>
@@ -7780,15 +7780,15 @@
       <c r="AS75" s="3"/>
     </row>
     <row r="76" spans="1:45" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="197"/>
-      <c r="B76" s="322"/>
-      <c r="C76" s="324"/>
-      <c r="D76" s="254"/>
+      <c r="A76" s="323"/>
+      <c r="B76" s="209"/>
+      <c r="C76" s="211"/>
+      <c r="D76" s="265"/>
       <c r="E76" s="145"/>
       <c r="F76" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="308"/>
+      <c r="G76" s="254"/>
       <c r="H76" s="117"/>
       <c r="I76" s="117"/>
       <c r="J76" s="117"/>
@@ -7798,7 +7798,7 @@
       <c r="N76" s="117">
         <v>12</v>
       </c>
-      <c r="O76" s="354"/>
+      <c r="O76" s="196"/>
       <c r="P76" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7836,15 +7836,15 @@
       <c r="AS76" s="3"/>
     </row>
     <row r="77" spans="1:45" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="197"/>
-      <c r="B77" s="322"/>
-      <c r="C77" s="324"/>
-      <c r="D77" s="257"/>
+      <c r="A77" s="323"/>
+      <c r="B77" s="209"/>
+      <c r="C77" s="211"/>
+      <c r="D77" s="266"/>
       <c r="E77" s="145"/>
       <c r="F77" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="G77" s="309"/>
+      <c r="G77" s="255"/>
       <c r="H77" s="118"/>
       <c r="I77" s="118"/>
       <c r="J77" s="118"/>
@@ -7854,7 +7854,7 @@
       <c r="N77" s="118">
         <v>12</v>
       </c>
-      <c r="O77" s="355"/>
+      <c r="O77" s="197"/>
       <c r="P77" s="9">
         <f t="shared" si="81"/>
         <v>12</v>
@@ -7892,13 +7892,13 @@
       <c r="AS77" s="3"/>
     </row>
     <row r="78" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="197"/>
-      <c r="B78" s="322"/>
-      <c r="C78" s="324"/>
-      <c r="D78" s="300"/>
-      <c r="E78" s="301"/>
-      <c r="F78" s="302"/>
-      <c r="G78" s="303"/>
+      <c r="A78" s="323"/>
+      <c r="B78" s="209"/>
+      <c r="C78" s="211"/>
+      <c r="D78" s="246"/>
+      <c r="E78" s="247"/>
+      <c r="F78" s="248"/>
+      <c r="G78" s="249"/>
       <c r="H78" s="112">
         <f>SUM(H74:H77)</f>
         <v>0</v>
@@ -7960,17 +7960,17 @@
       <c r="AS78" s="2"/>
     </row>
     <row r="79" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="197"/>
-      <c r="B79" s="322"/>
-      <c r="C79" s="324"/>
-      <c r="D79" s="316" t="s">
+      <c r="A79" s="323"/>
+      <c r="B79" s="209"/>
+      <c r="C79" s="211"/>
+      <c r="D79" s="262" t="s">
         <v>50</v>
       </c>
       <c r="E79" s="157"/>
       <c r="F79" s="158" t="s">
         <v>94</v>
       </c>
-      <c r="G79" s="310">
+      <c r="G79" s="256">
         <v>48</v>
       </c>
       <c r="H79" s="159">
@@ -7982,7 +7982,7 @@
       <c r="L79" s="159"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
-      <c r="O79" s="358">
+      <c r="O79" s="200">
         <f>SUM(P79:P82)</f>
         <v>48</v>
       </c>
@@ -8029,15 +8029,15 @@
       <c r="AS79" s="3"/>
     </row>
     <row r="80" spans="1:45" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="197"/>
-      <c r="B80" s="322"/>
-      <c r="C80" s="324"/>
-      <c r="D80" s="317"/>
+      <c r="A80" s="323"/>
+      <c r="B80" s="209"/>
+      <c r="C80" s="211"/>
+      <c r="D80" s="263"/>
       <c r="E80" s="154"/>
       <c r="F80" s="155" t="s">
         <v>95</v>
       </c>
-      <c r="G80" s="311"/>
+      <c r="G80" s="257"/>
       <c r="H80" s="156">
         <v>12</v>
       </c>
@@ -8047,7 +8047,7 @@
       <c r="L80" s="156"/>
       <c r="M80" s="156"/>
       <c r="N80" s="156"/>
-      <c r="O80" s="359"/>
+      <c r="O80" s="201"/>
       <c r="P80" s="9">
         <f t="shared" ref="P80:P82" si="83">SUM(H80:N80)</f>
         <v>12</v>
@@ -8085,15 +8085,15 @@
       <c r="AS80" s="3"/>
     </row>
     <row r="81" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="197"/>
-      <c r="B81" s="322"/>
-      <c r="C81" s="324"/>
-      <c r="D81" s="317"/>
+      <c r="A81" s="323"/>
+      <c r="B81" s="209"/>
+      <c r="C81" s="211"/>
+      <c r="D81" s="263"/>
       <c r="E81" s="154"/>
       <c r="F81" s="155" t="s">
         <v>96</v>
       </c>
-      <c r="G81" s="311"/>
+      <c r="G81" s="257"/>
       <c r="H81" s="156">
         <v>12</v>
       </c>
@@ -8103,7 +8103,7 @@
       <c r="L81" s="156"/>
       <c r="M81" s="156"/>
       <c r="N81" s="156"/>
-      <c r="O81" s="359"/>
+      <c r="O81" s="201"/>
       <c r="P81" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -8141,15 +8141,15 @@
       <c r="AS81" s="3"/>
     </row>
     <row r="82" spans="1:45" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="197"/>
-      <c r="B82" s="322"/>
-      <c r="C82" s="324"/>
-      <c r="D82" s="317"/>
+      <c r="A82" s="323"/>
+      <c r="B82" s="209"/>
+      <c r="C82" s="211"/>
+      <c r="D82" s="263"/>
       <c r="E82" s="154"/>
       <c r="F82" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="G82" s="311"/>
+      <c r="G82" s="257"/>
       <c r="H82" s="156">
         <v>12</v>
       </c>
@@ -8159,7 +8159,7 @@
       <c r="L82" s="156"/>
       <c r="M82" s="156"/>
       <c r="N82" s="156"/>
-      <c r="O82" s="359"/>
+      <c r="O82" s="201"/>
       <c r="P82" s="9">
         <f t="shared" si="83"/>
         <v>12</v>
@@ -8197,13 +8197,13 @@
       <c r="AS82" s="3"/>
     </row>
     <row r="83" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="197"/>
-      <c r="B83" s="322"/>
-      <c r="C83" s="324"/>
-      <c r="D83" s="304"/>
-      <c r="E83" s="305"/>
-      <c r="F83" s="305"/>
-      <c r="G83" s="305"/>
+      <c r="A83" s="323"/>
+      <c r="B83" s="209"/>
+      <c r="C83" s="211"/>
+      <c r="D83" s="250"/>
+      <c r="E83" s="251"/>
+      <c r="F83" s="251"/>
+      <c r="G83" s="251"/>
       <c r="H83" s="160">
         <f>SUM(H79:H82)</f>
         <v>48</v>
@@ -8265,17 +8265,17 @@
       <c r="AS83" s="2"/>
     </row>
     <row r="84" spans="1:45" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="197"/>
-      <c r="B84" s="322"/>
-      <c r="C84" s="325"/>
-      <c r="D84" s="314" t="s">
+      <c r="A84" s="323"/>
+      <c r="B84" s="209"/>
+      <c r="C84" s="212"/>
+      <c r="D84" s="260" t="s">
         <v>51</v>
       </c>
       <c r="E84" s="125"/>
       <c r="F84" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G84" s="312">
+      <c r="G84" s="258">
         <v>48</v>
       </c>
       <c r="H84" s="126"/>
@@ -8287,7 +8287,7 @@
       <c r="L84" s="126"/>
       <c r="M84" s="126"/>
       <c r="N84" s="126"/>
-      <c r="O84" s="356">
+      <c r="O84" s="198">
         <f>SUM(P84:P87)</f>
         <v>48</v>
       </c>
@@ -8334,15 +8334,15 @@
       <c r="AS84" s="3"/>
     </row>
     <row r="85" spans="1:45" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="197"/>
-      <c r="B85" s="322"/>
-      <c r="C85" s="325"/>
-      <c r="D85" s="315"/>
+      <c r="A85" s="323"/>
+      <c r="B85" s="209"/>
+      <c r="C85" s="212"/>
+      <c r="D85" s="261"/>
       <c r="E85" s="123"/>
       <c r="F85" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="G85" s="313"/>
+      <c r="G85" s="259"/>
       <c r="H85" s="124"/>
       <c r="I85" s="124">
         <v>12</v>
@@ -8352,7 +8352,7 @@
       <c r="L85" s="124"/>
       <c r="M85" s="124"/>
       <c r="N85" s="124"/>
-      <c r="O85" s="357"/>
+      <c r="O85" s="199"/>
       <c r="P85" s="9">
         <f t="shared" ref="P85:P87" si="90">SUM(H85:N85)</f>
         <v>12</v>
@@ -8390,15 +8390,15 @@
       <c r="AS85" s="3"/>
     </row>
     <row r="86" spans="1:45" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="197"/>
-      <c r="B86" s="322"/>
-      <c r="C86" s="325"/>
-      <c r="D86" s="315"/>
+      <c r="A86" s="323"/>
+      <c r="B86" s="209"/>
+      <c r="C86" s="212"/>
+      <c r="D86" s="261"/>
       <c r="E86" s="123"/>
       <c r="F86" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="313"/>
+      <c r="G86" s="259"/>
       <c r="H86" s="124"/>
       <c r="I86" s="124">
         <v>12</v>
@@ -8408,7 +8408,7 @@
       <c r="L86" s="124"/>
       <c r="M86" s="124"/>
       <c r="N86" s="124"/>
-      <c r="O86" s="357"/>
+      <c r="O86" s="199"/>
       <c r="P86" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8446,15 +8446,15 @@
       <c r="AS86" s="3"/>
     </row>
     <row r="87" spans="1:45" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="198"/>
-      <c r="B87" s="322"/>
-      <c r="C87" s="325"/>
-      <c r="D87" s="315"/>
+      <c r="A87" s="324"/>
+      <c r="B87" s="209"/>
+      <c r="C87" s="212"/>
+      <c r="D87" s="261"/>
       <c r="E87" s="123"/>
       <c r="F87" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="G87" s="313"/>
+      <c r="G87" s="259"/>
       <c r="H87" s="124"/>
       <c r="I87" s="124">
         <v>12</v>
@@ -8464,7 +8464,7 @@
       <c r="L87" s="124"/>
       <c r="M87" s="124"/>
       <c r="N87" s="124"/>
-      <c r="O87" s="357"/>
+      <c r="O87" s="199"/>
       <c r="P87" s="9">
         <f t="shared" si="90"/>
         <v>12</v>
@@ -8503,12 +8503,12 @@
     </row>
     <row r="88" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
-      <c r="B88" s="322"/>
-      <c r="C88" s="325"/>
-      <c r="D88" s="306"/>
-      <c r="E88" s="307"/>
-      <c r="F88" s="307"/>
-      <c r="G88" s="307"/>
+      <c r="B88" s="209"/>
+      <c r="C88" s="212"/>
+      <c r="D88" s="252"/>
+      <c r="E88" s="253"/>
+      <c r="F88" s="253"/>
+      <c r="G88" s="253"/>
       <c r="H88" s="162">
         <f>SUM(H84:H87)</f>
         <v>0</v>
@@ -8571,8 +8571,8 @@
     </row>
     <row r="89" spans="1:45" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
-      <c r="B89" s="322"/>
-      <c r="C89" s="325"/>
+      <c r="B89" s="209"/>
+      <c r="C89" s="212"/>
       <c r="D89" s="122" t="s">
         <v>17</v>
       </c>
@@ -8640,12 +8640,12 @@
     </row>
     <row r="90" spans="1:45" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
-      <c r="B90" s="322"/>
-      <c r="C90" s="325"/>
-      <c r="D90" s="249"/>
-      <c r="E90" s="297"/>
-      <c r="F90" s="297"/>
-      <c r="G90" s="297"/>
+      <c r="B90" s="209"/>
+      <c r="C90" s="212"/>
+      <c r="D90" s="242"/>
+      <c r="E90" s="243"/>
+      <c r="F90" s="243"/>
+      <c r="G90" s="243"/>
       <c r="H90" s="140">
         <f t="shared" ref="H90:N90" si="97">SUM(H89:H89)</f>
         <v>48</v>
@@ -8772,36 +8772,85 @@
       </c>
     </row>
     <row r="97" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="H97" s="296" t="s">
+      <c r="H97" s="213" t="s">
         <v>104</v>
       </c>
-      <c r="I97" s="296"/>
-      <c r="J97" s="296"/>
+      <c r="I97" s="213"/>
+      <c r="J97" s="213"/>
     </row>
     <row r="99" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="I99" s="296" t="s">
+      <c r="I99" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="J99" s="296"/>
-      <c r="K99" s="296"/>
-      <c r="L99" s="296"/>
+      <c r="J99" s="213"/>
+      <c r="K99" s="213"/>
+      <c r="L99" s="213"/>
     </row>
     <row r="101" spans="8:14" x14ac:dyDescent="0.3">
-      <c r="K101" s="296" t="s">
+      <c r="K101" s="213" t="s">
         <v>106</v>
       </c>
-      <c r="L101" s="296"/>
-      <c r="M101" s="296"/>
-      <c r="N101" s="296"/>
+      <c r="L101" s="213"/>
+      <c r="M101" s="213"/>
+      <c r="N101" s="213"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS91" xr:uid="{44B9DB88-0080-4900-9B58-5C638DC6AAB3}"/>
   <mergeCells count="75">
-    <mergeCell ref="O74:O77"/>
-    <mergeCell ref="O84:O87"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O62:O65"/>
-    <mergeCell ref="O67:O72"/>
+    <mergeCell ref="A2:A87"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O52:O55"/>
+    <mergeCell ref="O57:O60"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="O7:O10"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="O22:O25"/>
+    <mergeCell ref="O27:O30"/>
+    <mergeCell ref="O32:O35"/>
+    <mergeCell ref="O37:O40"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="K101:N101"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="D74:D77"/>
     <mergeCell ref="G67:G72"/>
     <mergeCell ref="B2:B90"/>
     <mergeCell ref="C2:C90"/>
@@ -8818,60 +8867,11 @@
     <mergeCell ref="D56:G56"/>
     <mergeCell ref="D67:D72"/>
     <mergeCell ref="D62:D65"/>
-    <mergeCell ref="K101:N101"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="D79:D82"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="O32:O35"/>
-    <mergeCell ref="O37:O40"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="G42:G45"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="O7:O10"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="O22:O25"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O52:O55"/>
-    <mergeCell ref="O57:O60"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="A2:A87"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="O74:O77"/>
+    <mergeCell ref="O84:O87"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O62:O65"/>
+    <mergeCell ref="O67:O72"/>
   </mergeCells>
   <conditionalFormatting sqref="H93:N93">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>